<commit_message>
feat: add new nodes to report
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fm2871\Documents\DocumentFilter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB142DAA-9EDF-4684-9D41-ACD769BD0758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7182C0B9-A718-4346-8A72-FC3902B91012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$V$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$V$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="205">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -667,6 +667,21 @@
   </si>
   <si>
     <t>1362/delay.log</t>
+  </si>
+  <si>
+    <t>1372/delay.log</t>
+  </si>
+  <si>
+    <t>1373/delay.log</t>
+  </si>
+  <si>
+    <t>EOMM MD BYTPASBUE1362 - .135</t>
+  </si>
+  <si>
+    <t>EOMM MD BYTPASBUE1372 - .122</t>
+  </si>
+  <si>
+    <t>EOMM MD BYTPASBUE1373 - .136</t>
   </si>
 </sst>
 </file>
@@ -674,9 +689,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -808,7 +823,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -818,7 +833,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -842,25 +857,25 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -933,7 +948,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1249,13 +1264,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-  <dimension ref="B2:W40"/>
+  <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="3.44140625" customWidth="1"/>
@@ -1594,14 +1609,14 @@
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="C11" s="24">
-        <v>1147</v>
+        <v>1372</v>
       </c>
       <c r="D11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>JAVA 21</v>
       </c>
       <c r="E11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1613,7 +1628,7 @@
       </c>
       <c r="G11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP+MBO</v>
+        <v>MBP</v>
       </c>
       <c r="H11" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1678,14 +1693,14 @@
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>11</v>
+        <v>201</v>
       </c>
       <c r="C12" s="24">
-        <v>541</v>
+        <v>1373</v>
       </c>
       <c r="D12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>JAVA 21</v>
       </c>
       <c r="E12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1697,7 +1712,7 @@
       </c>
       <c r="G12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP+MBO</v>
+        <v>MBP</v>
       </c>
       <c r="H12" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1762,10 +1777,10 @@
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C13" s="24">
-        <v>544</v>
+        <v>1147</v>
       </c>
       <c r="D13" s="19" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -1846,10 +1861,10 @@
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C14" s="24">
-        <v>981</v>
+        <v>541</v>
       </c>
       <c r="D14" s="19" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -1927,14 +1942,13 @@
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="W14" s="18"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C15" s="24">
-        <v>982</v>
+        <v>544</v>
       </c>
       <c r="D15" s="19" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2015,10 +2029,10 @@
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C16" s="24">
-        <v>1146</v>
+        <v>981</v>
       </c>
       <c r="D16" s="19" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2096,13 +2110,14 @@
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W16" s="18"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C17" s="24">
-        <v>1148</v>
+        <v>982</v>
       </c>
       <c r="D17" s="19" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2183,10 +2198,10 @@
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C18" s="24">
-        <v>543</v>
+        <v>1146</v>
       </c>
       <c r="D18" s="19" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2267,10 +2282,10 @@
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C19" s="24">
-        <v>542</v>
+        <v>1148</v>
       </c>
       <c r="D19" s="19" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2351,14 +2366,14 @@
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C20" s="24">
-        <v>819</v>
+        <v>543</v>
       </c>
       <c r="D20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>DMA</v>
+        <v>EOMM</v>
       </c>
       <c r="E20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2370,7 +2385,7 @@
       </c>
       <c r="G20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>DEDICADO</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H20" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B20,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2435,14 +2450,14 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="16" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C21" s="24">
-        <v>1115</v>
+        <v>542</v>
       </c>
       <c r="D21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>DMA</v>
+        <v>EOMM</v>
       </c>
       <c r="E21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2454,7 +2469,7 @@
       </c>
       <c r="G21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>DEDICADO</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H21" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2519,10 +2534,10 @@
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="16" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C22" s="24">
-        <v>1116</v>
+        <v>819</v>
       </c>
       <c r="D22" s="19" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2603,10 +2618,10 @@
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C23" s="24">
-        <v>560</v>
+        <v>1115</v>
       </c>
       <c r="D23" s="19" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2622,7 +2637,7 @@
       </c>
       <c r="G23" s="19" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBO</v>
+        <v>DEDICADO</v>
       </c>
       <c r="H23" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B23,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2687,10 +2702,10 @@
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C24" s="24">
-        <v>559</v>
+        <v>1116</v>
       </c>
       <c r="D24" s="19" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2706,7 +2721,7 @@
       </c>
       <c r="G24" s="19" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBO</v>
+        <v>DEDICADO</v>
       </c>
       <c r="H24" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B24,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2771,10 +2786,10 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="24">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D25" s="19" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2855,10 +2870,10 @@
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26" s="24">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D26" s="19" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2874,7 +2889,7 @@
       </c>
       <c r="G26" s="19" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBO</v>
       </c>
       <c r="H26" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B26,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2939,10 +2954,10 @@
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="24">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D27" s="19" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2958,7 +2973,7 @@
       </c>
       <c r="G27" s="19" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBO</v>
       </c>
       <c r="H27" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B27,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3023,10 +3038,10 @@
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C28" s="24">
-        <v>1114</v>
+        <v>562</v>
       </c>
       <c r="D28" s="19" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3107,10 +3122,10 @@
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C29" s="24">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D29" s="19" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3191,10 +3206,10 @@
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C30" s="24">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="D30" s="19" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3275,10 +3290,10 @@
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" s="24">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D31" s="19" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3359,10 +3374,10 @@
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C32" s="24">
-        <v>1003</v>
+        <v>1118</v>
       </c>
       <c r="D32" s="19" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3378,7 +3393,7 @@
       </c>
       <c r="G32" s="19" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>THROTTLE</v>
+        <v>MBP</v>
       </c>
       <c r="H32" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B32,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3443,14 +3458,14 @@
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C33" s="24">
-        <v>580</v>
+        <v>564</v>
       </c>
       <c r="D33" s="19" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>DMA</v>
       </c>
       <c r="E33" s="19" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -3462,7 +3477,7 @@
       </c>
       <c r="G33" s="19" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBO</v>
+        <v>MBP</v>
       </c>
       <c r="H33" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B33,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3527,14 +3542,14 @@
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C34" s="24">
-        <v>578</v>
+        <v>1003</v>
       </c>
       <c r="D34" s="19" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>DMA</v>
       </c>
       <c r="E34" s="19" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -3546,7 +3561,7 @@
       </c>
       <c r="G34" s="19" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBO</v>
+        <v>THROTTLE</v>
       </c>
       <c r="H34" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3611,10 +3626,10 @@
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35" s="24">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D35" s="19" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3695,10 +3710,10 @@
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C36" s="24">
-        <v>354</v>
+        <v>578</v>
       </c>
       <c r="D36" s="19" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3714,7 +3729,7 @@
       </c>
       <c r="G36" s="19" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBO</v>
       </c>
       <c r="H36" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B36,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3779,10 +3794,10 @@
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C37" s="24">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D37" s="19" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3798,7 +3813,7 @@
       </c>
       <c r="G37" s="19" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBO</v>
       </c>
       <c r="H37" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B37,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3863,10 +3878,10 @@
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C38" s="24">
-        <v>583</v>
+        <v>354</v>
       </c>
       <c r="D38" s="19" t="str">
         <f>+VLOOKUP($B38,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3947,24 +3962,24 @@
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="25">
-        <v>581</v>
-      </c>
-      <c r="D39" s="20" t="str">
+        <v>26</v>
+      </c>
+      <c r="C39" s="24">
+        <v>582</v>
+      </c>
+      <c r="D39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO</v>
       </c>
-      <c r="E39" s="20" t="str">
+      <c r="E39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F39" s="20" t="str">
+      <c r="F39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G39" s="20" t="str">
+      <c r="G39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
@@ -3972,55 +3987,55 @@
         <f>IF(IFERROR(VLOOKUP($B39,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B39,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I39" s="22" t="str">
+      <c r="I39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J39" s="22" t="str">
+      <c r="J39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K39" s="22" t="str">
+      <c r="K39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L39" s="22" t="str">
+      <c r="L39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M39" s="22" t="str">
+      <c r="M39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N39" s="22" t="str">
+      <c r="N39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O39" s="22" t="str">
+      <c r="O39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P39" s="22" t="str">
+      <c r="P39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q39" s="22" t="str">
+      <c r="Q39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R39" s="22" t="str">
+      <c r="R39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S39" s="22" t="str">
+      <c r="S39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T39" s="22" t="str">
+      <c r="T39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U39" s="22" t="str">
+      <c r="U39" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
@@ -4030,39 +4045,207 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="13"/>
+      <c r="B40" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="24">
+        <v>583</v>
+      </c>
+      <c r="D40" s="19" t="str">
+        <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E40" s="19" t="str">
+        <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,E$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="F40" s="19" t="str">
+        <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,F$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="G40" s="19" t="str">
+        <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,G$7,0)</f>
+        <v>MBP</v>
+      </c>
+      <c r="H40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B40,'Users+Static Data'!$F:$H,H$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="I40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V40" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="25">
+        <v>581</v>
+      </c>
+      <c r="D41" s="20" t="str">
+        <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E41" s="20" t="str">
+        <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,E$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="F41" s="20" t="str">
+        <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,F$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="G41" s="20" t="str">
+        <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,G$7,0)</f>
+        <v>MBP</v>
+      </c>
+      <c r="H41" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B41,'Users+Static Data'!$F:$H,H$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="I41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U41" s="22" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V41" s="21" t="str">
+        <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:V39" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:V39">
-      <sortCondition ref="J8:J39"/>
+  <autoFilter ref="B8:V41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:V41">
+      <sortCondition ref="J8:J41"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C8:V39">
+  <conditionalFormatting sqref="C8:V41">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>$D8="JAVA 21"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:G39">
+  <conditionalFormatting sqref="D8:G41">
     <cfRule type="expression" dxfId="6" priority="4">
       <formula>$D8="JAVA 21"</formula>
     </cfRule>
@@ -4076,14 +4259,14 @@
       <formula>$D8="DMA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I39 K9:L39 N9:Q39">
+  <conditionalFormatting sqref="I9:I41 K9:L41 N9:Q41">
     <cfRule type="expression" dxfId="2" priority="8">
-      <formula>I9=MIN(I$9:I$39)</formula>
+      <formula>I9=MIN(I$9:I$41)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J39">
+  <conditionalFormatting sqref="J9:J41">
     <cfRule type="expression" dxfId="1" priority="9">
-      <formula>J9=MIN($J$9:J$39)</formula>
+      <formula>J9=MIN($J$9:J$41)</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -4094,7 +4277,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K39">
+  <conditionalFormatting sqref="K9:K41">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4104,7 +4287,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O9:O39">
+  <conditionalFormatting sqref="O9:O41">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -4114,7 +4297,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P9:P39">
+  <conditionalFormatting sqref="P9:P41">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4124,7 +4307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q9:Q39">
+  <conditionalFormatting sqref="Q9:Q41">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4134,7 +4317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9:T39">
+  <conditionalFormatting sqref="T9:T41">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -4144,12 +4327,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9:U39">
+  <conditionalFormatting sqref="T9:U41">
     <cfRule type="expression" dxfId="0" priority="15">
-      <formula>T9=MIN(T$9:T$39)</formula>
+      <formula>T9=MIN(T$9:T$41)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:U39">
+  <conditionalFormatting sqref="U9:U41">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -4169,7 +4352,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
@@ -4195,13 +4378,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
-  <dimension ref="B1:O86"/>
+  <dimension ref="B1:O89"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L37" sqref="K37:O37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E87" sqref="E87:H89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.109375" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -5306,6 +5489,21 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K38" t="s">
+        <v>200</v>
+      </c>
+      <c r="L38" t="s">
+        <v>181</v>
+      </c>
+      <c r="M38" t="s">
+        <v>183</v>
+      </c>
+      <c r="N38" t="s">
+        <v>116</v>
+      </c>
+      <c r="O38" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
@@ -5324,6 +5522,21 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K39" t="s">
+        <v>201</v>
+      </c>
+      <c r="L39" t="s">
+        <v>181</v>
+      </c>
+      <c r="M39" t="s">
+        <v>183</v>
+      </c>
+      <c r="N39" t="s">
+        <v>116</v>
+      </c>
+      <c r="O39" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
@@ -5933,7 +6146,7 @@
         <v>1147</v>
       </c>
       <c r="H73" t="e">
-        <f t="shared" ref="H73:H86" si="1">+VLOOKUP(E73,B:C,2,0)</f>
+        <f t="shared" ref="H73:H89" si="1">+VLOOKUP(E73,B:C,2,0)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -6171,6 +6384,54 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>202</v>
+      </c>
+      <c r="F87" t="s">
+        <v>199</v>
+      </c>
+      <c r="G87" cm="1">
+        <f t="array" aca="1" ref="G87" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1)*1),MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1),"")))</f>
+        <v>1362</v>
+      </c>
+      <c r="H87" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E88" t="s">
+        <v>203</v>
+      </c>
+      <c r="F88" t="s">
+        <v>200</v>
+      </c>
+      <c r="G88" cm="1">
+        <f t="array" aca="1" ref="G88" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1)*1),MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1),"")))</f>
+        <v>1372</v>
+      </c>
+      <c r="H88" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E89" t="s">
+        <v>204</v>
+      </c>
+      <c r="F89" t="s">
+        <v>201</v>
+      </c>
+      <c r="G89" cm="1">
+        <f t="array" aca="1" ref="G89" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1)*1),MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1),"")))</f>
+        <v>1373</v>
+      </c>
+      <c r="H89" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: adjust template to match VMs state as of jun 6
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7182C0B9-A718-4346-8A72-FC3902B91012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798E90E4-DE27-4EE1-B80B-9BAFCC9C5086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$V$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$W$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$O$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="206">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -575,9 +576,6 @@
     <t>MAX Delay (ms)</t>
   </si>
   <si>
-    <t>MIN Delay (ms)</t>
-  </si>
-  <si>
     <t>Delay P95 (ms)</t>
   </si>
   <si>
@@ -603,9 +601,6 @@
   </si>
   <si>
     <t>THROTTLE</t>
-  </si>
-  <si>
-    <t>JAVA 21</t>
   </si>
   <si>
     <t>MBP+MBO</t>
@@ -631,14 +626,6 @@
 (cant)</t>
   </si>
   <si>
-    <t>Desvío Est. 
-Delay (ms)</t>
-  </si>
-  <si>
-    <t>Prom. Pond. 
-Delay (ms)</t>
-  </si>
-  <si>
     <t>Prom. 
 Delay (ms)</t>
   </si>
@@ -650,9 +637,6 @@
     <t>Prom. &lt; 95 (ms)</t>
   </si>
   <si>
-    <t>Mediana Delay (ms)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID
 </t>
   </si>
@@ -682,6 +666,31 @@
   </si>
   <si>
     <t>EOMM MD BYTPASBUE1373 - .136</t>
+  </si>
+  <si>
+    <t>EOMM J21</t>
+  </si>
+  <si>
+    <t>Artem J21</t>
+  </si>
+  <si>
+    <t>MIN 
+Delay 
+(ms)</t>
+  </si>
+  <si>
+    <t>Mediana Delay 
+(ms)</t>
+  </si>
+  <si>
+    <t>Prom. Pond. 
+Delay 
+(ms)</t>
+  </si>
+  <si>
+    <t>Desvío Est. 
+Delay 
+(ms)</t>
   </si>
 </sst>
 </file>
@@ -732,7 +741,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +769,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -825,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -873,18 +888,222 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1281,20 +1500,20 @@
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="1" customWidth="1"/>
-    <col min="12" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="11.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="1" customWidth="1"/>
+    <col min="14" max="17" width="8.88671875" style="1" customWidth="1"/>
     <col min="18" max="19" width="9.109375" style="1" customWidth="1"/>
-    <col min="20" max="21" width="7.88671875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.88671875" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
@@ -1309,7 +1528,7 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
@@ -1376,79 +1595,79 @@
     </row>
     <row r="8" spans="2:23" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>168</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>170</v>
       </c>
       <c r="O8" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="P8" s="12" t="s">
-        <v>173</v>
-      </c>
       <c r="Q8" s="12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="24">
-        <v>1256</v>
+        <v>541</v>
       </c>
       <c r="D9" s="19" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>JAVA 21</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E9" s="19" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1460,7 +1679,7 @@
       </c>
       <c r="G9" s="19" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H9" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B9,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1525,14 +1744,14 @@
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
-        <v>199</v>
+        <v>13</v>
       </c>
       <c r="C10" s="24">
-        <v>1362</v>
+        <v>543</v>
       </c>
       <c r="D10" s="19" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>JAVA 21</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E10" s="19" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1544,7 +1763,7 @@
       </c>
       <c r="G10" s="19" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H10" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B10,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1609,14 +1828,14 @@
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="C11" s="24">
-        <v>1372</v>
+        <v>544</v>
       </c>
       <c r="D11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>JAVA 21</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1628,7 +1847,7 @@
       </c>
       <c r="G11" s="19" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H11" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1693,14 +1912,14 @@
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>201</v>
+        <v>29</v>
       </c>
       <c r="C12" s="24">
-        <v>1373</v>
+        <v>981</v>
       </c>
       <c r="D12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>JAVA 21</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1712,7 +1931,7 @@
       </c>
       <c r="G12" s="19" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBP+MBO</v>
       </c>
       <c r="H12" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -1777,14 +1996,14 @@
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>7</v>
+        <v>194</v>
       </c>
       <c r="C13" s="24">
-        <v>1147</v>
+        <v>1362</v>
       </c>
       <c r="D13" s="19" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E13" s="19" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1861,14 +2080,14 @@
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>11</v>
+        <v>195</v>
       </c>
       <c r="C14" s="24">
-        <v>541</v>
+        <v>1372</v>
       </c>
       <c r="D14" s="19" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E14" s="19" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -1945,14 +2164,14 @@
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="C15" s="24">
-        <v>544</v>
+        <v>1373</v>
       </c>
       <c r="D15" s="19" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM J21</v>
       </c>
       <c r="E15" s="19" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2026,13 +2245,14 @@
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W15" s="18"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C16" s="24">
-        <v>981</v>
+        <v>542</v>
       </c>
       <c r="D16" s="19" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2110,7 +2330,6 @@
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="W16" s="18"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
@@ -2282,10 +2501,10 @@
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="24">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="D19" s="19" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2366,10 +2585,10 @@
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C20" s="24">
-        <v>543</v>
+        <v>1148</v>
       </c>
       <c r="D20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2450,14 +2669,14 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21" s="24">
-        <v>542</v>
+        <v>1256</v>
       </c>
       <c r="D21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>Artem J21</v>
       </c>
       <c r="E21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2469,7 +2688,7 @@
       </c>
       <c r="G21" s="19" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP+MBO</v>
+        <v>MBP</v>
       </c>
       <c r="H21" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2786,10 +3005,10 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C25" s="24">
-        <v>560</v>
+        <v>1003</v>
       </c>
       <c r="D25" s="19" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -2805,7 +3024,7 @@
       </c>
       <c r="G25" s="19" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBO</v>
+        <v>THROTTLE</v>
       </c>
       <c r="H25" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B25,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -2954,10 +3173,10 @@
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="24">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D27" s="19" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3038,10 +3257,10 @@
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="24">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D28" s="19" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3057,7 +3276,7 @@
       </c>
       <c r="G28" s="19" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
+        <v>MBO</v>
       </c>
       <c r="H28" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B28,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3122,10 +3341,10 @@
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="24">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D29" s="19" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3206,10 +3425,10 @@
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C30" s="24">
-        <v>1114</v>
+        <v>563</v>
       </c>
       <c r="D30" s="19" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3290,10 +3509,10 @@
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="24">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D31" s="19" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3374,10 +3593,10 @@
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C32" s="24">
-        <v>1118</v>
+        <v>565</v>
       </c>
       <c r="D32" s="19" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3458,10 +3677,10 @@
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C33" s="24">
-        <v>564</v>
+        <v>1114</v>
       </c>
       <c r="D33" s="19" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3542,10 +3761,10 @@
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C34" s="24">
-        <v>1003</v>
+        <v>1118</v>
       </c>
       <c r="D34" s="19" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3561,7 +3780,7 @@
       </c>
       <c r="G34" s="19" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>THROTTLE</v>
+        <v>MBP</v>
       </c>
       <c r="H34" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0))</f>
@@ -3626,10 +3845,10 @@
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C35" s="24">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D35" s="19" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3710,10 +3929,10 @@
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36" s="24">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D36" s="19" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3794,10 +4013,10 @@
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="24">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D37" s="19" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -3962,10 +4181,10 @@
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="24">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -4046,10 +4265,10 @@
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40" s="24">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D40" s="19" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -4130,10 +4349,10 @@
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C41" s="25">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D41" s="20" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,D$7,0)</f>
@@ -4235,50 +4454,14 @@
       <c r="V42" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:V41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:V41">
-      <sortCondition ref="J8:J41"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="C8:V41">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>$D8="JAVA 21"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:G41">
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$D8="JAVA 21"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$D8="ALGO"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$D8="EOMM"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>$D8="DMA"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I41 K9:L41 N9:Q41">
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>I9=MIN(I$9:I$41)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J41">
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>J9=MIN($J$9:J$41)</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <autoFilter ref="B8:W41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}"/>
+  <conditionalFormatting sqref="C9:V41">
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K41">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4288,7 +4471,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:O41">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4298,7 +4481,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:P41">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4308,6 +4491,41 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9:Q41">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9:T41">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U9:U41">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I41 K9:L41 N9:Q41 J9:J41 T9:U41">
+    <cfRule type="expression" dxfId="9" priority="13">
+      <formula>I9=MIN(I$9:I$41)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J41">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4317,29 +4535,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9:T41">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="D9:G41">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T9:U41">
-    <cfRule type="expression" dxfId="0" priority="15">
-      <formula>T9=MIN(T$9:T$41)</formula>
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U9:U41">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4381,7 +4588,7 @@
   <dimension ref="B1:O89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:H89"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4432,19 +4639,19 @@
         <v>167</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>168</v>
@@ -4454,7 +4661,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -4467,19 +4674,19 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="M7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N7" t="s">
         <v>116</v>
       </c>
       <c r="O7" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
@@ -4500,19 +4707,19 @@
         <v>#N/A</v>
       </c>
       <c r="K8" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="M8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N8" t="s">
         <v>116</v>
       </c>
       <c r="O8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
@@ -4533,19 +4740,19 @@
         <v>#N/A</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="M9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N9" t="s">
         <v>116</v>
       </c>
       <c r="O9" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
@@ -4566,19 +4773,19 @@
         <v>#N/A</v>
       </c>
       <c r="K10" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="M10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N10" t="s">
         <v>116</v>
       </c>
       <c r="O10" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
@@ -4599,13 +4806,13 @@
         <v>#N/A</v>
       </c>
       <c r="K11" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="M11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N11" t="s">
         <v>116</v>
@@ -4632,19 +4839,19 @@
         <v>#N/A</v>
       </c>
       <c r="K12" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N12" t="s">
         <v>116</v>
       </c>
       <c r="O12" t="s">
-        <v>182</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -4665,19 +4872,19 @@
         <v>#N/A</v>
       </c>
       <c r="K13" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N13" t="s">
         <v>116</v>
       </c>
       <c r="O13" t="s">
-        <v>182</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -4698,19 +4905,19 @@
         <v>#N/A</v>
       </c>
       <c r="K14" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N14" t="s">
         <v>116</v>
       </c>
       <c r="O14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -4731,13 +4938,13 @@
         <v>#N/A</v>
       </c>
       <c r="K15" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L15" t="s">
+        <v>113</v>
+      </c>
+      <c r="M15" t="s">
         <v>181</v>
-      </c>
-      <c r="M15" t="s">
-        <v>183</v>
       </c>
       <c r="N15" t="s">
         <v>116</v>
@@ -4764,19 +4971,19 @@
         <v>#N/A</v>
       </c>
       <c r="K16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="M16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N16" t="s">
         <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -4797,19 +5004,19 @@
         <v>#N/A</v>
       </c>
       <c r="K17" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N17" t="s">
         <v>116</v>
       </c>
       <c r="O17" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -4830,19 +5037,19 @@
         <v>#N/A</v>
       </c>
       <c r="K18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N18" t="s">
         <v>116</v>
       </c>
       <c r="O18" t="s">
-        <v>182</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -4863,19 +5070,19 @@
         <v>#N/A</v>
       </c>
       <c r="K19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N19" t="s">
         <v>116</v>
       </c>
       <c r="O19" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -4896,19 +5103,19 @@
         <v>#N/A</v>
       </c>
       <c r="K20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N20" t="s">
         <v>116</v>
       </c>
       <c r="O20" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -4929,13 +5136,13 @@
         <v>#N/A</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L21" t="s">
         <v>113</v>
       </c>
       <c r="M21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N21" t="s">
         <v>116</v>
@@ -4962,19 +5169,19 @@
         <v>#N/A</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L22" t="s">
         <v>113</v>
       </c>
       <c r="M22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N22" t="s">
         <v>116</v>
       </c>
       <c r="O22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
@@ -4995,19 +5202,19 @@
         <v>#N/A</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L23" t="s">
         <v>113</v>
       </c>
       <c r="M23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N23" t="s">
         <v>116</v>
       </c>
       <c r="O23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
@@ -5028,13 +5235,13 @@
         <v>#N/A</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L24" t="s">
         <v>113</v>
       </c>
       <c r="M24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N24" t="s">
         <v>116</v>
@@ -5061,13 +5268,13 @@
         <v>#N/A</v>
       </c>
       <c r="K25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L25" t="s">
         <v>113</v>
       </c>
       <c r="M25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N25" t="s">
         <v>116</v>
@@ -5094,19 +5301,19 @@
         <v>#N/A</v>
       </c>
       <c r="K26" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="L26" t="s">
         <v>113</v>
       </c>
       <c r="M26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N26" t="s">
         <v>116</v>
       </c>
       <c r="O26" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
@@ -5127,13 +5334,13 @@
         <v>#N/A</v>
       </c>
       <c r="K27" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="L27" t="s">
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="M27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N27" t="s">
         <v>116</v>
@@ -5160,19 +5367,19 @@
         <v>#N/A</v>
       </c>
       <c r="K28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" t="s">
-        <v>118</v>
+        <v>6</v>
+      </c>
+      <c r="L28" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="M28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N28" t="s">
         <v>116</v>
       </c>
       <c r="O28" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
@@ -5193,19 +5400,19 @@
         <v>#N/A</v>
       </c>
       <c r="K29" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" t="s">
-        <v>118</v>
+        <v>7</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="M29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N29" t="s">
         <v>116</v>
       </c>
       <c r="O29" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
@@ -5226,19 +5433,19 @@
         <v>#N/A</v>
       </c>
       <c r="K30" t="s">
-        <v>24</v>
-      </c>
-      <c r="L30" t="s">
-        <v>118</v>
+        <v>8</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="M30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N30" t="s">
         <v>116</v>
       </c>
       <c r="O30" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
@@ -5259,19 +5466,19 @@
         <v>#N/A</v>
       </c>
       <c r="K31" t="s">
-        <v>25</v>
-      </c>
-      <c r="L31" t="s">
-        <v>118</v>
+        <v>12</v>
+      </c>
+      <c r="L31" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="M31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N31" t="s">
         <v>116</v>
       </c>
       <c r="O31" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
@@ -5292,19 +5499,19 @@
         <v>#N/A</v>
       </c>
       <c r="K32" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" t="s">
-        <v>118</v>
+        <v>30</v>
+      </c>
+      <c r="L32" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="M32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N32" t="s">
         <v>116</v>
       </c>
       <c r="O32" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
@@ -5325,19 +5532,19 @@
         <v>#N/A</v>
       </c>
       <c r="K33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" t="s">
-        <v>118</v>
+        <v>194</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="M33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N33" t="s">
         <v>116</v>
       </c>
       <c r="O33" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
@@ -5358,19 +5565,19 @@
         <v>#N/A</v>
       </c>
       <c r="K34" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" t="s">
-        <v>113</v>
+        <v>195</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="M34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N34" t="s">
         <v>116</v>
       </c>
       <c r="O34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
@@ -5391,19 +5598,19 @@
         <v>#N/A</v>
       </c>
       <c r="K35" t="s">
-        <v>29</v>
-      </c>
-      <c r="L35" t="s">
-        <v>115</v>
+        <v>196</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="M35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N35" t="s">
         <v>116</v>
       </c>
       <c r="O35" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
@@ -5424,19 +5631,19 @@
         <v>#N/A</v>
       </c>
       <c r="K36" t="s">
-        <v>30</v>
-      </c>
-      <c r="L36" t="s">
-        <v>115</v>
+        <v>11</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="M36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N36" t="s">
         <v>116</v>
       </c>
       <c r="O36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
@@ -5457,19 +5664,19 @@
         <v>#N/A</v>
       </c>
       <c r="K37" t="s">
-        <v>199</v>
-      </c>
-      <c r="L37" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="M37" t="s">
         <v>181</v>
-      </c>
-      <c r="M37" t="s">
-        <v>183</v>
       </c>
       <c r="N37" t="s">
         <v>116</v>
       </c>
       <c r="O37" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
@@ -5490,19 +5697,19 @@
         <v>#N/A</v>
       </c>
       <c r="K38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>181</v>
-      </c>
-      <c r="M38" t="s">
-        <v>183</v>
       </c>
       <c r="N38" t="s">
         <v>116</v>
       </c>
       <c r="O38" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
@@ -5523,19 +5730,19 @@
         <v>#N/A</v>
       </c>
       <c r="K39" t="s">
-        <v>201</v>
-      </c>
-      <c r="L39" t="s">
+        <v>29</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="M39" t="s">
         <v>181</v>
-      </c>
-      <c r="M39" t="s">
-        <v>183</v>
       </c>
       <c r="N39" t="s">
         <v>116</v>
       </c>
       <c r="O39" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
@@ -6386,10 +6593,10 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E87" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F87" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G87" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1)*1),MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1),"")))</f>
@@ -6402,10 +6609,10 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F88" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G88" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1)*1),MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1),"")))</f>
@@ -6418,10 +6625,10 @@
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G89" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1)*1),MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1),"")))</f>
@@ -6433,6 +6640,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K6:O39" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K7:O39">
+      <sortCondition ref="L6:L39"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update template for 11.jun new nodes setup
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07068765-9191-4342-A9A8-1DE3D9DD50BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC4538F-BBDA-4C9E-8A49-E6DCF53B33F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="32" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="207">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>EOMM Manolito</t>
+  </si>
+  <si>
+    <t>ALGO Manolito</t>
   </si>
 </sst>
 </file>
@@ -894,129 +897,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1055,7 +936,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1064,142 +945,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2394,7 +2139,7 @@
       </c>
       <c r="D17" s="19" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM Manolito</v>
       </c>
       <c r="E17" s="19" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2478,7 +2223,7 @@
       </c>
       <c r="D18" s="19" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM Manolito</v>
       </c>
       <c r="E18" s="19" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2562,7 +2307,7 @@
       </c>
       <c r="D19" s="19" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM Manolito</v>
       </c>
       <c r="E19" s="19" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -2646,7 +2391,7 @@
       </c>
       <c r="D20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
+        <v>EOMM Manolito</v>
       </c>
       <c r="E20" s="19" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -3906,7 +3651,7 @@
       </c>
       <c r="D35" s="19" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E35" s="19" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -4242,7 +3987,7 @@
       </c>
       <c r="D39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E39" s="19" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -4510,11 +4255,43 @@
   </sheetData>
   <autoFilter ref="B8:W41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}"/>
   <conditionalFormatting sqref="C9:V41">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="1">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:G41">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="9">
+      <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:L41 N9:Q41 T9:U41">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>I9=MIN(I$9:I$41)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J41">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K41">
@@ -4577,38 +4354,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I41 K9:L41 N9:Q41 J9:J41 T9:U41">
-    <cfRule type="expression" dxfId="18" priority="15">
-      <formula>I9=MIN(I$9:I$41)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J41">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9:G41">
-    <cfRule type="expression" dxfId="17" priority="8">
-      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="9">
-      <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="10">
-      <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="11">
-      <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4648,7 +4393,7 @@
   <dimension ref="B1:O89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4770,7 +4515,7 @@
         <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
       <c r="M8" t="s">
         <v>181</v>
@@ -4869,7 +4614,7 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
       <c r="M11" t="s">
         <v>181</v>
@@ -5430,7 +5175,7 @@
         <v>6</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="M28" t="s">
         <v>181</v>
@@ -5463,7 +5208,7 @@
         <v>7</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="M29" t="s">
         <v>181</v>
@@ -5496,7 +5241,7 @@
         <v>8</v>
       </c>
       <c r="L30" s="27" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="M30" t="s">
         <v>181</v>
@@ -5562,7 +5307,7 @@
         <v>30</v>
       </c>
       <c r="L32" s="27" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="M32" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
feat: improvements to template
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC4538F-BBDA-4C9E-8A49-E6DCF53B33F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3912DA0-E65F-4D91-8FD4-463B65FB8906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-9315" windowWidth="29040" windowHeight="15720" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="32" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="210">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -598,9 +598,6 @@
   </si>
   <si>
     <t>DEDICADO</t>
-  </si>
-  <si>
-    <t>THROTTLE</t>
   </si>
   <si>
     <t>MBP+MBO</t>
@@ -634,14 +631,8 @@
 (ms)</t>
   </si>
   <si>
-    <t>Prom. &lt; 95 (ms)</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID
 </t>
-  </si>
-  <si>
-    <t>Prom. &gt; 95 (ms)</t>
   </si>
   <si>
     <t>Comentario:</t>
@@ -694,6 +685,24 @@
   </si>
   <si>
     <t>ALGO Manolito</t>
+  </si>
+  <si>
+    <t>MBP THROTTLE</t>
+  </si>
+  <si>
+    <t>DMA (alg s/ppt)</t>
+  </si>
+  <si>
+    <t>ALGO (dm s/ ppt)</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Prom. &lt; P95 (ms)</t>
+  </si>
+  <si>
+    <t>Prom. &gt; P95 (ms)</t>
   </si>
 </sst>
 </file>
@@ -843,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -874,7 +883,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,7 +905,19 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -951,6 +971,60 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1284,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
   <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,20 +1374,23 @@
     <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="11.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" style="1" customWidth="1"/>
     <col min="14" max="17" width="8.88671875" style="1" customWidth="1"/>
     <col min="18" max="19" width="9.109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="7.88671875" style="1" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.109375" customWidth="1"/>
+    <col min="23" max="23" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>193</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="W2" s="8"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
@@ -1323,12 +1400,14 @@
       <c r="C4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="22"/>
+      <c r="W4" s="9"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
-        <v>192</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="W5" s="9"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C7" s="16">
@@ -1391,10 +1470,13 @@
       <c r="V7" s="16">
         <v>16</v>
       </c>
+      <c r="W7" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="2:23" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>33</v>
@@ -1403,31 +1485,31 @@
         <v>177</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>168</v>
       </c>
       <c r="H8" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="K8" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>170</v>
@@ -1439,7 +1521,7 @@
         <v>172</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>174</v>
@@ -1448,2789 +1530,2824 @@
         <v>0</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="V8" s="11" t="s">
         <v>173</v>
+      </c>
+      <c r="W8" s="11" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>541</v>
       </c>
-      <c r="D9" s="19" t="str">
+      <c r="D9" s="18" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E9" s="19" t="str">
+      <c r="E9" s="18" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F9" s="19" t="str">
+      <c r="F9" s="18" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G9" s="19" t="str">
+      <c r="G9" s="18" t="str">
         <f>+VLOOKUP($B9,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H9" s="21" t="str">
+      <c r="H9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B9,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I9" s="21" t="str">
+      <c r="I9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J9" s="21" t="str">
+      <c r="J9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K9" s="21" t="str">
+      <c r="K9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L9" s="21" t="str">
+      <c r="L9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M9" s="21" t="str">
+      <c r="M9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N9" s="21" t="str">
+      <c r="N9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O9" s="21" t="str">
+      <c r="O9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P9" s="21" t="str">
+      <c r="P9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q9" s="21" t="str">
+      <c r="Q9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R9" s="21" t="str">
+      <c r="R9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S9" s="21" t="str">
+      <c r="S9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T9" s="21" t="str">
+      <c r="T9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U9" s="21" t="str">
+      <c r="U9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V9" s="21" t="str">
+      <c r="V9" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B9,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B9,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W9" s="23"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>543</v>
       </c>
-      <c r="D10" s="19" t="str">
+      <c r="D10" s="18" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E10" s="19" t="str">
+      <c r="E10" s="18" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F10" s="19" t="str">
+      <c r="F10" s="18" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G10" s="19" t="str">
+      <c r="G10" s="18" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H10" s="21" t="str">
+      <c r="H10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B10,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I10" s="21" t="str">
+      <c r="I10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J10" s="21" t="str">
+      <c r="J10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K10" s="21" t="str">
+      <c r="K10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L10" s="21" t="str">
+      <c r="L10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M10" s="21" t="str">
+      <c r="M10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N10" s="21" t="str">
+      <c r="N10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O10" s="21" t="str">
+      <c r="O10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P10" s="21" t="str">
+      <c r="P10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q10" s="21" t="str">
+      <c r="Q10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R10" s="21" t="str">
+      <c r="R10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S10" s="21" t="str">
+      <c r="S10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T10" s="21" t="str">
+      <c r="T10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U10" s="21" t="str">
+      <c r="U10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V10" s="21" t="str">
+      <c r="V10" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B10,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B10,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W10" s="23"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>544</v>
       </c>
-      <c r="D11" s="19" t="str">
+      <c r="D11" s="18" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E11" s="19" t="str">
+      <c r="E11" s="18" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F11" s="19" t="str">
+      <c r="F11" s="18" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G11" s="19" t="str">
+      <c r="G11" s="18" t="str">
         <f>+VLOOKUP($B11,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H11" s="21" t="str">
+      <c r="H11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B11,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I11" s="21" t="str">
+      <c r="I11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J11" s="21" t="str">
+      <c r="J11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K11" s="21" t="str">
+      <c r="K11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L11" s="21" t="str">
+      <c r="L11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M11" s="21" t="str">
+      <c r="M11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N11" s="21" t="str">
+      <c r="N11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O11" s="21" t="str">
+      <c r="O11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P11" s="21" t="str">
+      <c r="P11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q11" s="21" t="str">
+      <c r="Q11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R11" s="21" t="str">
+      <c r="R11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S11" s="21" t="str">
+      <c r="S11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T11" s="21" t="str">
+      <c r="T11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U11" s="21" t="str">
+      <c r="U11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V11" s="21" t="str">
+      <c r="V11" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B11,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B11,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W11" s="23"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <v>981</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="D12" s="18" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E12" s="19" t="str">
+      <c r="E12" s="18" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F12" s="19" t="str">
+      <c r="F12" s="18" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G12" s="19" t="str">
+      <c r="G12" s="18" t="str">
         <f>+VLOOKUP($B12,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H12" s="21" t="str">
+      <c r="H12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B12,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I12" s="21" t="str">
+      <c r="I12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J12" s="21" t="str">
+      <c r="J12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K12" s="21" t="str">
+      <c r="K12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L12" s="21" t="str">
+      <c r="L12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M12" s="21" t="str">
+      <c r="M12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N12" s="21" t="str">
+      <c r="N12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O12" s="21" t="str">
+      <c r="O12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P12" s="21" t="str">
+      <c r="P12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q12" s="21" t="str">
+      <c r="Q12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R12" s="21" t="str">
+      <c r="R12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S12" s="21" t="str">
+      <c r="S12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T12" s="21" t="str">
+      <c r="T12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U12" s="21" t="str">
+      <c r="U12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V12" s="21" t="str">
+      <c r="V12" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B12,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B12,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W12" s="23"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C13" s="24">
-        <v>1362</v>
-      </c>
-      <c r="D13" s="19" t="str">
+        <v>30</v>
+      </c>
+      <c r="C13" s="23">
+        <v>982</v>
+      </c>
+      <c r="D13" s="18" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E13" s="19" t="str">
+      <c r="E13" s="18" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F13" s="19" t="str">
+      <c r="F13" s="18" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G13" s="19" t="str">
+      <c r="G13" s="18" t="str">
         <f>+VLOOKUP($B13,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H13" s="21" t="str">
+      <c r="H13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B13,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I13" s="21" t="str">
+      <c r="I13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J13" s="21" t="str">
+      <c r="J13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K13" s="21" t="str">
+      <c r="K13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L13" s="21" t="str">
+      <c r="L13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M13" s="21" t="str">
+      <c r="M13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N13" s="21" t="str">
+      <c r="N13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O13" s="21" t="str">
+      <c r="O13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P13" s="21" t="str">
+      <c r="P13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q13" s="21" t="str">
+      <c r="Q13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R13" s="21" t="str">
+      <c r="R13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S13" s="21" t="str">
+      <c r="S13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T13" s="21" t="str">
+      <c r="T13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U13" s="21" t="str">
+      <c r="U13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V13" s="21" t="str">
+      <c r="V13" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B13,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B13,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W13" s="23"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="24">
-        <v>1372</v>
-      </c>
-      <c r="D14" s="19" t="str">
+        <v>6</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1146</v>
+      </c>
+      <c r="D14" s="18" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E14" s="19" t="str">
+      <c r="E14" s="18" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F14" s="19" t="str">
+      <c r="F14" s="18" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G14" s="19" t="str">
+      <c r="G14" s="18" t="str">
         <f>+VLOOKUP($B14,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H14" s="21" t="str">
+      <c r="H14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B14,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I14" s="21" t="str">
+      <c r="I14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J14" s="21" t="str">
+      <c r="J14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K14" s="21" t="str">
+      <c r="K14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L14" s="21" t="str">
+      <c r="L14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M14" s="21" t="str">
+      <c r="M14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N14" s="21" t="str">
+      <c r="N14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O14" s="21" t="str">
+      <c r="O14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P14" s="21" t="str">
+      <c r="P14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q14" s="21" t="str">
+      <c r="Q14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R14" s="21" t="str">
+      <c r="R14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S14" s="21" t="str">
+      <c r="S14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T14" s="21" t="str">
+      <c r="T14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U14" s="21" t="str">
+      <c r="U14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V14" s="21" t="str">
+      <c r="V14" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B14,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B14,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
+      <c r="W14" s="23"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="C15" s="24">
-        <v>1373</v>
-      </c>
-      <c r="D15" s="19" t="str">
+        <v>7</v>
+      </c>
+      <c r="C15" s="23">
+        <v>1147</v>
+      </c>
+      <c r="D15" s="18" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E15" s="19" t="str">
+      <c r="E15" s="18" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F15" s="19" t="str">
+      <c r="F15" s="18" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G15" s="19" t="str">
+      <c r="G15" s="18" t="str">
         <f>+VLOOKUP($B15,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H15" s="21" t="str">
+      <c r="H15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B15,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I15" s="21" t="str">
+      <c r="I15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J15" s="21" t="str">
+      <c r="J15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K15" s="21" t="str">
+      <c r="K15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L15" s="21" t="str">
+      <c r="L15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M15" s="21" t="str">
+      <c r="M15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N15" s="21" t="str">
+      <c r="N15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O15" s="21" t="str">
+      <c r="O15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P15" s="21" t="str">
+      <c r="P15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q15" s="21" t="str">
+      <c r="Q15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R15" s="21" t="str">
+      <c r="R15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S15" s="21" t="str">
+      <c r="S15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T15" s="21" t="str">
+      <c r="T15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U15" s="21" t="str">
+      <c r="U15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V15" s="21" t="str">
+      <c r="V15" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B15,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B15,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="W15" s="18"/>
+      <c r="W15" s="23"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="24">
-        <v>542</v>
-      </c>
-      <c r="D16" s="19" t="str">
+        <v>8</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1148</v>
+      </c>
+      <c r="D16" s="18" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM</v>
-      </c>
-      <c r="E16" s="19" t="str">
+        <v>EOMM Manolito</v>
+      </c>
+      <c r="E16" s="18" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F16" s="19" t="str">
+      <c r="F16" s="18" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G16" s="19" t="str">
+      <c r="G16" s="18" t="str">
         <f>+VLOOKUP($B16,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H16" s="21" t="str">
+      <c r="H16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B16,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I16" s="21" t="str">
+      <c r="I16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J16" s="21" t="str">
+      <c r="J16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K16" s="21" t="str">
+      <c r="K16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L16" s="21" t="str">
+      <c r="L16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M16" s="21" t="str">
+      <c r="M16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N16" s="21" t="str">
+      <c r="N16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O16" s="21" t="str">
+      <c r="O16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P16" s="21" t="str">
+      <c r="P16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q16" s="21" t="str">
+      <c r="Q16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R16" s="21" t="str">
+      <c r="R16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S16" s="21" t="str">
+      <c r="S16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T16" s="21" t="str">
+      <c r="T16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U16" s="21" t="str">
+      <c r="U16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V16" s="21" t="str">
+      <c r="V16" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B16,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W16" s="23"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="24">
-        <v>982</v>
-      </c>
-      <c r="D17" s="19" t="str">
+        <v>191</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1362</v>
+      </c>
+      <c r="D17" s="18" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E17" s="19" t="str">
+      <c r="E17" s="18" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F17" s="19" t="str">
+      <c r="F17" s="18" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G17" s="19" t="str">
+      <c r="G17" s="18" t="str">
         <f>+VLOOKUP($B17,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H17" s="21" t="str">
+      <c r="H17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B17,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I17" s="21" t="str">
+      <c r="I17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J17" s="21" t="str">
+      <c r="J17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K17" s="21" t="str">
+      <c r="K17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L17" s="21" t="str">
+      <c r="L17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M17" s="21" t="str">
+      <c r="M17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N17" s="21" t="str">
+      <c r="N17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O17" s="21" t="str">
+      <c r="O17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P17" s="21" t="str">
+      <c r="P17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q17" s="21" t="str">
+      <c r="Q17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R17" s="21" t="str">
+      <c r="R17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S17" s="21" t="str">
+      <c r="S17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T17" s="21" t="str">
+      <c r="T17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U17" s="21" t="str">
+      <c r="U17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V17" s="21" t="str">
+      <c r="V17" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B17,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B17,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W17" s="23"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="24">
-        <v>1146</v>
-      </c>
-      <c r="D18" s="19" t="str">
+        <v>192</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1372</v>
+      </c>
+      <c r="D18" s="18" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E18" s="19" t="str">
+      <c r="E18" s="18" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F18" s="19" t="str">
+      <c r="F18" s="18" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G18" s="19" t="str">
+      <c r="G18" s="18" t="str">
         <f>+VLOOKUP($B18,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H18" s="21" t="str">
+      <c r="H18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B18,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I18" s="21" t="str">
+      <c r="I18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J18" s="21" t="str">
+      <c r="J18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K18" s="21" t="str">
+      <c r="K18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L18" s="21" t="str">
+      <c r="L18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M18" s="21" t="str">
+      <c r="M18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N18" s="21" t="str">
+      <c r="N18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O18" s="21" t="str">
+      <c r="O18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P18" s="21" t="str">
+      <c r="P18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q18" s="21" t="str">
+      <c r="Q18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R18" s="21" t="str">
+      <c r="R18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S18" s="21" t="str">
+      <c r="S18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T18" s="21" t="str">
+      <c r="T18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U18" s="21" t="str">
+      <c r="U18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V18" s="21" t="str">
+      <c r="V18" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B18,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B18,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W18" s="23"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="24">
-        <v>1147</v>
-      </c>
-      <c r="D19" s="19" t="str">
+        <v>193</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1373</v>
+      </c>
+      <c r="D19" s="18" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>EOMM Manolito</v>
       </c>
-      <c r="E19" s="19" t="str">
+      <c r="E19" s="18" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F19" s="19" t="str">
+      <c r="F19" s="18" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G19" s="19" t="str">
+      <c r="G19" s="18" t="str">
         <f>+VLOOKUP($B19,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H19" s="21" t="str">
+      <c r="H19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B19,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I19" s="21" t="str">
+      <c r="I19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J19" s="21" t="str">
+      <c r="J19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K19" s="21" t="str">
+      <c r="K19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L19" s="21" t="str">
+      <c r="L19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M19" s="21" t="str">
+      <c r="M19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N19" s="21" t="str">
+      <c r="N19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O19" s="21" t="str">
+      <c r="O19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P19" s="21" t="str">
+      <c r="P19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q19" s="21" t="str">
+      <c r="Q19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R19" s="21" t="str">
+      <c r="R19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S19" s="21" t="str">
+      <c r="S19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T19" s="21" t="str">
+      <c r="T19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U19" s="21" t="str">
+      <c r="U19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V19" s="21" t="str">
+      <c r="V19" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B19,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B19,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W19" s="23"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="24">
-        <v>1148</v>
-      </c>
-      <c r="D20" s="19" t="str">
+        <v>12</v>
+      </c>
+      <c r="C20" s="23">
+        <v>542</v>
+      </c>
+      <c r="D20" s="18" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>EOMM Manolito</v>
-      </c>
-      <c r="E20" s="19" t="str">
+        <v>EOMM</v>
+      </c>
+      <c r="E20" s="18" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F20" s="19" t="str">
+      <c r="F20" s="18" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G20" s="19" t="str">
+      <c r="G20" s="18" t="str">
         <f>+VLOOKUP($B20,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP+MBO</v>
       </c>
-      <c r="H20" s="21" t="str">
+      <c r="H20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B20,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I20" s="21" t="str">
+      <c r="I20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J20" s="21" t="str">
+      <c r="J20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K20" s="21" t="str">
+      <c r="K20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L20" s="21" t="str">
+      <c r="L20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M20" s="21" t="str">
+      <c r="M20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N20" s="21" t="str">
+      <c r="N20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O20" s="21" t="str">
+      <c r="O20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P20" s="21" t="str">
+      <c r="P20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q20" s="21" t="str">
+      <c r="Q20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R20" s="21" t="str">
+      <c r="R20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S20" s="21" t="str">
+      <c r="S20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T20" s="21" t="str">
+      <c r="T20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U20" s="21" t="str">
+      <c r="U20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V20" s="21" t="str">
+      <c r="V20" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B20,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B20,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W20" s="23"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="23">
         <v>1256</v>
       </c>
-      <c r="D21" s="19" t="str">
+      <c r="D21" s="18" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA Artemis J21</v>
       </c>
-      <c r="E21" s="19" t="str">
+      <c r="E21" s="18" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F21" s="19" t="str">
+      <c r="F21" s="18" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G21" s="19" t="str">
+      <c r="G21" s="18" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H21" s="21" t="str">
+      <c r="H21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B21,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I21" s="21" t="str">
+      <c r="I21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J21" s="21" t="str">
+      <c r="J21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K21" s="21" t="str">
+      <c r="K21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L21" s="21" t="str">
+      <c r="L21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M21" s="21" t="str">
+      <c r="M21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N21" s="21" t="str">
+      <c r="N21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O21" s="21" t="str">
+      <c r="O21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P21" s="21" t="str">
+      <c r="P21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q21" s="21" t="str">
+      <c r="Q21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R21" s="21" t="str">
+      <c r="R21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S21" s="21" t="str">
+      <c r="S21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T21" s="21" t="str">
+      <c r="T21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U21" s="21" t="str">
+      <c r="U21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V21" s="21" t="str">
+      <c r="V21" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B21,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W21" s="23"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="24">
-        <v>819</v>
-      </c>
-      <c r="D22" s="19" t="str">
+        <v>10</v>
+      </c>
+      <c r="C22" s="23">
+        <v>354</v>
+      </c>
+      <c r="D22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>DMA</v>
-      </c>
-      <c r="E22" s="19" t="str">
+        <v>DMA (alg s/ppt)</v>
+      </c>
+      <c r="E22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F22" s="19" t="str">
+      <c r="F22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G22" s="19" t="str">
+      <c r="G22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>DEDICADO</v>
-      </c>
-      <c r="H22" s="21" t="str">
+        <v>MBP</v>
+      </c>
+      <c r="H22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B22,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I22" s="21" t="str">
+      <c r="I22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J22" s="21" t="str">
+      <c r="J22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K22" s="21" t="str">
+      <c r="K22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L22" s="21" t="str">
+      <c r="L22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M22" s="21" t="str">
+      <c r="M22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N22" s="21" t="str">
+      <c r="N22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O22" s="21" t="str">
+      <c r="O22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P22" s="21" t="str">
+      <c r="P22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q22" s="21" t="str">
+      <c r="Q22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R22" s="21" t="str">
+      <c r="R22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S22" s="21" t="str">
+      <c r="S22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T22" s="21" t="str">
+      <c r="T22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U22" s="21" t="str">
+      <c r="U22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V22" s="21" t="str">
+      <c r="V22" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B22,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W22" s="23"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="24">
-        <v>1115</v>
-      </c>
-      <c r="D23" s="19" t="str">
+        <v>28</v>
+      </c>
+      <c r="C23" s="23">
+        <v>819</v>
+      </c>
+      <c r="D23" s="18" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E23" s="19" t="str">
+      <c r="E23" s="18" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F23" s="19" t="str">
+      <c r="F23" s="18" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G23" s="19" t="str">
+      <c r="G23" s="18" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>DEDICADO</v>
       </c>
-      <c r="H23" s="21" t="str">
+      <c r="H23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B23,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I23" s="21" t="str">
+      <c r="I23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J23" s="21" t="str">
+      <c r="J23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K23" s="21" t="str">
+      <c r="K23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L23" s="21" t="str">
+      <c r="L23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M23" s="21" t="str">
+      <c r="M23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N23" s="21" t="str">
+      <c r="N23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O23" s="21" t="str">
+      <c r="O23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P23" s="21" t="str">
+      <c r="P23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q23" s="21" t="str">
+      <c r="Q23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R23" s="21" t="str">
+      <c r="R23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S23" s="21" t="str">
+      <c r="S23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T23" s="21" t="str">
+      <c r="T23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U23" s="21" t="str">
+      <c r="U23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V23" s="21" t="str">
+      <c r="V23" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B23,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W23" s="23"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="24">
-        <v>1116</v>
-      </c>
-      <c r="D24" s="19" t="str">
+        <v>3</v>
+      </c>
+      <c r="C24" s="23">
+        <v>1115</v>
+      </c>
+      <c r="D24" s="18" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E24" s="19" t="str">
+      <c r="E24" s="18" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F24" s="19" t="str">
+      <c r="F24" s="18" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G24" s="19" t="str">
+      <c r="G24" s="18" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>DEDICADO</v>
       </c>
-      <c r="H24" s="21" t="str">
+      <c r="H24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B24,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I24" s="21" t="str">
+      <c r="I24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J24" s="21" t="str">
+      <c r="J24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K24" s="21" t="str">
+      <c r="K24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L24" s="21" t="str">
+      <c r="L24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M24" s="21" t="str">
+      <c r="M24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N24" s="21" t="str">
+      <c r="N24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O24" s="21" t="str">
+      <c r="O24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P24" s="21" t="str">
+      <c r="P24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q24" s="21" t="str">
+      <c r="Q24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R24" s="21" t="str">
+      <c r="R24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S24" s="21" t="str">
+      <c r="S24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T24" s="21" t="str">
+      <c r="T24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U24" s="21" t="str">
+      <c r="U24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V24" s="21" t="str">
+      <c r="V24" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B24,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W24" s="23"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="24">
-        <v>1003</v>
-      </c>
-      <c r="D25" s="19" t="str">
+        <v>4</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1116</v>
+      </c>
+      <c r="D25" s="18" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E25" s="19" t="str">
+      <c r="E25" s="18" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F25" s="19" t="str">
+      <c r="F25" s="18" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G25" s="19" t="str">
+      <c r="G25" s="18" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>THROTTLE</v>
-      </c>
-      <c r="H25" s="21" t="str">
+        <v>DEDICADO</v>
+      </c>
+      <c r="H25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B25,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I25" s="21" t="str">
+      <c r="I25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J25" s="21" t="str">
+      <c r="J25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K25" s="21" t="str">
+      <c r="K25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L25" s="21" t="str">
+      <c r="L25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M25" s="21" t="str">
+      <c r="M25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N25" s="21" t="str">
+      <c r="N25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O25" s="21" t="str">
+      <c r="O25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P25" s="21" t="str">
+      <c r="P25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q25" s="21" t="str">
+      <c r="Q25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R25" s="21" t="str">
+      <c r="R25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S25" s="21" t="str">
+      <c r="S25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T25" s="21" t="str">
+      <c r="T25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U25" s="21" t="str">
+      <c r="U25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V25" s="21" t="str">
+      <c r="V25" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B25,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W25" s="23"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="23">
         <v>559</v>
       </c>
-      <c r="D26" s="19" t="str">
+      <c r="D26" s="18" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E26" s="19" t="str">
+      <c r="E26" s="18" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F26" s="19" t="str">
+      <c r="F26" s="18" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G26" s="19" t="str">
+      <c r="G26" s="18" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H26" s="21" t="str">
+      <c r="H26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B26,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I26" s="21" t="str">
+      <c r="I26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J26" s="21" t="str">
+      <c r="J26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K26" s="21" t="str">
+      <c r="K26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L26" s="21" t="str">
+      <c r="L26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M26" s="21" t="str">
+      <c r="M26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N26" s="21" t="str">
+      <c r="N26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O26" s="21" t="str">
+      <c r="O26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P26" s="21" t="str">
+      <c r="P26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q26" s="21" t="str">
+      <c r="Q26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R26" s="21" t="str">
+      <c r="R26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S26" s="21" t="str">
+      <c r="S26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T26" s="21" t="str">
+      <c r="T26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U26" s="21" t="str">
+      <c r="U26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V26" s="21" t="str">
+      <c r="V26" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B26,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W26" s="23"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="23">
         <v>560</v>
       </c>
-      <c r="D27" s="19" t="str">
+      <c r="D27" s="18" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E27" s="19" t="str">
+      <c r="E27" s="18" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F27" s="19" t="str">
+      <c r="F27" s="18" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G27" s="19" t="str">
+      <c r="G27" s="18" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H27" s="21" t="str">
+      <c r="H27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B27,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I27" s="21" t="str">
+      <c r="I27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J27" s="21" t="str">
+      <c r="J27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K27" s="21" t="str">
+      <c r="K27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L27" s="21" t="str">
+      <c r="L27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M27" s="21" t="str">
+      <c r="M27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N27" s="21" t="str">
+      <c r="N27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O27" s="21" t="str">
+      <c r="O27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P27" s="21" t="str">
+      <c r="P27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q27" s="21" t="str">
+      <c r="Q27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R27" s="21" t="str">
+      <c r="R27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S27" s="21" t="str">
+      <c r="S27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T27" s="21" t="str">
+      <c r="T27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U27" s="21" t="str">
+      <c r="U27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V27" s="21" t="str">
+      <c r="V27" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B27,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B27,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W27" s="23"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="23">
         <v>561</v>
       </c>
-      <c r="D28" s="19" t="str">
+      <c r="D28" s="18" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E28" s="19" t="str">
+      <c r="E28" s="18" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F28" s="19" t="str">
+      <c r="F28" s="18" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G28" s="19" t="str">
+      <c r="G28" s="18" t="str">
         <f>+VLOOKUP($B28,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H28" s="21" t="str">
+      <c r="H28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B28,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I28" s="21" t="str">
+      <c r="I28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J28" s="21" t="str">
+      <c r="J28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K28" s="21" t="str">
+      <c r="K28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L28" s="21" t="str">
+      <c r="L28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M28" s="21" t="str">
+      <c r="M28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N28" s="21" t="str">
+      <c r="N28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O28" s="21" t="str">
+      <c r="O28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P28" s="21" t="str">
+      <c r="P28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q28" s="21" t="str">
+      <c r="Q28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R28" s="21" t="str">
+      <c r="R28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S28" s="21" t="str">
+      <c r="S28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T28" s="21" t="str">
+      <c r="T28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U28" s="21" t="str">
+      <c r="U28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V28" s="21" t="str">
+      <c r="V28" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B28,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B28,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W28" s="23"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="23">
         <v>562</v>
       </c>
-      <c r="D29" s="19" t="str">
+      <c r="D29" s="18" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E29" s="19" t="str">
+      <c r="E29" s="18" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F29" s="19" t="str">
+      <c r="F29" s="18" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G29" s="19" t="str">
+      <c r="G29" s="18" t="str">
         <f>+VLOOKUP($B29,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H29" s="21" t="str">
+      <c r="H29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B29,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I29" s="21" t="str">
+      <c r="I29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J29" s="21" t="str">
+      <c r="J29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K29" s="21" t="str">
+      <c r="K29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L29" s="21" t="str">
+      <c r="L29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M29" s="21" t="str">
+      <c r="M29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N29" s="21" t="str">
+      <c r="N29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O29" s="21" t="str">
+      <c r="O29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P29" s="21" t="str">
+      <c r="P29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q29" s="21" t="str">
+      <c r="Q29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R29" s="21" t="str">
+      <c r="R29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S29" s="21" t="str">
+      <c r="S29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T29" s="21" t="str">
+      <c r="T29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U29" s="21" t="str">
+      <c r="U29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V29" s="21" t="str">
+      <c r="V29" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B29,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B29,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W29" s="23"/>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <v>563</v>
       </c>
-      <c r="D30" s="19" t="str">
+      <c r="D30" s="18" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E30" s="19" t="str">
+      <c r="E30" s="18" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F30" s="19" t="str">
+      <c r="F30" s="18" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G30" s="19" t="str">
+      <c r="G30" s="18" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H30" s="21" t="str">
+      <c r="H30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B30,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I30" s="21" t="str">
+      <c r="I30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J30" s="21" t="str">
+      <c r="J30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K30" s="21" t="str">
+      <c r="K30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L30" s="21" t="str">
+      <c r="L30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M30" s="21" t="str">
+      <c r="M30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N30" s="21" t="str">
+      <c r="N30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O30" s="21" t="str">
+      <c r="O30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P30" s="21" t="str">
+      <c r="P30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q30" s="21" t="str">
+      <c r="Q30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R30" s="21" t="str">
+      <c r="R30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S30" s="21" t="str">
+      <c r="S30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T30" s="21" t="str">
+      <c r="T30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U30" s="21" t="str">
+      <c r="U30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V30" s="21" t="str">
+      <c r="V30" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B30,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B30,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W30" s="23"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="23">
         <v>564</v>
       </c>
-      <c r="D31" s="19" t="str">
+      <c r="D31" s="18" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E31" s="19" t="str">
+      <c r="E31" s="18" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F31" s="19" t="str">
+      <c r="F31" s="18" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G31" s="19" t="str">
+      <c r="G31" s="18" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H31" s="21" t="str">
+      <c r="H31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B31,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I31" s="21" t="str">
+      <c r="I31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J31" s="21" t="str">
+      <c r="J31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K31" s="21" t="str">
+      <c r="K31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L31" s="21" t="str">
+      <c r="L31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M31" s="21" t="str">
+      <c r="M31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N31" s="21" t="str">
+      <c r="N31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O31" s="21" t="str">
+      <c r="O31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P31" s="21" t="str">
+      <c r="P31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q31" s="21" t="str">
+      <c r="Q31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R31" s="21" t="str">
+      <c r="R31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S31" s="21" t="str">
+      <c r="S31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T31" s="21" t="str">
+      <c r="T31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U31" s="21" t="str">
+      <c r="U31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V31" s="21" t="str">
+      <c r="V31" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B31,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B31,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W31" s="23"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="23">
         <v>565</v>
       </c>
-      <c r="D32" s="19" t="str">
+      <c r="D32" s="18" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E32" s="19" t="str">
+      <c r="E32" s="18" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F32" s="19" t="str">
+      <c r="F32" s="18" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G32" s="19" t="str">
+      <c r="G32" s="18" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H32" s="21" t="str">
+      <c r="H32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B32,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I32" s="21" t="str">
+      <c r="I32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J32" s="21" t="str">
+      <c r="J32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K32" s="21" t="str">
+      <c r="K32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L32" s="21" t="str">
+      <c r="L32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M32" s="21" t="str">
+      <c r="M32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N32" s="21" t="str">
+      <c r="N32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O32" s="21" t="str">
+      <c r="O32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P32" s="21" t="str">
+      <c r="P32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q32" s="21" t="str">
+      <c r="Q32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R32" s="21" t="str">
+      <c r="R32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S32" s="21" t="str">
+      <c r="S32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T32" s="21" t="str">
+      <c r="T32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U32" s="21" t="str">
+      <c r="U32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V32" s="21" t="str">
+      <c r="V32" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B32,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B32,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W32" s="23"/>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="23">
         <v>1114</v>
       </c>
-      <c r="D33" s="19" t="str">
+      <c r="D33" s="18" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E33" s="19" t="str">
+      <c r="E33" s="18" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F33" s="19" t="str">
+      <c r="F33" s="18" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G33" s="19" t="str">
+      <c r="G33" s="18" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H33" s="21" t="str">
+      <c r="H33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B33,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I33" s="21" t="str">
+      <c r="I33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J33" s="21" t="str">
+      <c r="J33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K33" s="21" t="str">
+      <c r="K33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L33" s="21" t="str">
+      <c r="L33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M33" s="21" t="str">
+      <c r="M33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N33" s="21" t="str">
+      <c r="N33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O33" s="21" t="str">
+      <c r="O33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P33" s="21" t="str">
+      <c r="P33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q33" s="21" t="str">
+      <c r="Q33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R33" s="21" t="str">
+      <c r="R33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S33" s="21" t="str">
+      <c r="S33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T33" s="21" t="str">
+      <c r="T33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U33" s="21" t="str">
+      <c r="U33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V33" s="21" t="str">
+      <c r="V33" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B33,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B33,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W33" s="23"/>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>1118</v>
       </c>
-      <c r="D34" s="19" t="str">
+      <c r="D34" s="18" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>DMA</v>
       </c>
-      <c r="E34" s="19" t="str">
+      <c r="E34" s="18" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F34" s="19" t="str">
+      <c r="F34" s="18" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G34" s="19" t="str">
+      <c r="G34" s="18" t="str">
         <f>+VLOOKUP($B34,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H34" s="21" t="str">
+      <c r="H34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B34,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I34" s="21" t="str">
+      <c r="I34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J34" s="21" t="str">
+      <c r="J34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K34" s="21" t="str">
+      <c r="K34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L34" s="21" t="str">
+      <c r="L34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M34" s="21" t="str">
+      <c r="M34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N34" s="21" t="str">
+      <c r="N34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O34" s="21" t="str">
+      <c r="O34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P34" s="21" t="str">
+      <c r="P34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q34" s="21" t="str">
+      <c r="Q34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R34" s="21" t="str">
+      <c r="R34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S34" s="21" t="str">
+      <c r="S34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T34" s="21" t="str">
+      <c r="T34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U34" s="21" t="str">
+      <c r="U34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V34" s="21" t="str">
+      <c r="V34" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B34,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B34,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W34" s="23"/>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="23">
         <v>578</v>
       </c>
-      <c r="D35" s="19" t="str">
+      <c r="D35" s="18" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO Manolito</v>
       </c>
-      <c r="E35" s="19" t="str">
+      <c r="E35" s="18" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F35" s="19" t="str">
+      <c r="F35" s="18" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G35" s="19" t="str">
+      <c r="G35" s="18" t="str">
         <f>+VLOOKUP($B35,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H35" s="21" t="str">
+      <c r="H35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B35,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I35" s="21" t="str">
+      <c r="I35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J35" s="21" t="str">
+      <c r="J35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K35" s="21" t="str">
+      <c r="K35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L35" s="21" t="str">
+      <c r="L35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M35" s="21" t="str">
+      <c r="M35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N35" s="21" t="str">
+      <c r="N35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O35" s="21" t="str">
+      <c r="O35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P35" s="21" t="str">
+      <c r="P35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q35" s="21" t="str">
+      <c r="Q35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R35" s="21" t="str">
+      <c r="R35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S35" s="21" t="str">
+      <c r="S35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T35" s="21" t="str">
+      <c r="T35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U35" s="21" t="str">
+      <c r="U35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V35" s="21" t="str">
+      <c r="V35" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B35,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B35,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W35" s="23"/>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="23">
         <v>579</v>
       </c>
-      <c r="D36" s="19" t="str">
+      <c r="D36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO</v>
       </c>
-      <c r="E36" s="19" t="str">
+      <c r="E36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F36" s="19" t="str">
+      <c r="F36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G36" s="19" t="str">
+      <c r="G36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H36" s="21" t="str">
+      <c r="H36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B36,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I36" s="21" t="str">
+      <c r="I36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J36" s="21" t="str">
+      <c r="J36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K36" s="21" t="str">
+      <c r="K36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L36" s="21" t="str">
+      <c r="L36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M36" s="21" t="str">
+      <c r="M36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N36" s="21" t="str">
+      <c r="N36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O36" s="21" t="str">
+      <c r="O36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P36" s="21" t="str">
+      <c r="P36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q36" s="21" t="str">
+      <c r="Q36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R36" s="21" t="str">
+      <c r="R36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S36" s="21" t="str">
+      <c r="S36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T36" s="21" t="str">
+      <c r="T36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U36" s="21" t="str">
+      <c r="U36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V36" s="21" t="str">
+      <c r="V36" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B36,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B36,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W36" s="23"/>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="23">
         <v>580</v>
       </c>
-      <c r="D37" s="19" t="str">
+      <c r="D37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO</v>
       </c>
-      <c r="E37" s="19" t="str">
+      <c r="E37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F37" s="19" t="str">
+      <c r="F37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G37" s="19" t="str">
+      <c r="G37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBO</v>
       </c>
-      <c r="H37" s="21" t="str">
+      <c r="H37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B37,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I37" s="21" t="str">
+      <c r="I37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J37" s="21" t="str">
+      <c r="J37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K37" s="21" t="str">
+      <c r="K37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L37" s="21" t="str">
+      <c r="L37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M37" s="21" t="str">
+      <c r="M37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N37" s="21" t="str">
+      <c r="N37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O37" s="21" t="str">
+      <c r="O37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P37" s="21" t="str">
+      <c r="P37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q37" s="21" t="str">
+      <c r="Q37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R37" s="21" t="str">
+      <c r="R37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S37" s="21" t="str">
+      <c r="S37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T37" s="21" t="str">
+      <c r="T37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U37" s="21" t="str">
+      <c r="U37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V37" s="21" t="str">
+      <c r="V37" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B37,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B37,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W37" s="23"/>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="24">
-        <v>354</v>
-      </c>
-      <c r="D38" s="19" t="str">
+        <v>1</v>
+      </c>
+      <c r="C38" s="23">
+        <v>1003</v>
+      </c>
+      <c r="D38" s="18" t="str">
         <f>+VLOOKUP($B38,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
-      </c>
-      <c r="E38" s="19" t="str">
+        <v>ALGO (dm s/ ppt)</v>
+      </c>
+      <c r="E38" s="18" t="str">
         <f>+VLOOKUP($B38,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F38" s="19" t="str">
+      <c r="F38" s="18" t="str">
         <f>+VLOOKUP($B38,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G38" s="19" t="str">
+      <c r="G38" s="18" t="str">
         <f>+VLOOKUP($B38,'Users+Static Data'!$K:$O,G$7,0)</f>
-        <v>MBP</v>
-      </c>
-      <c r="H38" s="21" t="str">
+        <v>MBP THROTTLE</v>
+      </c>
+      <c r="H38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B38,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I38" s="21" t="str">
+      <c r="I38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J38" s="21" t="str">
+      <c r="J38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K38" s="21" t="str">
+      <c r="K38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L38" s="21" t="str">
+      <c r="L38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M38" s="21" t="str">
+      <c r="M38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N38" s="21" t="str">
+      <c r="N38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O38" s="21" t="str">
+      <c r="O38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P38" s="21" t="str">
+      <c r="P38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q38" s="21" t="str">
+      <c r="Q38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R38" s="21" t="str">
+      <c r="R38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S38" s="21" t="str">
+      <c r="S38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T38" s="21" t="str">
+      <c r="T38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U38" s="21" t="str">
+      <c r="U38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V38" s="21" t="str">
+      <c r="V38" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B38,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B38,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W38" s="23"/>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="23">
         <v>581</v>
       </c>
-      <c r="D39" s="19" t="str">
+      <c r="D39" s="18" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO Manolito</v>
       </c>
-      <c r="E39" s="19" t="str">
+      <c r="E39" s="18" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F39" s="19" t="str">
+      <c r="F39" s="18" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G39" s="19" t="str">
+      <c r="G39" s="18" t="str">
         <f>+VLOOKUP($B39,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H39" s="21" t="str">
+      <c r="H39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B39,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I39" s="21" t="str">
+      <c r="I39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J39" s="21" t="str">
+      <c r="J39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K39" s="21" t="str">
+      <c r="K39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L39" s="21" t="str">
+      <c r="L39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M39" s="21" t="str">
+      <c r="M39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N39" s="21" t="str">
+      <c r="N39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O39" s="21" t="str">
+      <c r="O39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P39" s="21" t="str">
+      <c r="P39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q39" s="21" t="str">
+      <c r="Q39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R39" s="21" t="str">
+      <c r="R39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S39" s="21" t="str">
+      <c r="S39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T39" s="21" t="str">
+      <c r="T39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U39" s="21" t="str">
+      <c r="U39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V39" s="21" t="str">
+      <c r="V39" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B39,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B39,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W39" s="23"/>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="23">
         <v>582</v>
       </c>
-      <c r="D40" s="19" t="str">
+      <c r="D40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO</v>
       </c>
-      <c r="E40" s="19" t="str">
+      <c r="E40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F40" s="19" t="str">
+      <c r="F40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G40" s="19" t="str">
+      <c r="G40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H40" s="21" t="str">
+      <c r="H40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B40,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I40" s="21" t="str">
+      <c r="I40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J40" s="21" t="str">
+      <c r="J40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K40" s="21" t="str">
+      <c r="K40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L40" s="21" t="str">
+      <c r="L40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M40" s="21" t="str">
+      <c r="M40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N40" s="21" t="str">
+      <c r="N40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O40" s="21" t="str">
+      <c r="O40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P40" s="21" t="str">
+      <c r="P40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q40" s="21" t="str">
+      <c r="Q40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R40" s="21" t="str">
+      <c r="R40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S40" s="21" t="str">
+      <c r="S40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T40" s="21" t="str">
+      <c r="T40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U40" s="21" t="str">
+      <c r="U40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V40" s="21" t="str">
+      <c r="V40" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B40,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B40,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W40" s="23"/>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="24">
         <v>583</v>
       </c>
-      <c r="D41" s="20" t="str">
+      <c r="D41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,D$7,0)</f>
         <v>ALGO</v>
       </c>
-      <c r="E41" s="20" t="str">
+      <c r="E41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,E$7,0)</f>
         <v>BE</v>
       </c>
-      <c r="F41" s="20" t="str">
+      <c r="F41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,F$7,0)</f>
         <v>MD</v>
       </c>
-      <c r="G41" s="20" t="str">
+      <c r="G41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,G$7,0)</f>
         <v>MBP</v>
       </c>
-      <c r="H41" s="21" t="str">
+      <c r="H41" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Users+Static Data'!$F:$H,H$7,0),0)=0,"n/a",VLOOKUP($B41,'Users+Static Data'!$F:$H,H$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="I41" s="22" t="str">
+      <c r="I41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,I$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,I$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="J41" s="22" t="str">
+      <c r="J41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,J$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="K41" s="22" t="str">
+      <c r="K41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,K$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="L41" s="22" t="str">
+      <c r="L41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,L$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="M41" s="22" t="str">
+      <c r="M41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,M$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="N41" s="22" t="str">
+      <c r="N41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,N$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="O41" s="22" t="str">
+      <c r="O41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,O$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="P41" s="22" t="str">
+      <c r="P41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,P$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="Q41" s="22" t="str">
+      <c r="Q41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,Q$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="R41" s="22" t="str">
+      <c r="R41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,R$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="S41" s="22" t="str">
+      <c r="S41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,S$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="T41" s="22" t="str">
+      <c r="T41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,T$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="U41" s="22" t="str">
+      <c r="U41" s="21" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,U$7,0))</f>
         <v>n/a</v>
       </c>
-      <c r="V41" s="21" t="str">
+      <c r="V41" s="20" t="str">
         <f>IF(IFERROR(VLOOKUP($B41,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B41,'Report Data'!$A:$AG,V$7,0))</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W41" s="24"/>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -4251,41 +4368,33 @@
       <c r="T42" s="14"/>
       <c r="U42" s="14"/>
       <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:W41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}"/>
-  <conditionalFormatting sqref="C9:V41">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <autoFilter ref="B8:W41" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:W41">
+      <sortCondition descending="1" ref="D8:D41"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="D9:G41">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9:G41">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:L41 N9:Q41 T9:U41">
-    <cfRule type="expression" dxfId="0" priority="15">
-      <formula>I9=MIN(I$9:I$41)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J9:J41">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4295,7 +4404,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K41">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4305,7 +4414,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:O41">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4315,7 +4424,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:P41">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4325,7 +4434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9:Q41">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4335,7 +4444,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:T41">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4344,14 +4453,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="T9:U41 N9:Q41 I9:L41">
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>I9=MIN(I$9:I$41)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="U9:U41">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:W41">
+    <cfRule type="expression" dxfId="11" priority="3">
+      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="4">
+      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4392,8 +4514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
   <dimension ref="B1:O89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4411,25 +4533,25 @@
     <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-    </row>
-    <row r="5" spans="2:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+    <row r="1" spans="2:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" spans="2:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="2:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="2:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="2:15" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
@@ -4453,10 +4575,10 @@
         <v>177</v>
       </c>
       <c r="M6" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>183</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>168</v>
@@ -4482,10 +4604,10 @@
         <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="M7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N7" t="s">
         <v>116</v>
@@ -4515,10 +4637,10 @@
         <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N8" t="s">
         <v>116</v>
@@ -4551,7 +4673,7 @@
         <v>118</v>
       </c>
       <c r="M9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N9" t="s">
         <v>116</v>
@@ -4584,7 +4706,7 @@
         <v>118</v>
       </c>
       <c r="M10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N10" t="s">
         <v>116</v>
@@ -4614,10 +4736,10 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N11" t="s">
         <v>116</v>
@@ -4650,7 +4772,7 @@
         <v>118</v>
       </c>
       <c r="M12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N12" t="s">
         <v>116</v>
@@ -4683,7 +4805,7 @@
         <v>118</v>
       </c>
       <c r="M13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N13" t="s">
         <v>116</v>
@@ -4713,16 +4835,16 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="M14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N14" t="s">
         <v>116</v>
       </c>
       <c r="O14" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -4749,7 +4871,7 @@
         <v>113</v>
       </c>
       <c r="M15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N15" t="s">
         <v>116</v>
@@ -4782,7 +4904,7 @@
         <v>113</v>
       </c>
       <c r="M16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N16" t="s">
         <v>116</v>
@@ -4815,7 +4937,7 @@
         <v>113</v>
       </c>
       <c r="M17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N17" t="s">
         <v>116</v>
@@ -4848,7 +4970,7 @@
         <v>113</v>
       </c>
       <c r="M18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N18" t="s">
         <v>116</v>
@@ -4881,7 +5003,7 @@
         <v>113</v>
       </c>
       <c r="M19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N19" t="s">
         <v>116</v>
@@ -4914,7 +5036,7 @@
         <v>113</v>
       </c>
       <c r="M20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N20" t="s">
         <v>116</v>
@@ -4947,7 +5069,7 @@
         <v>113</v>
       </c>
       <c r="M21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N21" t="s">
         <v>116</v>
@@ -4980,7 +5102,7 @@
         <v>113</v>
       </c>
       <c r="M22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N22" t="s">
         <v>116</v>
@@ -5013,7 +5135,7 @@
         <v>113</v>
       </c>
       <c r="M23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N23" t="s">
         <v>116</v>
@@ -5046,7 +5168,7 @@
         <v>113</v>
       </c>
       <c r="M24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N24" t="s">
         <v>116</v>
@@ -5079,7 +5201,7 @@
         <v>113</v>
       </c>
       <c r="M25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N25" t="s">
         <v>116</v>
@@ -5112,7 +5234,7 @@
         <v>113</v>
       </c>
       <c r="M26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N26" t="s">
         <v>116</v>
@@ -5142,10 +5264,10 @@
         <v>9</v>
       </c>
       <c r="L27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N27" t="s">
         <v>116</v>
@@ -5174,17 +5296,17 @@
       <c r="K28" t="s">
         <v>6</v>
       </c>
-      <c r="L28" s="27" t="s">
-        <v>205</v>
+      <c r="L28" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N28" t="s">
         <v>116</v>
       </c>
       <c r="O28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
@@ -5207,17 +5329,17 @@
       <c r="K29" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="27" t="s">
-        <v>205</v>
+      <c r="L29" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N29" t="s">
         <v>116</v>
       </c>
       <c r="O29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
@@ -5240,17 +5362,17 @@
       <c r="K30" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="27" t="s">
-        <v>205</v>
+      <c r="L30" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N30" t="s">
         <v>116</v>
       </c>
       <c r="O30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
@@ -5273,17 +5395,17 @@
       <c r="K31" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="27" t="s">
+      <c r="L31" s="26" t="s">
         <v>115</v>
       </c>
       <c r="M31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N31" t="s">
         <v>116</v>
       </c>
       <c r="O31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
@@ -5306,17 +5428,17 @@
       <c r="K32" t="s">
         <v>30</v>
       </c>
-      <c r="L32" s="27" t="s">
-        <v>205</v>
+      <c r="L32" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N32" t="s">
         <v>116</v>
       </c>
       <c r="O32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
@@ -5337,19 +5459,19 @@
         <v>#N/A</v>
       </c>
       <c r="K33" t="s">
-        <v>194</v>
-      </c>
-      <c r="L33" s="27" t="s">
-        <v>205</v>
+        <v>191</v>
+      </c>
+      <c r="L33" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N33" t="s">
         <v>116</v>
       </c>
       <c r="O33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
@@ -5370,19 +5492,19 @@
         <v>#N/A</v>
       </c>
       <c r="K34" t="s">
-        <v>195</v>
-      </c>
-      <c r="L34" s="27" t="s">
-        <v>205</v>
+        <v>192</v>
+      </c>
+      <c r="L34" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N34" t="s">
         <v>116</v>
       </c>
       <c r="O34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
@@ -5403,19 +5525,19 @@
         <v>#N/A</v>
       </c>
       <c r="K35" t="s">
-        <v>196</v>
-      </c>
-      <c r="L35" s="27" t="s">
-        <v>205</v>
+        <v>193</v>
+      </c>
+      <c r="L35" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N35" t="s">
         <v>116</v>
       </c>
       <c r="O35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
@@ -5438,17 +5560,17 @@
       <c r="K36" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="27" t="s">
-        <v>205</v>
+      <c r="L36" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N36" t="s">
         <v>116</v>
       </c>
       <c r="O36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
@@ -5471,17 +5593,17 @@
       <c r="K37" t="s">
         <v>13</v>
       </c>
-      <c r="L37" s="27" t="s">
-        <v>205</v>
+      <c r="L37" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N37" t="s">
         <v>116</v>
       </c>
       <c r="O37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
@@ -5504,17 +5626,17 @@
       <c r="K38" t="s">
         <v>14</v>
       </c>
-      <c r="L38" s="27" t="s">
-        <v>205</v>
+      <c r="L38" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N38" t="s">
         <v>116</v>
       </c>
       <c r="O38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
@@ -5537,17 +5659,17 @@
       <c r="K39" t="s">
         <v>29</v>
       </c>
-      <c r="L39" s="27" t="s">
-        <v>205</v>
+      <c r="L39" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="M39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N39" t="s">
         <v>116</v>
       </c>
       <c r="O39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
@@ -6398,10 +6520,10 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E87" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F87" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G87" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1)*1),MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1),"")))</f>
@@ -6414,10 +6536,10 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F88" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G88" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1)*1),MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1),"")))</f>
@@ -6430,10 +6552,10 @@
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F89" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G89" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1)*1),MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1),"")))</f>

</xml_diff>

<commit_message>
feat: template updated to match new node deploys
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3912DA0-E65F-4D91-8FD4-463B65FB8906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED893B6-DAC7-448B-BBA8-9AC3DE216779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-9315" windowWidth="29040" windowHeight="15720" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="209">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>MBO</t>
-  </si>
-  <si>
-    <t>ALGO</t>
   </si>
   <si>
     <t>197/delay.log</t>
@@ -690,9 +687,6 @@
     <t>MBP THROTTLE</t>
   </si>
   <si>
-    <t>DMA (alg s/ppt)</t>
-  </si>
-  <si>
     <t>ALGO (dm s/ ppt)</t>
   </si>
   <si>
@@ -703,6 +697,9 @@
   </si>
   <si>
     <t>Prom. &gt; P95 (ms)</t>
+  </si>
+  <si>
+    <t>DMA Mano. (alg s/ppt)</t>
   </si>
 </sst>
 </file>
@@ -905,19 +902,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -971,60 +956,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1358,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
   <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,7 +1319,7 @@
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="W2" s="8"/>
     </row>
@@ -1405,7 +1336,7 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="W5" s="9"/>
     </row>
@@ -1476,70 +1407,70 @@
     </row>
     <row r="8" spans="2:23" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="K8" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="L8" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q8" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="R8" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
@@ -2224,7 +2155,7 @@
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="23">
         <v>1362</v>
@@ -2309,7 +2240,7 @@
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" s="23">
         <v>1372</v>
@@ -2394,7 +2325,7 @@
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C19" s="23">
         <v>1373</v>
@@ -2656,7 +2587,7 @@
       </c>
       <c r="D22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>DMA (alg s/ppt)</v>
+        <v>DMA Mano. (alg s/ppt)</v>
       </c>
       <c r="E22" s="18" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -3846,7 +3777,7 @@
       </c>
       <c r="D36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E36" s="18" t="str">
         <f>+VLOOKUP($B36,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -3931,7 +3862,7 @@
       </c>
       <c r="D37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E37" s="18" t="str">
         <f>+VLOOKUP($B37,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -4186,7 +4117,7 @@
       </c>
       <c r="D40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E40" s="18" t="str">
         <f>+VLOOKUP($B40,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -4271,7 +4202,7 @@
       </c>
       <c r="D41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,D$7,0)</f>
-        <v>ALGO</v>
+        <v>ALGO Manolito</v>
       </c>
       <c r="E41" s="19" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$O,E$7,0)</f>
@@ -4376,21 +4307,34 @@
       <sortCondition descending="1" ref="D8:D41"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="D9:G41">
-    <cfRule type="expression" dxfId="17" priority="7">
+  <conditionalFormatting sqref="C9:W41">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="11">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:G41">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:L41 N9:Q41 T9:U41">
+    <cfRule type="expression" dxfId="0" priority="18">
+      <formula>I9=MIN(I$9:I$41)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J41">
@@ -4453,11 +4397,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T9:U41 N9:Q41 I9:L41">
-    <cfRule type="expression" dxfId="12" priority="18">
-      <formula>I9=MIN(I$9:I$41)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U9:U41">
     <cfRule type="colorScale" priority="42">
       <colorScale>
@@ -4466,14 +4405,6 @@
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:W41">
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>ISNUMBER(SEARCH("Manolito", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>ISNUMBER(SEARCH("J21", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4557,38 +4488,38 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M6" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="N6" s="8" t="s">
-        <v>182</v>
-      </c>
       <c r="O6" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -4604,10 +4535,10 @@
         <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="M7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N7" t="s">
         <v>116</v>
@@ -4623,7 +4554,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F8,ROW(INDIRECT("1"&amp;":"&amp;LEN(F8))),1)*1),MID(F8,ROW(INDIRECT("1"&amp;":"&amp;LEN(F8))),1),"")))</f>
@@ -4637,10 +4568,10 @@
         <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N8" t="s">
         <v>116</v>
@@ -4656,7 +4587,7 @@
         <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G9" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F9,ROW(INDIRECT("1"&amp;":"&amp;LEN(F9))),1)*1),MID(F9,ROW(INDIRECT("1"&amp;":"&amp;LEN(F9))),1),"")))</f>
@@ -4670,10 +4601,10 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="M9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N9" t="s">
         <v>116</v>
@@ -4689,7 +4620,7 @@
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G10" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F10,ROW(INDIRECT("1"&amp;":"&amp;LEN(F10))),1)*1),MID(F10,ROW(INDIRECT("1"&amp;":"&amp;LEN(F10))),1),"")))</f>
@@ -4703,10 +4634,10 @@
         <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="M10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N10" t="s">
         <v>116</v>
@@ -4722,7 +4653,7 @@
         <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G11" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F11,ROW(INDIRECT("1"&amp;":"&amp;LEN(F11))),1)*1),MID(F11,ROW(INDIRECT("1"&amp;":"&amp;LEN(F11))),1),"")))</f>
@@ -4736,10 +4667,10 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N11" t="s">
         <v>116</v>
@@ -4755,7 +4686,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G12" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F12,ROW(INDIRECT("1"&amp;":"&amp;LEN(F12))),1)*1),MID(F12,ROW(INDIRECT("1"&amp;":"&amp;LEN(F12))),1),"")))</f>
@@ -4769,10 +4700,10 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="M12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N12" t="s">
         <v>116</v>
@@ -4788,7 +4719,7 @@
         <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F13,ROW(INDIRECT("1"&amp;":"&amp;LEN(F13))),1)*1),MID(F13,ROW(INDIRECT("1"&amp;":"&amp;LEN(F13))),1),"")))</f>
@@ -4802,10 +4733,10 @@
         <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="M13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N13" t="s">
         <v>116</v>
@@ -4835,16 +4766,16 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N14" t="s">
         <v>116</v>
       </c>
       <c r="O14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -4871,7 +4802,7 @@
         <v>113</v>
       </c>
       <c r="M15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N15" t="s">
         <v>116</v>
@@ -4904,13 +4835,13 @@
         <v>113</v>
       </c>
       <c r="M16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N16" t="s">
         <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -4920,7 +4851,7 @@
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G17" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F17,ROW(INDIRECT("1"&amp;":"&amp;LEN(F17))),1)*1),MID(F17,ROW(INDIRECT("1"&amp;":"&amp;LEN(F17))),1),"")))</f>
@@ -4937,13 +4868,13 @@
         <v>113</v>
       </c>
       <c r="M17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N17" t="s">
         <v>116</v>
       </c>
       <c r="O17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -4953,7 +4884,7 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G18" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F18,ROW(INDIRECT("1"&amp;":"&amp;LEN(F18))),1)*1),MID(F18,ROW(INDIRECT("1"&amp;":"&amp;LEN(F18))),1),"")))</f>
@@ -4970,7 +4901,7 @@
         <v>113</v>
       </c>
       <c r="M18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N18" t="s">
         <v>116</v>
@@ -4986,7 +4917,7 @@
         <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G19" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F19,ROW(INDIRECT("1"&amp;":"&amp;LEN(F19))),1)*1),MID(F19,ROW(INDIRECT("1"&amp;":"&amp;LEN(F19))),1),"")))</f>
@@ -5003,7 +4934,7 @@
         <v>113</v>
       </c>
       <c r="M19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N19" t="s">
         <v>116</v>
@@ -5019,7 +4950,7 @@
         <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G20" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F20,ROW(INDIRECT("1"&amp;":"&amp;LEN(F20))),1)*1),MID(F20,ROW(INDIRECT("1"&amp;":"&amp;LEN(F20))),1),"")))</f>
@@ -5036,7 +4967,7 @@
         <v>113</v>
       </c>
       <c r="M20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N20" t="s">
         <v>116</v>
@@ -5052,7 +4983,7 @@
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G21" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F21,ROW(INDIRECT("1"&amp;":"&amp;LEN(F21))),1)*1),MID(F21,ROW(INDIRECT("1"&amp;":"&amp;LEN(F21))),1),"")))</f>
@@ -5069,7 +5000,7 @@
         <v>113</v>
       </c>
       <c r="M21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N21" t="s">
         <v>116</v>
@@ -5102,7 +5033,7 @@
         <v>113</v>
       </c>
       <c r="M22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N22" t="s">
         <v>116</v>
@@ -5135,7 +5066,7 @@
         <v>113</v>
       </c>
       <c r="M23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N23" t="s">
         <v>116</v>
@@ -5168,7 +5099,7 @@
         <v>113</v>
       </c>
       <c r="M24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N24" t="s">
         <v>116</v>
@@ -5184,7 +5115,7 @@
         <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G25" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F25,ROW(INDIRECT("1"&amp;":"&amp;LEN(F25))),1)*1),MID(F25,ROW(INDIRECT("1"&amp;":"&amp;LEN(F25))),1),"")))</f>
@@ -5201,7 +5132,7 @@
         <v>113</v>
       </c>
       <c r="M25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N25" t="s">
         <v>116</v>
@@ -5217,7 +5148,7 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G26" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F26,ROW(INDIRECT("1"&amp;":"&amp;LEN(F26))),1)*1),MID(F26,ROW(INDIRECT("1"&amp;":"&amp;LEN(F26))),1),"")))</f>
@@ -5234,13 +5165,13 @@
         <v>113</v>
       </c>
       <c r="M26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N26" t="s">
         <v>116</v>
       </c>
       <c r="O26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
@@ -5250,7 +5181,7 @@
         <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G27" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F27,ROW(INDIRECT("1"&amp;":"&amp;LEN(F27))),1)*1),MID(F27,ROW(INDIRECT("1"&amp;":"&amp;LEN(F27))),1),"")))</f>
@@ -5264,10 +5195,10 @@
         <v>9</v>
       </c>
       <c r="L27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N27" t="s">
         <v>116</v>
@@ -5283,7 +5214,7 @@
         <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G28" cm="1">
         <f t="array" aca="1" ref="G28" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F28,ROW(INDIRECT("1"&amp;":"&amp;LEN(F28))),1)*1),MID(F28,ROW(INDIRECT("1"&amp;":"&amp;LEN(F28))),1),"")))</f>
@@ -5297,16 +5228,16 @@
         <v>6</v>
       </c>
       <c r="L28" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N28" t="s">
         <v>116</v>
       </c>
       <c r="O28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
@@ -5316,7 +5247,7 @@
         <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" cm="1">
         <f t="array" aca="1" ref="G29" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F29,ROW(INDIRECT("1"&amp;":"&amp;LEN(F29))),1)*1),MID(F29,ROW(INDIRECT("1"&amp;":"&amp;LEN(F29))),1),"")))</f>
@@ -5330,16 +5261,16 @@
         <v>7</v>
       </c>
       <c r="L29" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N29" t="s">
         <v>116</v>
       </c>
       <c r="O29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
@@ -5349,7 +5280,7 @@
         <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" cm="1">
         <f t="array" aca="1" ref="G30" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F30,ROW(INDIRECT("1"&amp;":"&amp;LEN(F30))),1)*1),MID(F30,ROW(INDIRECT("1"&amp;":"&amp;LEN(F30))),1),"")))</f>
@@ -5363,16 +5294,16 @@
         <v>8</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N30" t="s">
         <v>116</v>
       </c>
       <c r="O30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
@@ -5382,7 +5313,7 @@
         <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31" cm="1">
         <f t="array" aca="1" ref="G31" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F31,ROW(INDIRECT("1"&amp;":"&amp;LEN(F31))),1)*1),MID(F31,ROW(INDIRECT("1"&amp;":"&amp;LEN(F31))),1),"")))</f>
@@ -5399,13 +5330,13 @@
         <v>115</v>
       </c>
       <c r="M31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N31" t="s">
         <v>116</v>
       </c>
       <c r="O31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
@@ -5415,7 +5346,7 @@
         <v>58</v>
       </c>
       <c r="F32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G32" cm="1">
         <f t="array" aca="1" ref="G32" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F32,ROW(INDIRECT("1"&amp;":"&amp;LEN(F32))),1)*1),MID(F32,ROW(INDIRECT("1"&amp;":"&amp;LEN(F32))),1),"")))</f>
@@ -5429,16 +5360,16 @@
         <v>30</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N32" t="s">
         <v>116</v>
       </c>
       <c r="O32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
@@ -5448,7 +5379,7 @@
         <v>59</v>
       </c>
       <c r="F33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G33" cm="1">
         <f t="array" aca="1" ref="G33" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F33,ROW(INDIRECT("1"&amp;":"&amp;LEN(F33))),1)*1),MID(F33,ROW(INDIRECT("1"&amp;":"&amp;LEN(F33))),1),"")))</f>
@@ -5459,19 +5390,19 @@
         <v>#N/A</v>
       </c>
       <c r="K33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L33" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N33" t="s">
         <v>116</v>
       </c>
       <c r="O33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
@@ -5481,7 +5412,7 @@
         <v>60</v>
       </c>
       <c r="F34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G34" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F34,ROW(INDIRECT("1"&amp;":"&amp;LEN(F34))),1)*1),MID(F34,ROW(INDIRECT("1"&amp;":"&amp;LEN(F34))),1),"")))</f>
@@ -5492,19 +5423,19 @@
         <v>#N/A</v>
       </c>
       <c r="K34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L34" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N34" t="s">
         <v>116</v>
       </c>
       <c r="O34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
@@ -5525,19 +5456,19 @@
         <v>#N/A</v>
       </c>
       <c r="K35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N35" t="s">
         <v>116</v>
       </c>
       <c r="O35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
@@ -5547,7 +5478,7 @@
         <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G36" cm="1">
         <f t="array" aca="1" ref="G36" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F36,ROW(INDIRECT("1"&amp;":"&amp;LEN(F36))),1)*1),MID(F36,ROW(INDIRECT("1"&amp;":"&amp;LEN(F36))),1),"")))</f>
@@ -5561,16 +5492,16 @@
         <v>11</v>
       </c>
       <c r="L36" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N36" t="s">
         <v>116</v>
       </c>
       <c r="O36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
@@ -5580,7 +5511,7 @@
         <v>63</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G37" cm="1">
         <f t="array" aca="1" ref="G37" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F37,ROW(INDIRECT("1"&amp;":"&amp;LEN(F37))),1)*1),MID(F37,ROW(INDIRECT("1"&amp;":"&amp;LEN(F37))),1),"")))</f>
@@ -5594,16 +5525,16 @@
         <v>13</v>
       </c>
       <c r="L37" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N37" t="s">
         <v>116</v>
       </c>
       <c r="O37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
@@ -5627,16 +5558,16 @@
         <v>14</v>
       </c>
       <c r="L38" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N38" t="s">
         <v>116</v>
       </c>
       <c r="O38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
@@ -5660,16 +5591,16 @@
         <v>29</v>
       </c>
       <c r="L39" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N39" t="s">
         <v>116</v>
       </c>
       <c r="O39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
@@ -5697,7 +5628,7 @@
         <v>67</v>
       </c>
       <c r="F41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G41" cm="1">
         <f t="array" aca="1" ref="G41" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F41,ROW(INDIRECT("1"&amp;":"&amp;LEN(F41))),1)*1),MID(F41,ROW(INDIRECT("1"&amp;":"&amp;LEN(F41))),1),"")))</f>
@@ -5715,7 +5646,7 @@
         <v>68</v>
       </c>
       <c r="F42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G42" cm="1">
         <f t="array" aca="1" ref="G42" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F42,ROW(INDIRECT("1"&amp;":"&amp;LEN(F42))),1)*1),MID(F42,ROW(INDIRECT("1"&amp;":"&amp;LEN(F42))),1),"")))</f>
@@ -5751,7 +5682,7 @@
         <v>70</v>
       </c>
       <c r="F44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G44" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F44,ROW(INDIRECT("1"&amp;":"&amp;LEN(F44))),1)*1),MID(F44,ROW(INDIRECT("1"&amp;":"&amp;LEN(F44))),1),"")))</f>
@@ -5769,7 +5700,7 @@
         <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G45" cm="1">
         <f t="array" aca="1" ref="G45" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F45,ROW(INDIRECT("1"&amp;":"&amp;LEN(F45))),1)*1),MID(F45,ROW(INDIRECT("1"&amp;":"&amp;LEN(F45))),1),"")))</f>
@@ -5787,7 +5718,7 @@
         <v>72</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G46" cm="1">
         <f t="array" aca="1" ref="G46" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F46,ROW(INDIRECT("1"&amp;":"&amp;LEN(F46))),1)*1),MID(F46,ROW(INDIRECT("1"&amp;":"&amp;LEN(F46))),1),"")))</f>
@@ -5823,7 +5754,7 @@
         <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G48" cm="1">
         <f t="array" aca="1" ref="G48" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F48,ROW(INDIRECT("1"&amp;":"&amp;LEN(F48))),1)*1),MID(F48,ROW(INDIRECT("1"&amp;":"&amp;LEN(F48))),1),"")))</f>
@@ -5841,7 +5772,7 @@
         <v>75</v>
       </c>
       <c r="F49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G49" cm="1">
         <f t="array" aca="1" ref="G49" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F49,ROW(INDIRECT("1"&amp;":"&amp;LEN(F49))),1)*1),MID(F49,ROW(INDIRECT("1"&amp;":"&amp;LEN(F49))),1),"")))</f>
@@ -5859,7 +5790,7 @@
         <v>76</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G50" cm="1">
         <f t="array" aca="1" ref="G50" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F50,ROW(INDIRECT("1"&amp;":"&amp;LEN(F50))),1)*1),MID(F50,ROW(INDIRECT("1"&amp;":"&amp;LEN(F50))),1),"")))</f>
@@ -5913,7 +5844,7 @@
         <v>79</v>
       </c>
       <c r="F53" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G53" cm="1">
         <f t="array" aca="1" ref="G53" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F53,ROW(INDIRECT("1"&amp;":"&amp;LEN(F53))),1)*1),MID(F53,ROW(INDIRECT("1"&amp;":"&amp;LEN(F53))),1),"")))</f>
@@ -5931,7 +5862,7 @@
         <v>80</v>
       </c>
       <c r="F54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G54" cm="1">
         <f t="array" aca="1" ref="G54" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F54,ROW(INDIRECT("1"&amp;":"&amp;LEN(F54))),1)*1),MID(F54,ROW(INDIRECT("1"&amp;":"&amp;LEN(F54))),1),"")))</f>
@@ -5967,7 +5898,7 @@
         <v>82</v>
       </c>
       <c r="F56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G56" cm="1">
         <f t="array" aca="1" ref="G56" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F56,ROW(INDIRECT("1"&amp;":"&amp;LEN(F56))),1)*1),MID(F56,ROW(INDIRECT("1"&amp;":"&amp;LEN(F56))),1),"")))</f>
@@ -6003,7 +5934,7 @@
         <v>84</v>
       </c>
       <c r="F58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G58" cm="1">
         <f t="array" aca="1" ref="G58" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F58,ROW(INDIRECT("1"&amp;":"&amp;LEN(F58))),1)*1),MID(F58,ROW(INDIRECT("1"&amp;":"&amp;LEN(F58))),1),"")))</f>
@@ -6057,7 +5988,7 @@
         <v>87</v>
       </c>
       <c r="F61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G61" cm="1">
         <f t="array" aca="1" ref="G61" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F61,ROW(INDIRECT("1"&amp;":"&amp;LEN(F61))),1)*1),MID(F61,ROW(INDIRECT("1"&amp;":"&amp;LEN(F61))),1),"")))</f>
@@ -6075,7 +6006,7 @@
         <v>88</v>
       </c>
       <c r="F62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G62" cm="1">
         <f t="array" aca="1" ref="G62" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F62,ROW(INDIRECT("1"&amp;":"&amp;LEN(F62))),1)*1),MID(F62,ROW(INDIRECT("1"&amp;":"&amp;LEN(F62))),1),"")))</f>
@@ -6111,7 +6042,7 @@
         <v>90</v>
       </c>
       <c r="F64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G64" cm="1">
         <f t="array" aca="1" ref="G64" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F64,ROW(INDIRECT("1"&amp;":"&amp;LEN(F64))),1)*1),MID(F64,ROW(INDIRECT("1"&amp;":"&amp;LEN(F64))),1),"")))</f>
@@ -6165,7 +6096,7 @@
         <v>93</v>
       </c>
       <c r="F67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G67" cm="1">
         <f t="array" aca="1" ref="G67" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F67,ROW(INDIRECT("1"&amp;":"&amp;LEN(F67))),1)*1),MID(F67,ROW(INDIRECT("1"&amp;":"&amp;LEN(F67))),1),"")))</f>
@@ -6183,7 +6114,7 @@
         <v>94</v>
       </c>
       <c r="F68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G68" cm="1">
         <f t="array" aca="1" ref="G68" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F68,ROW(INDIRECT("1"&amp;":"&amp;LEN(F68))),1)*1),MID(F68,ROW(INDIRECT("1"&amp;":"&amp;LEN(F68))),1),"")))</f>
@@ -6201,7 +6132,7 @@
         <v>95</v>
       </c>
       <c r="F69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G69" cm="1">
         <f t="array" aca="1" ref="G69" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F69,ROW(INDIRECT("1"&amp;":"&amp;LEN(F69))),1)*1),MID(F69,ROW(INDIRECT("1"&amp;":"&amp;LEN(F69))),1),"")))</f>
@@ -6219,7 +6150,7 @@
         <v>96</v>
       </c>
       <c r="F70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G70" cm="1">
         <f t="array" aca="1" ref="G70" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F70,ROW(INDIRECT("1"&amp;":"&amp;LEN(F70))),1)*1),MID(F70,ROW(INDIRECT("1"&amp;":"&amp;LEN(F70))),1),"")))</f>
@@ -6237,7 +6168,7 @@
         <v>97</v>
       </c>
       <c r="F71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G71" cm="1">
         <f t="array" aca="1" ref="G71" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F71,ROW(INDIRECT("1"&amp;":"&amp;LEN(F71))),1)*1),MID(F71,ROW(INDIRECT("1"&amp;":"&amp;LEN(F71))),1),"")))</f>
@@ -6327,7 +6258,7 @@
         <v>102</v>
       </c>
       <c r="F76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G76" cm="1">
         <f t="array" aca="1" ref="G76" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F76,ROW(INDIRECT("1"&amp;":"&amp;LEN(F76))),1)*1),MID(F76,ROW(INDIRECT("1"&amp;":"&amp;LEN(F76))),1),"")))</f>
@@ -6345,7 +6276,7 @@
         <v>103</v>
       </c>
       <c r="F77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G77" cm="1">
         <f t="array" aca="1" ref="G77" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F77,ROW(INDIRECT("1"&amp;":"&amp;LEN(F77))),1)*1),MID(F77,ROW(INDIRECT("1"&amp;":"&amp;LEN(F77))),1),"")))</f>
@@ -6381,7 +6312,7 @@
         <v>105</v>
       </c>
       <c r="F79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G79" cm="1">
         <f t="array" aca="1" ref="G79" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F79,ROW(INDIRECT("1"&amp;":"&amp;LEN(F79))),1)*1),MID(F79,ROW(INDIRECT("1"&amp;":"&amp;LEN(F79))),1),"")))</f>
@@ -6399,7 +6330,7 @@
         <v>106</v>
       </c>
       <c r="F80" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G80" cm="1">
         <f t="array" aca="1" ref="G80" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F80,ROW(INDIRECT("1"&amp;":"&amp;LEN(F80))),1)*1),MID(F80,ROW(INDIRECT("1"&amp;":"&amp;LEN(F80))),1),"")))</f>
@@ -6417,7 +6348,7 @@
         <v>107</v>
       </c>
       <c r="F81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G81" cm="1">
         <f t="array" aca="1" ref="G81" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F81,ROW(INDIRECT("1"&amp;":"&amp;LEN(F81))),1)*1),MID(F81,ROW(INDIRECT("1"&amp;":"&amp;LEN(F81))),1),"")))</f>
@@ -6435,7 +6366,7 @@
         <v>108</v>
       </c>
       <c r="F82" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G82" cm="1">
         <f t="array" aca="1" ref="G82" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F82,ROW(INDIRECT("1"&amp;":"&amp;LEN(F82))),1)*1),MID(F82,ROW(INDIRECT("1"&amp;":"&amp;LEN(F82))),1),"")))</f>
@@ -6520,10 +6451,10 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G87" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1)*1),MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1),"")))</f>
@@ -6536,10 +6467,10 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F88" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G88" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1)*1),MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1),"")))</f>
@@ -6552,10 +6483,10 @@
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G89" cm="1">
         <f t="array" aca="1" ref="G89" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1)*1),MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1),"")))</f>

</xml_diff>

<commit_message>
refactor: minor change in style
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BD00B6-8C39-42AD-AC51-79BDBF90C2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544E8034-7432-4EA4-BFCD-982668805855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -945,150 +945,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -1144,39 +1001,16 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1219,18 +1053,6 @@
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1564,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
   <dimension ref="B2:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4725,16 +4547,25 @@
       <sortCondition descending="1" ref="D8:D41"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C9:X41">
-    <cfRule type="expression" dxfId="15" priority="8">
-      <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
+  <conditionalFormatting sqref="D9:H41">
+    <cfRule type="expression" dxfId="15" priority="1">
+      <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="9">
-      <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>IF(ISNUMBER(SEARCH("J21", $E9))=TRUE,FALSE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:M41 O9:R41 U9:V41">
-    <cfRule type="expression" dxfId="13" priority="23">
+    <cfRule type="expression" dxfId="10" priority="23">
       <formula>J9=MIN(J$9:J$41)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4808,21 +4639,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:H41">
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
+  <conditionalFormatting sqref="C9:H41">
+    <cfRule type="expression" dxfId="9" priority="8">
+      <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>IF(ISNUMBER(SEARCH("J21", $E9))=TRUE,FALSE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3">
-      <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
-      <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: template updated with new deploys
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fm2871\Documents\DocumentFilter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4147880E-1B4C-4473-A94D-4D1CA9D1F8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3EB21-63AA-4653-833B-E7E1A61B2470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="211">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>REPORTE DIARIO - DELAY BE MD - INSTRUMENTOS BYMA, ALUA, AL30</t>
+  </si>
+  <si>
+    <t>Manolito (algo s/ppt)</t>
   </si>
 </sst>
 </file>
@@ -710,9 +713,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -878,7 +881,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -888,7 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -908,19 +911,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -936,7 +939,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1008,7 +1011,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1330,7 +1333,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="3.44140625" customWidth="1"/>
@@ -1620,7 +1623,7 @@
       </c>
       <c r="E10" s="17" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F10" s="17" t="str">
         <f>+VLOOKUP($B10,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3133,7 +3136,7 @@
       </c>
       <c r="E27" s="17" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>MANOLITO</v>
+        <v>Manolito (algo s/ppt)</v>
       </c>
       <c r="F27" s="17" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -4597,7 +4600,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.77734375" style="5" bestFit="1" customWidth="1"/>
@@ -4626,10 +4629,10 @@
   <dimension ref="B1:P89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.109375" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -4722,7 +4725,7 @@
         <v>113</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="N7" t="s">
         <v>179</v>
@@ -5586,7 +5589,7 @@
         <v>115</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="N31" t="s">
         <v>179</v>
@@ -6781,11 +6784,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K6:P39" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K7:P39">
-      <sortCondition ref="L6:L39"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="K6:P39" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: new template for node deploys from 26.jun
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3EB21-63AA-4653-833B-E7E1A61B2470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DA90D4-174E-4F2D-95C7-4BCE4AFD62D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="32" r:id="rId1"/>
@@ -1329,9 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
   <dimension ref="B2:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2602,7 +2600,7 @@
       </c>
       <c r="E21" s="17" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F21" s="17" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3403,7 +3401,7 @@
       </c>
       <c r="E30" s="17" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F30" s="17" t="str">
         <f>+VLOOKUP($B30,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3492,7 +3490,7 @@
       </c>
       <c r="E31" s="17" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F31" s="17" t="str">
         <f>+VLOOKUP($B31,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -4628,8 +4626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
   <dimension ref="B1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5336,8 +5334,8 @@
       <c r="L24" t="s">
         <v>113</v>
       </c>
-      <c r="M24" t="s">
-        <v>203</v>
+      <c r="M24" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N24" t="s">
         <v>179</v>
@@ -5372,8 +5370,8 @@
       <c r="L25" t="s">
         <v>113</v>
       </c>
-      <c r="M25" t="s">
-        <v>203</v>
+      <c r="M25" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N25" t="s">
         <v>179</v>
@@ -5408,8 +5406,8 @@
       <c r="L26" t="s">
         <v>113</v>
       </c>
-      <c r="M26" t="s">
-        <v>203</v>
+      <c r="M26" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N26" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
feat: template to execute after 30.jun
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DA90D4-174E-4F2D-95C7-4BCE4AFD62D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320E1D62-6543-43D9-81F9-0856A9334FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="212">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>Manolito (algo s/ppt)</t>
+  </si>
+  <si>
+    <t>Java 6 (dma s/ ppt)</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1332,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
   <dimension ref="B2:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2689,7 +2694,7 @@
       </c>
       <c r="E22" s="17" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F22" s="17" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2778,7 +2783,7 @@
       </c>
       <c r="E23" s="17" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F23" s="17" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3579,7 +3584,7 @@
       </c>
       <c r="E32" s="17" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F32" s="17" t="str">
         <f>+VLOOKUP($B32,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3668,7 +3673,7 @@
       </c>
       <c r="E33" s="17" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F33" s="17" t="str">
         <f>+VLOOKUP($B33,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -4382,7 +4387,7 @@
       </c>
       <c r="E41" s="18" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>Java 6 (dma s/ ppt)</v>
       </c>
       <c r="F41" s="18" t="str">
         <f>+VLOOKUP($B41,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -4596,7 +4601,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4626,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB93F688-C610-4B96-A520-A5F303764A6B}">
   <dimension ref="B1:P89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4975,7 +4982,7 @@
         <v>204</v>
       </c>
       <c r="M14" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="N14" t="s">
         <v>179</v>
@@ -5010,8 +5017,8 @@
       <c r="L15" t="s">
         <v>113</v>
       </c>
-      <c r="M15" t="s">
-        <v>203</v>
+      <c r="M15" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N15" t="s">
         <v>179</v>
@@ -5046,8 +5053,8 @@
       <c r="L16" t="s">
         <v>113</v>
       </c>
-      <c r="M16" t="s">
-        <v>203</v>
+      <c r="M16" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N16" t="s">
         <v>179</v>
@@ -5082,8 +5089,8 @@
       <c r="L17" t="s">
         <v>113</v>
       </c>
-      <c r="M17" t="s">
-        <v>203</v>
+      <c r="M17" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N17" t="s">
         <v>179</v>
@@ -5118,8 +5125,8 @@
       <c r="L18" t="s">
         <v>113</v>
       </c>
-      <c r="M18" t="s">
-        <v>203</v>
+      <c r="M18" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="N18" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
feat: update nodes maping
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D846B-EB12-43E3-BE0A-86F485CBCC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A257F97-D429-4A70-8A8E-B96B2A1BFD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,30 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="218">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -183,36 +161,9 @@
     <t>HUB - byypasbue161 - .113 - .113</t>
   </si>
   <si>
-    <t>MBP 667 BTYPASBUE1118 - .133</t>
-  </si>
-  <si>
     <t>EOMM MD BYYPASBUE982 - .74</t>
   </si>
   <si>
-    <t>XSIU - byypasbue354 -.83 - .83</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE551 - .35</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE589 - .237</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE590 - .238</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE573 - .214</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE571 - .212</t>
-  </si>
-  <si>
-    <t>MBO 667 BYYPASBUE561 .202 - .202</t>
-  </si>
-  <si>
-    <t>MBP 667 BYYPASBUE564 .205 - .205</t>
-  </si>
-  <si>
     <t>EOMM MD BYYPASBUE542 .26 - .26</t>
   </si>
   <si>
@@ -237,18 +188,9 @@
     <t>DMA - byypasbue170 - .62 - .62</t>
   </si>
   <si>
-    <t>MitchData - BYYPASBUE550 - .34</t>
-  </si>
-  <si>
-    <t>MitchData - BYYPASBUE572 - .213</t>
-  </si>
-  <si>
     <t>OMS - byypasbue344 -.58 - .58</t>
   </si>
   <si>
-    <t>MBP 667 BYYPASBUE565 .206 - .206</t>
-  </si>
-  <si>
     <t>OR DMA - BYYPASBUE554 .38 - .38</t>
   </si>
   <si>
@@ -258,9 +200,6 @@
     <t>MBO 10 BYYPASBUE580 .221 - .221</t>
   </si>
   <si>
-    <t>MBO 667 BYYPASBUE560 .201 - .201</t>
-  </si>
-  <si>
     <t>EOMM MD BYYPASBUE543 .27 - .27</t>
   </si>
   <si>
@@ -270,9 +209,6 @@
     <t>DMA MBO 20 BYYPASBUE709 - .243</t>
   </si>
   <si>
-    <t>MBP 667 BYTPASBUE819 - .232</t>
-  </si>
-  <si>
     <t>TCR BYYPASBUE858 - .44</t>
   </si>
   <si>
@@ -282,9 +218,6 @@
     <t>ER BYTPASBUE789 - .47</t>
   </si>
   <si>
-    <t>MBP 667 BYYPASBUE1115 - .250</t>
-  </si>
-  <si>
     <t>OR ALGO BYYPASBUE661 - .174</t>
   </si>
   <si>
@@ -294,12 +227,6 @@
     <t>DMA MBO 20 BYYPASBUE711 - .244</t>
   </si>
   <si>
-    <t>MBP 667 BYYPASBUE562 .203 - .203</t>
-  </si>
-  <si>
-    <t>MBP 667 BYYPASBUE563 .204 - .204</t>
-  </si>
-  <si>
     <t>CON DMA BYYPASBUE558 .199 - .199</t>
   </si>
   <si>
@@ -330,9 +257,6 @@
     <t>OR ALGO BYYPASBUE574 .215 - .215</t>
   </si>
   <si>
-    <t>MBO 667 BYYPASBUE559 .200 - .200</t>
-  </si>
-  <si>
     <t>EOMM OR BYYPASBUE539 .22 - .22</t>
   </si>
   <si>
@@ -369,9 +293,6 @@
     <t>EOMM MD BYYPASBUE981 - .73</t>
   </si>
   <si>
-    <t>BETA - byypasbue352 - .81</t>
-  </si>
-  <si>
     <t>OR DMA - BYYPASBUE555 .39 - .39</t>
   </si>
   <si>
@@ -388,18 +309,6 @@
   </si>
   <si>
     <t>EOMM OR BYYPASBUE538 .21 - .21</t>
-  </si>
-  <si>
-    <t>MBP 10 BYYPASBUE1003 .19 - .19</t>
-  </si>
-  <si>
-    <t>MBP 667 BYYPASBUE1114 - .249</t>
-  </si>
-  <si>
-    <t>MBP 667 BYYPASBUE1116 - .134</t>
-  </si>
-  <si>
-    <t>OR ALGO BYYPASBUE1146 - .138</t>
   </si>
   <si>
     <t>DMA</t>
@@ -705,12 +614,6 @@
     <t>REPORTE DIARIO - DELAY BE MD - INSTRUMENTOS BYMA, ALUA, AL30</t>
   </si>
   <si>
-    <t>Manolito (algo s/ppt)</t>
-  </si>
-  <si>
-    <t>Java 6 (dma s/ ppt)</t>
-  </si>
-  <si>
     <t>1387/delay.log</t>
   </si>
   <si>
@@ -736,6 +639,72 @@
   </si>
   <si>
     <t>MBP 10 BYTPASBUE1387 .141 - .141</t>
+  </si>
+  <si>
+    <t>DMA MBP BYTPASBUE1118 - .133</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE354 - .83</t>
+  </si>
+  <si>
+    <t>EOMM M DATA BYYPASBUE551 - .35</t>
+  </si>
+  <si>
+    <t>ALGO M DATA BYYPASBUE589 - .237</t>
+  </si>
+  <si>
+    <t>ALGO M DATA BYYPASBUE590 - .238</t>
+  </si>
+  <si>
+    <t>DMA M DATA BYYPASBUE573 - .214</t>
+  </si>
+  <si>
+    <t>DMA M DATA BYYPASBUE571 - .212</t>
+  </si>
+  <si>
+    <t>DMA MBO BYYPASBUE561 - .202</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE564 - .205</t>
+  </si>
+  <si>
+    <t>EOMM M DATA BYYPASBUE550 - .34</t>
+  </si>
+  <si>
+    <t>DMA M DATA BYYPASBUE572 - .213</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE565 - .206</t>
+  </si>
+  <si>
+    <t>DMA MBO BYYPASBUE560 - .201</t>
+  </si>
+  <si>
+    <t>DMA MBP BYTPASBUE819 - .232</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE1115 - .250</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE562 - .203</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE563 - .204</t>
+  </si>
+  <si>
+    <t>DMA MBO BYYPASBUE559 - .200</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE352 - .81</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE1003 - .19</t>
+  </si>
+  <si>
+    <t>DMA MBP BYYPASBUE1114 - .249</t>
+  </si>
+  <si>
+    <t>DMA MBP BYTPASBUE1116 - .134</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1339,7 @@
   <dimension ref="B2:X46"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,7 +1367,7 @@
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="X2" s="8"/>
     </row>
@@ -1417,7 +1386,7 @@
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="X5" s="9"/>
     </row>
@@ -1491,73 +1460,73 @@
     </row>
     <row r="8" spans="2:24" s="10" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="K8" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="L8" s="22" t="s">
-        <v>208</v>
-      </c>
       <c r="M8" s="22" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="P8" s="22" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="S8" s="22" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="T8" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="22" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="V8" s="22" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="W8" s="20" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -2363,7 +2332,7 @@
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="C18" s="24">
         <v>1362</v>
@@ -2452,7 +2421,7 @@
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="C19" s="24">
         <v>1372</v>
@@ -2541,7 +2510,7 @@
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C20" s="24">
         <v>1373</v>
@@ -2630,10 +2599,10 @@
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C21" s="24">
-        <v>819</v>
+        <v>559</v>
       </c>
       <c r="D21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -2641,7 +2610,7 @@
       </c>
       <c r="E21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>MANOLITO</v>
+        <v>Java 6</v>
       </c>
       <c r="F21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2653,7 +2622,7 @@
       </c>
       <c r="H21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>DEDICADO</v>
+        <v>MBO</v>
       </c>
       <c r="I21" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B21,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B21,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -2719,10 +2688,10 @@
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C22" s="24">
-        <v>1115</v>
+        <v>560</v>
       </c>
       <c r="D22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -2730,7 +2699,7 @@
       </c>
       <c r="E22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>MANOLITO</v>
+        <v>Java 6</v>
       </c>
       <c r="F22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2742,7 +2711,7 @@
       </c>
       <c r="H22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>DEDICADO</v>
+        <v>MBO</v>
       </c>
       <c r="I22" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B22,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B22,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -2808,10 +2777,10 @@
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C23" s="24">
-        <v>1116</v>
+        <v>561</v>
       </c>
       <c r="D23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -2819,7 +2788,7 @@
       </c>
       <c r="E23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>MANOLITO</v>
+        <v>Java 6</v>
       </c>
       <c r="F23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2831,7 +2800,7 @@
       </c>
       <c r="H23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>DEDICADO</v>
+        <v>MBO</v>
       </c>
       <c r="I23" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B23,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B23,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -2897,10 +2866,10 @@
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C24" s="24">
-        <v>559</v>
+        <v>819</v>
       </c>
       <c r="D24" s="14" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -2908,7 +2877,7 @@
       </c>
       <c r="E24" s="14" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F24" s="14" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2920,7 +2889,7 @@
       </c>
       <c r="H24" s="14" t="str">
         <f>+VLOOKUP($B24,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBO</v>
+        <v>DEDICADO</v>
       </c>
       <c r="I24" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B24,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B24,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -2986,10 +2955,10 @@
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C25" s="24">
-        <v>560</v>
+        <v>1115</v>
       </c>
       <c r="D25" s="14" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -2997,7 +2966,7 @@
       </c>
       <c r="E25" s="14" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F25" s="14" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3009,7 +2978,7 @@
       </c>
       <c r="H25" s="14" t="str">
         <f>+VLOOKUP($B25,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBO</v>
+        <v>DEDICADO</v>
       </c>
       <c r="I25" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B25,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B25,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -3075,10 +3044,10 @@
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C26" s="24">
-        <v>561</v>
+        <v>1116</v>
       </c>
       <c r="D26" s="14" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -3086,7 +3055,7 @@
       </c>
       <c r="E26" s="14" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F26" s="14" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3098,7 +3067,7 @@
       </c>
       <c r="H26" s="14" t="str">
         <f>+VLOOKUP($B26,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBO</v>
+        <v>DEDICADO</v>
       </c>
       <c r="I26" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B26,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B26,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -3175,7 +3144,7 @@
       </c>
       <c r="E27" s="14" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Manolito (algo s/ppt)</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F27" s="14" t="str">
         <f>+VLOOKUP($B27,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3873,7 +3842,7 @@
         <v>n/a</v>
       </c>
       <c r="X34" s="25" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.3">
@@ -4145,7 +4114,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="C38" s="24">
         <v>1389</v>
@@ -4234,7 +4203,7 @@
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="C39" s="24">
         <v>1390</v>
@@ -4590,7 +4559,7 @@
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="C43" s="24">
         <v>1387</v>
@@ -4679,7 +4648,7 @@
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="C44" s="24">
         <v>1388</v>
@@ -4779,7 +4748,7 @@
       </c>
       <c r="E45" s="14" t="str">
         <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6 (dma s/ ppt)</v>
+        <v>Java 6</v>
       </c>
       <c r="F45" s="14" t="str">
         <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -4854,7 +4823,7 @@
         <v>n/a</v>
       </c>
       <c r="X45" s="25" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.3">
@@ -4910,11 +4879,6 @@
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="5">
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:M45 O9:R45 U9:V45">
-    <cfRule type="expression" dxfId="0" priority="23">
-      <formula>J9=MIN(J$9:J$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K45">
@@ -4987,6 +4951,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J9:M45 O9:R45 U9:V45">
+    <cfRule type="expression" dxfId="0" priority="48">
+      <formula>J9=MIN(J$9:J$45)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5069,41 +5038,41 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="6" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -5119,19 +5088,19 @@
         <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="N7" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O7" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P7" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -5141,10 +5110,9 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G8" cm="1">
-        <f t="array" aca="1" ref="G8" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F8,ROW(INDIRECT("1"&amp;":"&amp;LEN(F8))),1)*1),MID(F8,ROW(INDIRECT("1"&amp;":"&amp;LEN(F8))),1),"")))</f>
+        <v>95</v>
+      </c>
+      <c r="G8">
         <v>197</v>
       </c>
       <c r="H8" t="e">
@@ -5155,19 +5123,19 @@
         <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N8" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O8" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
@@ -5177,10 +5145,9 @@
         <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" cm="1">
-        <f t="array" aca="1" ref="G9" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F9,ROW(INDIRECT("1"&amp;":"&amp;LEN(F9))),1)*1),MID(F9,ROW(INDIRECT("1"&amp;":"&amp;LEN(F9))),1),"")))</f>
+        <v>96</v>
+      </c>
+      <c r="G9">
         <v>196</v>
       </c>
       <c r="H9" t="e">
@@ -5191,19 +5158,19 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N9" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O9" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P9" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
@@ -5213,10 +5180,9 @@
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" cm="1">
-        <f t="array" aca="1" ref="G10" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F10,ROW(INDIRECT("1"&amp;":"&amp;LEN(F10))),1)*1),MID(F10,ROW(INDIRECT("1"&amp;":"&amp;LEN(F10))),1),"")))</f>
+        <v>97</v>
+      </c>
+      <c r="G10">
         <v>129</v>
       </c>
       <c r="H10" t="e">
@@ -5227,19 +5193,19 @@
         <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N10" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O10" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P10" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
@@ -5249,10 +5215,9 @@
         <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" cm="1">
-        <f t="array" aca="1" ref="G11" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F11,ROW(INDIRECT("1"&amp;":"&amp;LEN(F11))),1)*1),MID(F11,ROW(INDIRECT("1"&amp;":"&amp;LEN(F11))),1),"")))</f>
+        <v>98</v>
+      </c>
+      <c r="G11">
         <v>128</v>
       </c>
       <c r="H11" t="e">
@@ -5263,19 +5228,19 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N11" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P11" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
@@ -5285,10 +5250,9 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" cm="1">
-        <f t="array" aca="1" ref="G12" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F12,ROW(INDIRECT("1"&amp;":"&amp;LEN(F12))),1)*1),MID(F12,ROW(INDIRECT("1"&amp;":"&amp;LEN(F12))),1),"")))</f>
+        <v>99</v>
+      </c>
+      <c r="G12">
         <v>194</v>
       </c>
       <c r="H12" t="e">
@@ -5299,19 +5263,19 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N12" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P12" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
@@ -5321,10 +5285,9 @@
         <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" cm="1">
-        <f t="array" aca="1" ref="G13" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F13,ROW(INDIRECT("1"&amp;":"&amp;LEN(F13))),1)*1),MID(F13,ROW(INDIRECT("1"&amp;":"&amp;LEN(F13))),1),"")))</f>
+        <v>100</v>
+      </c>
+      <c r="G13">
         <v>161</v>
       </c>
       <c r="H13" t="e">
@@ -5335,32 +5298,31 @@
         <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N13" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O13" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P13" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" cm="1">
-        <f t="array" aca="1" ref="G14" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F14,ROW(INDIRECT("1"&amp;":"&amp;LEN(F14))),1)*1),MID(F14,ROW(INDIRECT("1"&amp;":"&amp;LEN(F14))),1),"")))</f>
+      <c r="G14">
         <v>1118</v>
       </c>
       <c r="H14" t="e">
@@ -5371,32 +5333,31 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M14" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="N14" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P14" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="G15" cm="1">
-        <f t="array" aca="1" ref="G15" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F15,ROW(INDIRECT("1"&amp;":"&amp;LEN(F15))),1)*1),MID(F15,ROW(INDIRECT("1"&amp;":"&amp;LEN(F15))),1),"")))</f>
+      <c r="G15">
         <v>982</v>
       </c>
       <c r="H15" t="e">
@@ -5407,32 +5368,31 @@
         <v>2</v>
       </c>
       <c r="L15" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N15" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O15" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P15" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" cm="1">
-        <f t="array" aca="1" ref="G16" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F16,ROW(INDIRECT("1"&amp;":"&amp;LEN(F16))),1)*1),MID(F16,ROW(INDIRECT("1"&amp;":"&amp;LEN(F16))),1),"")))</f>
+      <c r="G16">
         <v>354</v>
       </c>
       <c r="H16" t="e">
@@ -5443,32 +5403,31 @@
         <v>3</v>
       </c>
       <c r="L16" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N16" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O16" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P16" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>198</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" cm="1">
-        <f t="array" aca="1" ref="G17" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F17,ROW(INDIRECT("1"&amp;":"&amp;LEN(F17))),1)*1),MID(F17,ROW(INDIRECT("1"&amp;":"&amp;LEN(F17))),1),"")))</f>
+        <v>101</v>
+      </c>
+      <c r="G17">
         <v>551</v>
       </c>
       <c r="H17" t="e">
@@ -5479,32 +5438,31 @@
         <v>4</v>
       </c>
       <c r="L17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N17" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O17" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P17" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" cm="1">
-        <f t="array" aca="1" ref="G18" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F18,ROW(INDIRECT("1"&amp;":"&amp;LEN(F18))),1)*1),MID(F18,ROW(INDIRECT("1"&amp;":"&amp;LEN(F18))),1),"")))</f>
+        <v>102</v>
+      </c>
+      <c r="G18">
         <v>589</v>
       </c>
       <c r="H18" t="e">
@@ -5515,32 +5473,31 @@
         <v>5</v>
       </c>
       <c r="L18" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N18" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O18" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P18" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" cm="1">
-        <f t="array" aca="1" ref="G19" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F19,ROW(INDIRECT("1"&amp;":"&amp;LEN(F19))),1)*1),MID(F19,ROW(INDIRECT("1"&amp;":"&amp;LEN(F19))),1),"")))</f>
+        <v>103</v>
+      </c>
+      <c r="G19">
         <v>590</v>
       </c>
       <c r="H19" t="e">
@@ -5551,32 +5508,31 @@
         <v>15</v>
       </c>
       <c r="L19" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M19" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="N19" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O19" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P19" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" cm="1">
-        <f t="array" aca="1" ref="G20" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F20,ROW(INDIRECT("1"&amp;":"&amp;LEN(F20))),1)*1),MID(F20,ROW(INDIRECT("1"&amp;":"&amp;LEN(F20))),1),"")))</f>
+        <v>104</v>
+      </c>
+      <c r="G20">
         <v>573</v>
       </c>
       <c r="H20" t="e">
@@ -5587,32 +5543,31 @@
         <v>16</v>
       </c>
       <c r="L20" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M20" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="N20" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O20" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P20" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" cm="1">
-        <f t="array" aca="1" ref="G21" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F21,ROW(INDIRECT("1"&amp;":"&amp;LEN(F21))),1)*1),MID(F21,ROW(INDIRECT("1"&amp;":"&amp;LEN(F21))),1),"")))</f>
+        <v>105</v>
+      </c>
+      <c r="G21">
         <v>571</v>
       </c>
       <c r="H21" t="e">
@@ -5623,32 +5578,31 @@
         <v>17</v>
       </c>
       <c r="L21" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M21" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="N21" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O21" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P21" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
       </c>
-      <c r="G22" cm="1">
-        <f t="array" aca="1" ref="G22" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F22,ROW(INDIRECT("1"&amp;":"&amp;LEN(F22))),1)*1),MID(F22,ROW(INDIRECT("1"&amp;":"&amp;LEN(F22))),1),"")))</f>
+      <c r="G22">
         <v>561</v>
       </c>
       <c r="H22" t="e">
@@ -5659,32 +5613,31 @@
         <v>18</v>
       </c>
       <c r="L22" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N22" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O22" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P22" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>204</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
-      <c r="G23" cm="1">
-        <f t="array" aca="1" ref="G23" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F23,ROW(INDIRECT("1"&amp;":"&amp;LEN(F23))),1)*1),MID(F23,ROW(INDIRECT("1"&amp;":"&amp;LEN(F23))),1),"")))</f>
+      <c r="G23">
         <v>564</v>
       </c>
       <c r="H23" t="e">
@@ -5695,32 +5648,31 @@
         <v>19</v>
       </c>
       <c r="L23" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N23" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O23" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P23" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
       </c>
-      <c r="G24" cm="1">
-        <f t="array" aca="1" ref="G24" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F24,ROW(INDIRECT("1"&amp;":"&amp;LEN(F24))),1)*1),MID(F24,ROW(INDIRECT("1"&amp;":"&amp;LEN(F24))),1),"")))</f>
+      <c r="G24">
         <v>542</v>
       </c>
       <c r="H24" t="e">
@@ -5731,32 +5683,31 @@
         <v>20</v>
       </c>
       <c r="L24" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N24" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O24" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P24" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" cm="1">
-        <f t="array" aca="1" ref="G25" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F25,ROW(INDIRECT("1"&amp;":"&amp;LEN(F25))),1)*1),MID(F25,ROW(INDIRECT("1"&amp;":"&amp;LEN(F25))),1),"")))</f>
+        <v>106</v>
+      </c>
+      <c r="G25">
         <v>537</v>
       </c>
       <c r="H25" t="e">
@@ -5767,32 +5718,31 @@
         <v>21</v>
       </c>
       <c r="L25" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N25" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O25" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P25" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" cm="1">
-        <f t="array" aca="1" ref="G26" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F26,ROW(INDIRECT("1"&amp;":"&amp;LEN(F26))),1)*1),MID(F26,ROW(INDIRECT("1"&amp;":"&amp;LEN(F26))),1),"")))</f>
+        <v>107</v>
+      </c>
+      <c r="G26">
         <v>540</v>
       </c>
       <c r="H26" t="e">
@@ -5803,32 +5753,31 @@
         <v>28</v>
       </c>
       <c r="L26" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N26" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O26" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P26" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
-      </c>
-      <c r="G27" cm="1">
-        <f t="array" aca="1" ref="G27" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F27,ROW(INDIRECT("1"&amp;":"&amp;LEN(F27))),1)*1),MID(F27,ROW(INDIRECT("1"&amp;":"&amp;LEN(F27))),1),"")))</f>
+        <v>108</v>
+      </c>
+      <c r="G27">
         <v>653</v>
       </c>
       <c r="H27" t="e">
@@ -5839,32 +5788,31 @@
         <v>9</v>
       </c>
       <c r="L27" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="M27" s="18" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="N27" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O27" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P27" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>132</v>
-      </c>
-      <c r="G28" cm="1">
-        <f t="array" aca="1" ref="G28" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F28,ROW(INDIRECT("1"&amp;":"&amp;LEN(F28))),1)*1),MID(F28,ROW(INDIRECT("1"&amp;":"&amp;LEN(F28))),1),"")))</f>
+        <v>109</v>
+      </c>
+      <c r="G28">
         <v>834</v>
       </c>
       <c r="H28" t="e">
@@ -5875,32 +5823,31 @@
         <v>6</v>
       </c>
       <c r="L28" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N28" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O28" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P28" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" cm="1">
-        <f t="array" aca="1" ref="G29" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F29,ROW(INDIRECT("1"&amp;":"&amp;LEN(F29))),1)*1),MID(F29,ROW(INDIRECT("1"&amp;":"&amp;LEN(F29))),1),"")))</f>
+        <v>110</v>
+      </c>
+      <c r="G29">
         <v>712</v>
       </c>
       <c r="H29" t="e">
@@ -5911,32 +5858,31 @@
         <v>7</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N29" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O29" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P29" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G30" cm="1">
-        <f t="array" aca="1" ref="G30" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F30,ROW(INDIRECT("1"&amp;":"&amp;LEN(F30))),1)*1),MID(F30,ROW(INDIRECT("1"&amp;":"&amp;LEN(F30))),1),"")))</f>
+        <v>99</v>
+      </c>
+      <c r="G30">
         <v>194</v>
       </c>
       <c r="H30" t="e">
@@ -5947,32 +5893,31 @@
         <v>8</v>
       </c>
       <c r="L30" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N30" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O30" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P30" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" cm="1">
-        <f t="array" aca="1" ref="G31" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F31,ROW(INDIRECT("1"&amp;":"&amp;LEN(F31))),1)*1),MID(F31,ROW(INDIRECT("1"&amp;":"&amp;LEN(F31))),1),"")))</f>
+        <v>111</v>
+      </c>
+      <c r="G31">
         <v>170</v>
       </c>
       <c r="H31" t="e">
@@ -5983,32 +5928,31 @@
         <v>12</v>
       </c>
       <c r="L31" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N31" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O31" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P31" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>205</v>
       </c>
       <c r="F32" t="s">
-        <v>135</v>
-      </c>
-      <c r="G32" cm="1">
-        <f t="array" aca="1" ref="G32" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F32,ROW(INDIRECT("1"&amp;":"&amp;LEN(F32))),1)*1),MID(F32,ROW(INDIRECT("1"&amp;":"&amp;LEN(F32))),1),"")))</f>
+        <v>112</v>
+      </c>
+      <c r="G32">
         <v>550</v>
       </c>
       <c r="H32" t="e">
@@ -6019,32 +5963,31 @@
         <v>30</v>
       </c>
       <c r="L32" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N32" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O32" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P32" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>206</v>
       </c>
       <c r="F33" t="s">
-        <v>136</v>
-      </c>
-      <c r="G33" cm="1">
-        <f t="array" aca="1" ref="G33" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F33,ROW(INDIRECT("1"&amp;":"&amp;LEN(F33))),1)*1),MID(F33,ROW(INDIRECT("1"&amp;":"&amp;LEN(F33))),1),"")))</f>
+        <v>113</v>
+      </c>
+      <c r="G33">
         <v>572</v>
       </c>
       <c r="H33" t="e">
@@ -6052,35 +5995,34 @@
         <v>#N/A</v>
       </c>
       <c r="K33" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N33" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O33" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P33" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="E34" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
-      </c>
-      <c r="G34" cm="1">
-        <f t="array" aca="1" ref="G34" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F34,ROW(INDIRECT("1"&amp;":"&amp;LEN(F34))),1)*1),MID(F34,ROW(INDIRECT("1"&amp;":"&amp;LEN(F34))),1),"")))</f>
+        <v>114</v>
+      </c>
+      <c r="G34">
         <v>344</v>
       </c>
       <c r="H34" t="e">
@@ -6088,35 +6030,34 @@
         <v>#N/A</v>
       </c>
       <c r="K34" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N34" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O34" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P34" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>207</v>
       </c>
       <c r="F35" t="s">
         <v>21</v>
       </c>
-      <c r="G35" cm="1">
-        <f t="array" aca="1" ref="G35" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F35,ROW(INDIRECT("1"&amp;":"&amp;LEN(F35))),1)*1),MID(F35,ROW(INDIRECT("1"&amp;":"&amp;LEN(F35))),1),"")))</f>
+      <c r="G35">
         <v>565</v>
       </c>
       <c r="H35" t="e">
@@ -6124,35 +6065,34 @@
         <v>#N/A</v>
       </c>
       <c r="K35" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="L35" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N35" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O35" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P35" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F36" t="s">
-        <v>138</v>
-      </c>
-      <c r="G36" cm="1">
-        <f t="array" aca="1" ref="G36" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F36,ROW(INDIRECT("1"&amp;":"&amp;LEN(F36))),1)*1),MID(F36,ROW(INDIRECT("1"&amp;":"&amp;LEN(F36))),1),"")))</f>
+        <v>115</v>
+      </c>
+      <c r="G36">
         <v>554</v>
       </c>
       <c r="H36" t="e">
@@ -6163,32 +6103,31 @@
         <v>11</v>
       </c>
       <c r="L36" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N36" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O36" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P36" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="E37" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
-        <v>139</v>
-      </c>
-      <c r="G37" cm="1">
-        <f t="array" aca="1" ref="G37" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F37,ROW(INDIRECT("1"&amp;":"&amp;LEN(F37))),1)*1),MID(F37,ROW(INDIRECT("1"&amp;":"&amp;LEN(F37))),1),"")))</f>
+        <v>116</v>
+      </c>
+      <c r="G37">
         <v>556</v>
       </c>
       <c r="H37" t="e">
@@ -6199,32 +6138,31 @@
         <v>13</v>
       </c>
       <c r="L37" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N37" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O37" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P37" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F38" t="s">
         <v>24</v>
       </c>
-      <c r="G38" cm="1">
-        <f t="array" aca="1" ref="G38" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F38,ROW(INDIRECT("1"&amp;":"&amp;LEN(F38))),1)*1),MID(F38,ROW(INDIRECT("1"&amp;":"&amp;LEN(F38))),1),"")))</f>
+      <c r="G38">
         <v>580</v>
       </c>
       <c r="H38" t="e">
@@ -6235,32 +6173,31 @@
         <v>14</v>
       </c>
       <c r="L38" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N38" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O38" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P38" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>208</v>
       </c>
       <c r="F39" t="s">
         <v>16</v>
       </c>
-      <c r="G39" cm="1">
-        <f t="array" aca="1" ref="G39" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F39,ROW(INDIRECT("1"&amp;":"&amp;LEN(F39))),1)*1),MID(F39,ROW(INDIRECT("1"&amp;":"&amp;LEN(F39))),1),"")))</f>
+      <c r="G39">
         <v>560</v>
       </c>
       <c r="H39" t="e">
@@ -6271,32 +6208,31 @@
         <v>29</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="M39" s="18" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N39" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O39" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P39" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
-      <c r="G40" cm="1">
-        <f t="array" aca="1" ref="G40" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F40,ROW(INDIRECT("1"&amp;":"&amp;LEN(F40))),1)*1),MID(F40,ROW(INDIRECT("1"&amp;":"&amp;LEN(F40))),1),"")))</f>
+      <c r="G40">
         <v>543</v>
       </c>
       <c r="H40" t="e">
@@ -6304,35 +6240,34 @@
         <v>#N/A</v>
       </c>
       <c r="K40" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="L40" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M40" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N40" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O40" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P40" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>140</v>
-      </c>
-      <c r="G41" cm="1">
-        <f t="array" aca="1" ref="G41" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F41,ROW(INDIRECT("1"&amp;":"&amp;LEN(F41))),1)*1),MID(F41,ROW(INDIRECT("1"&amp;":"&amp;LEN(F41))),1),"")))</f>
+        <v>117</v>
+      </c>
+      <c r="G41">
         <v>790</v>
       </c>
       <c r="H41" t="e">
@@ -6340,35 +6275,34 @@
         <v>#N/A</v>
       </c>
       <c r="K41" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="L41" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M41" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N41" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O41" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P41" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="E42" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
-      </c>
-      <c r="G42" cm="1">
-        <f t="array" aca="1" ref="G42" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F42,ROW(INDIRECT("1"&amp;":"&amp;LEN(F42))),1)*1),MID(F42,ROW(INDIRECT("1"&amp;":"&amp;LEN(F42))),1),"")))</f>
+        <v>118</v>
+      </c>
+      <c r="G42">
         <v>709</v>
       </c>
       <c r="H42" t="e">
@@ -6376,35 +6310,34 @@
         <v>#N/A</v>
       </c>
       <c r="K42" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="L42" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M42" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N42" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O42" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P42" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="E43" t="s">
-        <v>69</v>
+        <v>209</v>
       </c>
       <c r="F43" t="s">
         <v>28</v>
       </c>
-      <c r="G43" cm="1">
-        <f t="array" aca="1" ref="G43" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F43,ROW(INDIRECT("1"&amp;":"&amp;LEN(F43))),1)*1),MID(F43,ROW(INDIRECT("1"&amp;":"&amp;LEN(F43))),1),"")))</f>
+      <c r="G43">
         <v>819</v>
       </c>
       <c r="H43" t="e">
@@ -6412,35 +6345,34 @@
         <v>#N/A</v>
       </c>
       <c r="K43" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="L43" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M43" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="N43" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="O43" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="P43" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
-        <v>142</v>
-      </c>
-      <c r="G44" cm="1">
-        <f t="array" aca="1" ref="G44" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F44,ROW(INDIRECT("1"&amp;":"&amp;LEN(F44))),1)*1),MID(F44,ROW(INDIRECT("1"&amp;":"&amp;LEN(F44))),1),"")))</f>
+        <v>119</v>
+      </c>
+      <c r="G44">
         <v>858</v>
       </c>
       <c r="H44" t="e">
@@ -6452,13 +6384,12 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" cm="1">
-        <f t="array" aca="1" ref="G45" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F45,ROW(INDIRECT("1"&amp;":"&amp;LEN(F45))),1)*1),MID(F45,ROW(INDIRECT("1"&amp;":"&amp;LEN(F45))),1),"")))</f>
+        <v>120</v>
+      </c>
+      <c r="G45">
         <v>862</v>
       </c>
       <c r="H45" t="e">
@@ -6470,13 +6401,12 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="E46" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F46" t="s">
-        <v>144</v>
-      </c>
-      <c r="G46" cm="1">
-        <f t="array" aca="1" ref="G46" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F46,ROW(INDIRECT("1"&amp;":"&amp;LEN(F46))),1)*1),MID(F46,ROW(INDIRECT("1"&amp;":"&amp;LEN(F46))),1),"")))</f>
+        <v>121</v>
+      </c>
+      <c r="G46">
         <v>789</v>
       </c>
       <c r="H46" t="e">
@@ -6488,13 +6418,12 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>210</v>
       </c>
       <c r="F47" t="s">
         <v>3</v>
       </c>
-      <c r="G47" cm="1">
-        <f t="array" aca="1" ref="G47" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F47,ROW(INDIRECT("1"&amp;":"&amp;LEN(F47))),1)*1),MID(F47,ROW(INDIRECT("1"&amp;":"&amp;LEN(F47))),1),"")))</f>
+      <c r="G47">
         <v>1115</v>
       </c>
       <c r="H47" t="e">
@@ -6506,13 +6435,12 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F48" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" cm="1">
-        <f t="array" aca="1" ref="G48" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F48,ROW(INDIRECT("1"&amp;":"&amp;LEN(F48))),1)*1),MID(F48,ROW(INDIRECT("1"&amp;":"&amp;LEN(F48))),1),"")))</f>
+        <v>122</v>
+      </c>
+      <c r="G48">
         <v>661</v>
       </c>
       <c r="H48" t="e">
@@ -6524,13 +6452,12 @@
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F49" t="s">
-        <v>146</v>
-      </c>
-      <c r="G49" cm="1">
-        <f t="array" aca="1" ref="G49" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F49,ROW(INDIRECT("1"&amp;":"&amp;LEN(F49))),1)*1),MID(F49,ROW(INDIRECT("1"&amp;":"&amp;LEN(F49))),1),"")))</f>
+        <v>123</v>
+      </c>
+      <c r="G49">
         <v>1145</v>
       </c>
       <c r="H49" t="e">
@@ -6542,13 +6469,12 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="E50" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>147</v>
-      </c>
-      <c r="G50" cm="1">
-        <f t="array" aca="1" ref="G50" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F50,ROW(INDIRECT("1"&amp;":"&amp;LEN(F50))),1)*1),MID(F50,ROW(INDIRECT("1"&amp;":"&amp;LEN(F50))),1),"")))</f>
+        <v>124</v>
+      </c>
+      <c r="G50">
         <v>711</v>
       </c>
       <c r="H50" t="e">
@@ -6560,13 +6486,12 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="E51" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
       <c r="F51" t="s">
         <v>18</v>
       </c>
-      <c r="G51" cm="1">
-        <f t="array" aca="1" ref="G51" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F51,ROW(INDIRECT("1"&amp;":"&amp;LEN(F51))),1)*1),MID(F51,ROW(INDIRECT("1"&amp;":"&amp;LEN(F51))),1),"")))</f>
+      <c r="G51">
         <v>562</v>
       </c>
       <c r="H51" t="e">
@@ -6578,13 +6503,12 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="E52" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
       </c>
-      <c r="G52" cm="1">
-        <f t="array" aca="1" ref="G52" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F52,ROW(INDIRECT("1"&amp;":"&amp;LEN(F52))),1)*1),MID(F52,ROW(INDIRECT("1"&amp;":"&amp;LEN(F52))),1),"")))</f>
+      <c r="G52">
         <v>563</v>
       </c>
       <c r="H52" t="e">
@@ -6596,13 +6520,12 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F53" t="s">
-        <v>148</v>
-      </c>
-      <c r="G53" cm="1">
-        <f t="array" aca="1" ref="G53" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F53,ROW(INDIRECT("1"&amp;":"&amp;LEN(F53))),1)*1),MID(F53,ROW(INDIRECT("1"&amp;":"&amp;LEN(F53))),1),"")))</f>
+        <v>125</v>
+      </c>
+      <c r="G53">
         <v>558</v>
       </c>
       <c r="H53" t="e">
@@ -6614,13 +6537,12 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="F54" t="s">
-        <v>149</v>
-      </c>
-      <c r="G54" cm="1">
-        <f t="array" aca="1" ref="G54" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F54,ROW(INDIRECT("1"&amp;":"&amp;LEN(F54))),1)*1),MID(F54,ROW(INDIRECT("1"&amp;":"&amp;LEN(F54))),1),"")))</f>
+        <v>126</v>
+      </c>
+      <c r="G54">
         <v>552</v>
       </c>
       <c r="H54" t="e">
@@ -6632,13 +6554,12 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F55" t="s">
         <v>27</v>
       </c>
-      <c r="G55" cm="1">
-        <f t="array" aca="1" ref="G55" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F55,ROW(INDIRECT("1"&amp;":"&amp;LEN(F55))),1)*1),MID(F55,ROW(INDIRECT("1"&amp;":"&amp;LEN(F55))),1),"")))</f>
+      <c r="G55">
         <v>583</v>
       </c>
       <c r="H55" t="e">
@@ -6650,13 +6571,12 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F56" t="s">
-        <v>150</v>
-      </c>
-      <c r="G56" cm="1">
-        <f t="array" aca="1" ref="G56" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F56,ROW(INDIRECT("1"&amp;":"&amp;LEN(F56))),1)*1),MID(F56,ROW(INDIRECT("1"&amp;":"&amp;LEN(F56))),1),"")))</f>
+        <v>127</v>
+      </c>
+      <c r="G56">
         <v>576</v>
       </c>
       <c r="H56" t="e">
@@ -6668,13 +6588,12 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="E57" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F57" t="s">
         <v>26</v>
       </c>
-      <c r="G57" cm="1">
-        <f t="array" aca="1" ref="G57" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F57,ROW(INDIRECT("1"&amp;":"&amp;LEN(F57))),1)*1),MID(F57,ROW(INDIRECT("1"&amp;":"&amp;LEN(F57))),1),"")))</f>
+      <c r="G57">
         <v>582</v>
       </c>
       <c r="H57" t="e">
@@ -6686,13 +6605,12 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="E58" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F58" t="s">
-        <v>151</v>
-      </c>
-      <c r="G58" cm="1">
-        <f t="array" aca="1" ref="G58" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F58,ROW(INDIRECT("1"&amp;":"&amp;LEN(F58))),1)*1),MID(F58,ROW(INDIRECT("1"&amp;":"&amp;LEN(F58))),1),"")))</f>
+        <v>128</v>
+      </c>
+      <c r="G58">
         <v>557</v>
       </c>
       <c r="H58" t="e">
@@ -6704,13 +6622,12 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="E59" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F59" t="s">
         <v>23</v>
       </c>
-      <c r="G59" cm="1">
-        <f t="array" aca="1" ref="G59" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F59,ROW(INDIRECT("1"&amp;":"&amp;LEN(F59))),1)*1),MID(F59,ROW(INDIRECT("1"&amp;":"&amp;LEN(F59))),1),"")))</f>
+      <c r="G59">
         <v>579</v>
       </c>
       <c r="H59" t="e">
@@ -6722,13 +6639,12 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
       </c>
-      <c r="G60" cm="1">
-        <f t="array" aca="1" ref="G60" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F60,ROW(INDIRECT("1"&amp;":"&amp;LEN(F60))),1)*1),MID(F60,ROW(INDIRECT("1"&amp;":"&amp;LEN(F60))),1),"")))</f>
+      <c r="G60">
         <v>578</v>
       </c>
       <c r="H60" t="e">
@@ -6740,13 +6656,12 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F61" t="s">
-        <v>152</v>
-      </c>
-      <c r="G61" cm="1">
-        <f t="array" aca="1" ref="G61" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F61,ROW(INDIRECT("1"&amp;":"&amp;LEN(F61))),1)*1),MID(F61,ROW(INDIRECT("1"&amp;":"&amp;LEN(F61))),1),"")))</f>
+        <v>129</v>
+      </c>
+      <c r="G61">
         <v>575</v>
       </c>
       <c r="H61" t="e">
@@ -6758,13 +6673,12 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="E62" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="F62" t="s">
-        <v>153</v>
-      </c>
-      <c r="G62" cm="1">
-        <f t="array" aca="1" ref="G62" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F62,ROW(INDIRECT("1"&amp;":"&amp;LEN(F62))),1)*1),MID(F62,ROW(INDIRECT("1"&amp;":"&amp;LEN(F62))),1),"")))</f>
+        <v>130</v>
+      </c>
+      <c r="G62">
         <v>574</v>
       </c>
       <c r="H62" t="e">
@@ -6776,13 +6690,12 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="E63" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
       <c r="F63" t="s">
         <v>15</v>
       </c>
-      <c r="G63" cm="1">
-        <f t="array" aca="1" ref="G63" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F63,ROW(INDIRECT("1"&amp;":"&amp;LEN(F63))),1)*1),MID(F63,ROW(INDIRECT("1"&amp;":"&amp;LEN(F63))),1),"")))</f>
+      <c r="G63">
         <v>559</v>
       </c>
       <c r="H63" t="e">
@@ -6794,13 +6707,12 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="E64" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="F64" t="s">
-        <v>154</v>
-      </c>
-      <c r="G64" cm="1">
-        <f t="array" aca="1" ref="G64" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F64,ROW(INDIRECT("1"&amp;":"&amp;LEN(F64))),1)*1),MID(F64,ROW(INDIRECT("1"&amp;":"&amp;LEN(F64))),1),"")))</f>
+        <v>131</v>
+      </c>
+      <c r="G64">
         <v>539</v>
       </c>
       <c r="H64" t="e">
@@ -6812,13 +6724,12 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="E65" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
       </c>
-      <c r="G65" cm="1">
-        <f t="array" aca="1" ref="G65" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F65,ROW(INDIRECT("1"&amp;":"&amp;LEN(F65))),1)*1),MID(F65,ROW(INDIRECT("1"&amp;":"&amp;LEN(F65))),1),"")))</f>
+      <c r="G65">
         <v>544</v>
       </c>
       <c r="H65" t="e">
@@ -6830,13 +6741,12 @@
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="E66" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
-      <c r="G66" cm="1">
-        <f t="array" aca="1" ref="G66" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F66,ROW(INDIRECT("1"&amp;":"&amp;LEN(F66))),1)*1),MID(F66,ROW(INDIRECT("1"&amp;":"&amp;LEN(F66))),1),"")))</f>
+      <c r="G66">
         <v>541</v>
       </c>
       <c r="H66" t="e">
@@ -6848,13 +6758,12 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="E67" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="F67" t="s">
-        <v>155</v>
-      </c>
-      <c r="G67" cm="1">
-        <f t="array" aca="1" ref="G67" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F67,ROW(INDIRECT("1"&amp;":"&amp;LEN(F67))),1)*1),MID(F67,ROW(INDIRECT("1"&amp;":"&amp;LEN(F67))),1),"")))</f>
+        <v>132</v>
+      </c>
+      <c r="G67">
         <v>652</v>
       </c>
       <c r="H67" t="e">
@@ -6866,13 +6775,12 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="E68" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F68" t="s">
-        <v>156</v>
-      </c>
-      <c r="G68" cm="1">
-        <f t="array" aca="1" ref="G68" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F68,ROW(INDIRECT("1"&amp;":"&amp;LEN(F68))),1)*1),MID(F68,ROW(INDIRECT("1"&amp;":"&amp;LEN(F68))),1),"")))</f>
+        <v>133</v>
+      </c>
+      <c r="G68">
         <v>713</v>
       </c>
       <c r="H68" t="e">
@@ -6884,13 +6792,12 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="E69" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="F69" t="s">
-        <v>157</v>
-      </c>
-      <c r="G69" cm="1">
-        <f t="array" aca="1" ref="G69" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F69,ROW(INDIRECT("1"&amp;":"&amp;LEN(F69))),1)*1),MID(F69,ROW(INDIRECT("1"&amp;":"&amp;LEN(F69))),1),"")))</f>
+        <v>134</v>
+      </c>
+      <c r="G69">
         <v>1054</v>
       </c>
       <c r="H69" t="e">
@@ -6902,13 +6809,12 @@
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="E70" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="F70" t="s">
-        <v>158</v>
-      </c>
-      <c r="G70" cm="1">
-        <f t="array" aca="1" ref="G70" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F70,ROW(INDIRECT("1"&amp;":"&amp;LEN(F70))),1)*1),MID(F70,ROW(INDIRECT("1"&amp;":"&amp;LEN(F70))),1),"")))</f>
+        <v>135</v>
+      </c>
+      <c r="G70">
         <v>1053</v>
       </c>
       <c r="H70" t="e">
@@ -6920,13 +6826,12 @@
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="E71" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F71" t="s">
-        <v>159</v>
-      </c>
-      <c r="G71" cm="1">
-        <f t="array" aca="1" ref="G71" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F71,ROW(INDIRECT("1"&amp;":"&amp;LEN(F71))),1)*1),MID(F71,ROW(INDIRECT("1"&amp;":"&amp;LEN(F71))),1),"")))</f>
+        <v>136</v>
+      </c>
+      <c r="G71">
         <v>662</v>
       </c>
       <c r="H71" t="e">
@@ -6938,13 +6843,12 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="E72" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="F72" t="s">
         <v>6</v>
       </c>
-      <c r="G72" cm="1">
-        <f t="array" aca="1" ref="G72" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F72,ROW(INDIRECT("1"&amp;":"&amp;LEN(F72))),1)*1),MID(F72,ROW(INDIRECT("1"&amp;":"&amp;LEN(F72))),1),"")))</f>
+      <c r="G72">
         <v>1146</v>
       </c>
       <c r="H72" t="e">
@@ -6956,13 +6860,12 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F73" t="s">
         <v>7</v>
       </c>
-      <c r="G73" cm="1">
-        <f t="array" aca="1" ref="G73" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F73,ROW(INDIRECT("1"&amp;":"&amp;LEN(F73))),1)*1),MID(F73,ROW(INDIRECT("1"&amp;":"&amp;LEN(F73))),1),"")))</f>
+      <c r="G73">
         <v>1147</v>
       </c>
       <c r="H73" t="e">
@@ -6974,13 +6877,12 @@
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="E74" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
         <v>8</v>
       </c>
-      <c r="G74" cm="1">
-        <f t="array" aca="1" ref="G74" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F74,ROW(INDIRECT("1"&amp;":"&amp;LEN(F74))),1)*1),MID(F74,ROW(INDIRECT("1"&amp;":"&amp;LEN(F74))),1),"")))</f>
+      <c r="G74">
         <v>1148</v>
       </c>
       <c r="H74" t="e">
@@ -6992,13 +6894,12 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="E75" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="F75" t="s">
         <v>29</v>
       </c>
-      <c r="G75" cm="1">
-        <f t="array" aca="1" ref="G75" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F75,ROW(INDIRECT("1"&amp;":"&amp;LEN(F75))),1)*1),MID(F75,ROW(INDIRECT("1"&amp;":"&amp;LEN(F75))),1),"")))</f>
+      <c r="G75">
         <v>981</v>
       </c>
       <c r="H75" t="e">
@@ -7010,13 +6911,12 @@
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="E76" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
       <c r="F76" t="s">
-        <v>160</v>
-      </c>
-      <c r="G76" cm="1">
-        <f t="array" aca="1" ref="G76" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F76,ROW(INDIRECT("1"&amp;":"&amp;LEN(F76))),1)*1),MID(F76,ROW(INDIRECT("1"&amp;":"&amp;LEN(F76))),1),"")))</f>
+        <v>137</v>
+      </c>
+      <c r="G76">
         <v>352</v>
       </c>
       <c r="H76" t="e">
@@ -7028,13 +6928,12 @@
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="E77" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="F77" t="s">
-        <v>161</v>
-      </c>
-      <c r="G77" cm="1">
-        <f t="array" aca="1" ref="G77" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F77,ROW(INDIRECT("1"&amp;":"&amp;LEN(F77))),1)*1),MID(F77,ROW(INDIRECT("1"&amp;":"&amp;LEN(F77))),1),"")))</f>
+        <v>138</v>
+      </c>
+      <c r="G77">
         <v>555</v>
       </c>
       <c r="H77" t="e">
@@ -7046,13 +6945,12 @@
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="F78" t="s">
         <v>25</v>
       </c>
-      <c r="G78" cm="1">
-        <f t="array" aca="1" ref="G78" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F78,ROW(INDIRECT("1"&amp;":"&amp;LEN(F78))),1)*1),MID(F78,ROW(INDIRECT("1"&amp;":"&amp;LEN(F78))),1),"")))</f>
+      <c r="G78">
         <v>581</v>
       </c>
       <c r="H78" t="e">
@@ -7064,13 +6962,12 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="E79" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="F79" t="s">
-        <v>162</v>
-      </c>
-      <c r="G79" cm="1">
-        <f t="array" aca="1" ref="G79" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F79,ROW(INDIRECT("1"&amp;":"&amp;LEN(F79))),1)*1),MID(F79,ROW(INDIRECT("1"&amp;":"&amp;LEN(F79))),1),"")))</f>
+        <v>139</v>
+      </c>
+      <c r="G79">
         <v>353</v>
       </c>
       <c r="H79" t="e">
@@ -7082,13 +6979,12 @@
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="E80" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="F80" t="s">
-        <v>163</v>
-      </c>
-      <c r="G80" cm="1">
-        <f t="array" aca="1" ref="G80" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F80,ROW(INDIRECT("1"&amp;":"&amp;LEN(F80))),1)*1),MID(F80,ROW(INDIRECT("1"&amp;":"&amp;LEN(F80))),1),"")))</f>
+        <v>140</v>
+      </c>
+      <c r="G80">
         <v>577</v>
       </c>
       <c r="H80" t="e">
@@ -7100,13 +6996,12 @@
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="E81" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="F81" t="s">
-        <v>164</v>
-      </c>
-      <c r="G81" cm="1">
-        <f t="array" aca="1" ref="G81" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F81,ROW(INDIRECT("1"&amp;":"&amp;LEN(F81))),1)*1),MID(F81,ROW(INDIRECT("1"&amp;":"&amp;LEN(F81))),1),"")))</f>
+        <v>141</v>
+      </c>
+      <c r="G81">
         <v>553</v>
       </c>
       <c r="H81" t="e">
@@ -7118,13 +7013,12 @@
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="E82" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="F82" t="s">
-        <v>165</v>
-      </c>
-      <c r="G82" cm="1">
-        <f t="array" aca="1" ref="G82" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F82,ROW(INDIRECT("1"&amp;":"&amp;LEN(F82))),1)*1),MID(F82,ROW(INDIRECT("1"&amp;":"&amp;LEN(F82))),1),"")))</f>
+        <v>142</v>
+      </c>
+      <c r="G82">
         <v>538</v>
       </c>
       <c r="H82" t="e">
@@ -7136,13 +7030,12 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="F83" t="s">
         <v>1</v>
       </c>
-      <c r="G83" cm="1">
-        <f t="array" aca="1" ref="G83" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F83,ROW(INDIRECT("1"&amp;":"&amp;LEN(F83))),1)*1),MID(F83,ROW(INDIRECT("1"&amp;":"&amp;LEN(F83))),1),"")))</f>
+      <c r="G83">
         <v>1003</v>
       </c>
       <c r="H83" t="e">
@@ -7154,13 +7047,12 @@
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="E84" t="s">
-        <v>110</v>
+        <v>216</v>
       </c>
       <c r="F84" t="s">
         <v>2</v>
       </c>
-      <c r="G84" cm="1">
-        <f t="array" aca="1" ref="G84" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F84,ROW(INDIRECT("1"&amp;":"&amp;LEN(F84))),1)*1),MID(F84,ROW(INDIRECT("1"&amp;":"&amp;LEN(F84))),1),"")))</f>
+      <c r="G84">
         <v>1114</v>
       </c>
       <c r="H84" t="e">
@@ -7172,13 +7064,12 @@
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="E85" t="s">
-        <v>111</v>
+        <v>217</v>
       </c>
       <c r="F85" t="s">
         <v>4</v>
       </c>
-      <c r="G85" cm="1">
-        <f t="array" aca="1" ref="G85" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F85,ROW(INDIRECT("1"&amp;":"&amp;LEN(F85))),1)*1),MID(F85,ROW(INDIRECT("1"&amp;":"&amp;LEN(F85))),1),"")))</f>
+      <c r="G85">
         <v>1116</v>
       </c>
       <c r="H85" t="e">
@@ -7190,13 +7081,12 @@
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="E86" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F86" t="s">
         <v>6</v>
       </c>
-      <c r="G86" cm="1">
-        <f t="array" aca="1" ref="G86" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F86,ROW(INDIRECT("1"&amp;":"&amp;LEN(F86))),1)*1),MID(F86,ROW(INDIRECT("1"&amp;":"&amp;LEN(F86))),1),"")))</f>
+      <c r="G86">
         <v>1146</v>
       </c>
       <c r="H86" t="e">
@@ -7206,13 +7096,12 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E87" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="F87" t="s">
-        <v>189</v>
-      </c>
-      <c r="G87" cm="1">
-        <f t="array" aca="1" ref="G87" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1)*1),MID(F87,ROW(INDIRECT("1"&amp;":"&amp;LEN(F87))),1),"")))</f>
+        <v>166</v>
+      </c>
+      <c r="G87">
         <v>1362</v>
       </c>
       <c r="H87" t="e">
@@ -7222,13 +7111,12 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="F88" t="s">
-        <v>190</v>
-      </c>
-      <c r="G88" cm="1">
-        <f t="array" aca="1" ref="G88" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1)*1),MID(F88,ROW(INDIRECT("1"&amp;":"&amp;LEN(F88))),1),"")))</f>
+        <v>167</v>
+      </c>
+      <c r="G88">
         <v>1372</v>
       </c>
       <c r="H88" t="e">
@@ -7238,13 +7126,12 @@
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="F89" t="s">
-        <v>191</v>
-      </c>
-      <c r="G89" cm="1">
-        <f t="array" aca="1" ref="G89" ca="1">VALUE(_xlfn.TEXTJOIN("",TRUE,IF(ISNUMBER(MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1)*1),MID(F89,ROW(INDIRECT("1"&amp;":"&amp;LEN(F89))),1),"")))</f>
+        <v>168</v>
+      </c>
+      <c r="G89">
         <v>1373</v>
       </c>
       <c r="H89" t="e">
@@ -7254,10 +7141,10 @@
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E90" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="F90" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="G90">
         <v>1387</v>
@@ -7269,10 +7156,10 @@
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E91" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="F91" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="G91">
         <v>1388</v>
@@ -7284,10 +7171,10 @@
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="F92" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="G92">
         <v>1389</v>
@@ -7299,10 +7186,10 @@
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="F93" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="G93">
         <v>1390</v>

</xml_diff>

<commit_message>
feat: update template with new nodes config
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A257F97-D429-4A70-8A8E-B96B2A1BFD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C218048-D0DB-4C8B-8F7A-8410EE434C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,8 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$X$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$P$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$X$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$P$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="215">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -576,9 +576,6 @@
 (ms)</t>
   </si>
   <si>
-    <t>MBP THROTTLE</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
@@ -589,9 +586,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>Java 6</t>
   </si>
   <si>
     <t>ALGO</t>
@@ -624,9 +618,6 @@
   </si>
   <si>
     <t>1390/delay.log</t>
-  </si>
-  <si>
-    <t>nodo dedicado a un único cliente que fué desactivado</t>
   </si>
   <si>
     <t>MBP 10 BYTPASBUE1388 .157 - .157</t>
@@ -1336,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-  <dimension ref="B2:X46"/>
+  <dimension ref="B2:X45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1367,7 +1358,7 @@
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="X2" s="8"/>
     </row>
@@ -1469,7 +1460,7 @@
         <v>153</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>160</v>
@@ -1490,7 +1481,7 @@
         <v>162</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M8" s="22" t="s">
         <v>174</v>
@@ -1517,16 +1508,16 @@
         <v>0</v>
       </c>
       <c r="U8" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="V8" s="22" t="s">
         <v>177</v>
-      </c>
-      <c r="V8" s="22" t="s">
-        <v>178</v>
       </c>
       <c r="W8" s="20" t="s">
         <v>149</v>
       </c>
       <c r="X8" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -2610,7 +2601,7 @@
       </c>
       <c r="E21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F21" s="14" t="str">
         <f>+VLOOKUP($B21,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2699,7 +2690,7 @@
       </c>
       <c r="E22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F22" s="14" t="str">
         <f>+VLOOKUP($B22,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -2788,7 +2779,7 @@
       </c>
       <c r="E23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
+        <v>MANOLITO</v>
       </c>
       <c r="F23" s="14" t="str">
         <f>+VLOOKUP($B23,'Users+Static Data'!$K:$P,F$7,0)</f>
@@ -3842,7 +3833,7 @@
         <v>n/a</v>
       </c>
       <c r="X34" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.3">
@@ -4114,7 +4105,7 @@
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C38" s="24">
         <v>1389</v>
@@ -4203,7 +4194,7 @@
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C39" s="24">
         <v>1390</v>
@@ -4559,7 +4550,7 @@
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C43" s="24">
         <v>1387</v>
@@ -4646,9 +4637,9 @@
       </c>
       <c r="X43" s="25"/>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C44" s="24">
         <v>1388</v>
@@ -4735,128 +4726,37 @@
       </c>
       <c r="X44" s="25"/>
     </row>
-    <row r="45" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="24">
-        <v>1003</v>
-      </c>
-      <c r="D45" s="14" t="str">
-        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,D$7,0)</f>
-        <v>ALGO</v>
-      </c>
-      <c r="E45" s="14" t="str">
-        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,E$7,0)</f>
-        <v>Java 6</v>
-      </c>
-      <c r="F45" s="14" t="str">
-        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,F$7,0)</f>
-        <v>BE</v>
-      </c>
-      <c r="G45" s="14" t="str">
-        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,G$7,0)</f>
-        <v>MD</v>
-      </c>
-      <c r="H45" s="14" t="str">
-        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBP THROTTLE</v>
-      </c>
-      <c r="I45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="J45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,J$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="K45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,K$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="L45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,L$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="M45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,M$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="N45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,N$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="O45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,O$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="P45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,P$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="Q45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,Q$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="R45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,R$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="S45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,S$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="T45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,T$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="U45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,U$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="V45" s="15" t="str">
-        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,V$7,0))</f>
-        <v>n/a</v>
-      </c>
-      <c r="W45" s="15" t="str">
-        <f>IF(ISNUMBER(VLOOKUP($B45,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B45,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
-        <v>n/a</v>
-      </c>
-      <c r="X45" s="25" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="27"/>
-      <c r="T46" s="27"/>
-      <c r="U46" s="27"/>
-      <c r="V46" s="27"/>
-      <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
+      <c r="V45" s="27"/>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:X45" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:X45">
-      <sortCondition descending="1" ref="D8:D45"/>
+  <autoFilter ref="B8:X44" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:X44">
+      <sortCondition descending="1" ref="D8:D44"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C9:H45">
+  <conditionalFormatting sqref="C9:H44">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
     </cfRule>
@@ -4864,7 +4764,7 @@
       <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:H45">
+  <conditionalFormatting sqref="D9:H44">
     <cfRule type="expression" dxfId="5" priority="1">
       <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
@@ -4881,8 +4781,8 @@
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K45">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="K9:K44">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4891,8 +4791,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9:L45">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="L9:L44">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4901,8 +4801,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P9:P45">
-    <cfRule type="colorScale" priority="27">
+  <conditionalFormatting sqref="P9:P44">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4911,8 +4811,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q9:Q45">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="Q9:Q44">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4921,8 +4821,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R9:R45">
-    <cfRule type="colorScale" priority="29">
+  <conditionalFormatting sqref="R9:R44">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4931,8 +4831,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:U45">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="U9:U44">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4941,19 +4841,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V9:V45">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="U9:V44 O9:R44 J9:M44">
+    <cfRule type="expression" dxfId="0" priority="62">
+      <formula>J9=MIN(J$9:J$44)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V9:V44">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:M45 O9:R45 U9:V45">
-    <cfRule type="expression" dxfId="0" priority="48">
-      <formula>J9=MIN(J$9:J$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5056,7 +4956,7 @@
         <v>153</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>157</v>
@@ -5091,7 +4991,7 @@
         <v>90</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N7" t="s">
         <v>156</v>
@@ -5123,10 +5023,10 @@
         <v>22</v>
       </c>
       <c r="L8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N8" t="s">
         <v>156</v>
@@ -5158,10 +5058,10 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N9" t="s">
         <v>156</v>
@@ -5193,10 +5093,10 @@
         <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N10" t="s">
         <v>156</v>
@@ -5228,10 +5128,10 @@
         <v>25</v>
       </c>
       <c r="L11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N11" t="s">
         <v>156</v>
@@ -5263,10 +5163,10 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N12" t="s">
         <v>156</v>
@@ -5298,10 +5198,10 @@
         <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N13" t="s">
         <v>156</v>
@@ -5317,7 +5217,7 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -5330,12 +5230,12 @@
         <v>#N/A</v>
       </c>
       <c r="K14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" t="s">
-        <v>181</v>
-      </c>
-      <c r="M14" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="18" t="s">
         <v>180</v>
       </c>
       <c r="N14" t="s">
@@ -5345,7 +5245,7 @@
         <v>93</v>
       </c>
       <c r="P14" t="s">
-        <v>175</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -5365,13 +5265,13 @@
         <v>#N/A</v>
       </c>
       <c r="K15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" t="s">
         <v>90</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N15" t="s">
         <v>156</v>
@@ -5380,14 +5280,14 @@
         <v>93</v>
       </c>
       <c r="P15" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -5400,13 +5300,13 @@
         <v>#N/A</v>
       </c>
       <c r="K16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16" t="s">
         <v>90</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N16" t="s">
         <v>156</v>
@@ -5422,7 +5322,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="E17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F17" t="s">
         <v>101</v>
@@ -5435,13 +5335,13 @@
         <v>#N/A</v>
       </c>
       <c r="K17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L17" t="s">
         <v>90</v>
       </c>
       <c r="M17" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N17" t="s">
         <v>156</v>
@@ -5450,14 +5350,14 @@
         <v>93</v>
       </c>
       <c r="P17" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="E18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F18" t="s">
         <v>102</v>
@@ -5470,13 +5370,13 @@
         <v>#N/A</v>
       </c>
       <c r="K18" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L18" t="s">
         <v>90</v>
       </c>
       <c r="M18" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N18" t="s">
         <v>156</v>
@@ -5485,14 +5385,14 @@
         <v>93</v>
       </c>
       <c r="P18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="E19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F19" t="s">
         <v>103</v>
@@ -5505,12 +5405,12 @@
         <v>#N/A</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L19" t="s">
         <v>90</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="18" t="s">
         <v>180</v>
       </c>
       <c r="N19" t="s">
@@ -5527,7 +5427,7 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F20" t="s">
         <v>104</v>
@@ -5540,12 +5440,12 @@
         <v>#N/A</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L20" t="s">
         <v>90</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="18" t="s">
         <v>180</v>
       </c>
       <c r="N20" t="s">
@@ -5562,7 +5462,7 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F21" t="s">
         <v>105</v>
@@ -5575,12 +5475,12 @@
         <v>#N/A</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L21" t="s">
         <v>90</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="18" t="s">
         <v>180</v>
       </c>
       <c r="N21" t="s">
@@ -5590,14 +5490,14 @@
         <v>93</v>
       </c>
       <c r="P21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="E22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
@@ -5610,13 +5510,13 @@
         <v>#N/A</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L22" t="s">
         <v>90</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N22" t="s">
         <v>156</v>
@@ -5632,7 +5532,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="E23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -5645,13 +5545,13 @@
         <v>#N/A</v>
       </c>
       <c r="K23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L23" t="s">
         <v>90</v>
       </c>
       <c r="M23" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N23" t="s">
         <v>156</v>
@@ -5680,13 +5580,13 @@
         <v>#N/A</v>
       </c>
       <c r="K24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L24" t="s">
         <v>90</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N24" t="s">
         <v>156</v>
@@ -5715,13 +5615,13 @@
         <v>#N/A</v>
       </c>
       <c r="K25" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="L25" t="s">
         <v>90</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N25" t="s">
         <v>156</v>
@@ -5730,7 +5630,7 @@
         <v>93</v>
       </c>
       <c r="P25" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
@@ -5750,13 +5650,13 @@
         <v>#N/A</v>
       </c>
       <c r="K26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="L26" t="s">
         <v>90</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N26" t="s">
         <v>156</v>
@@ -5765,7 +5665,7 @@
         <v>93</v>
       </c>
       <c r="P26" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
@@ -5785,13 +5685,13 @@
         <v>#N/A</v>
       </c>
       <c r="K27" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" t="s">
-        <v>90</v>
+        <v>6</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="M27" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N27" t="s">
         <v>156</v>
@@ -5800,7 +5700,7 @@
         <v>93</v>
       </c>
       <c r="P27" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
@@ -5820,13 +5720,13 @@
         <v>#N/A</v>
       </c>
       <c r="K28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L28" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M28" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N28" t="s">
         <v>156</v>
@@ -5855,13 +5755,13 @@
         <v>#N/A</v>
       </c>
       <c r="K29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L29" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M29" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N29" t="s">
         <v>156</v>
@@ -5890,13 +5790,13 @@
         <v>#N/A</v>
       </c>
       <c r="K30" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L30" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M30" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N30" t="s">
         <v>156</v>
@@ -5925,13 +5825,13 @@
         <v>#N/A</v>
       </c>
       <c r="K31" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="L31" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M31" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N31" t="s">
         <v>156</v>
@@ -5947,7 +5847,7 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="E32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F32" t="s">
         <v>112</v>
@@ -5960,13 +5860,13 @@
         <v>#N/A</v>
       </c>
       <c r="K32" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="L32" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N32" t="s">
         <v>156</v>
@@ -5982,7 +5882,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="E33" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F33" t="s">
         <v>113</v>
@@ -5995,13 +5895,13 @@
         <v>#N/A</v>
       </c>
       <c r="K33" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L33" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M33" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N33" t="s">
         <v>156</v>
@@ -6030,13 +5930,13 @@
         <v>#N/A</v>
       </c>
       <c r="K34" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L34" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N34" t="s">
         <v>156</v>
@@ -6052,7 +5952,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="E35" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F35" t="s">
         <v>21</v>
@@ -6065,13 +5965,13 @@
         <v>#N/A</v>
       </c>
       <c r="K35" t="s">
-        <v>168</v>
+        <v>11</v>
       </c>
       <c r="L35" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M35" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N35" t="s">
         <v>156</v>
@@ -6100,13 +6000,13 @@
         <v>#N/A</v>
       </c>
       <c r="K36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L36" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N36" t="s">
         <v>156</v>
@@ -6135,13 +6035,13 @@
         <v>#N/A</v>
       </c>
       <c r="K37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L37" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N37" t="s">
         <v>156</v>
@@ -6170,13 +6070,13 @@
         <v>#N/A</v>
       </c>
       <c r="K38" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="L38" s="18" t="s">
         <v>92</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N38" t="s">
         <v>156</v>
@@ -6192,7 +6092,7 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="E39" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F39" t="s">
         <v>16</v>
@@ -6205,13 +6105,13 @@
         <v>#N/A</v>
       </c>
       <c r="K39" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="M39" s="18" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="L39" t="s">
+        <v>179</v>
+      </c>
+      <c r="M39" t="s">
+        <v>180</v>
       </c>
       <c r="N39" t="s">
         <v>156</v>
@@ -6220,7 +6120,7 @@
         <v>93</v>
       </c>
       <c r="P39" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
@@ -6240,13 +6140,13 @@
         <v>#N/A</v>
       </c>
       <c r="K40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N40" t="s">
         <v>156</v>
@@ -6275,13 +6175,13 @@
         <v>#N/A</v>
       </c>
       <c r="K41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L41" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M41" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N41" t="s">
         <v>156</v>
@@ -6290,7 +6190,7 @@
         <v>93</v>
       </c>
       <c r="P41" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
@@ -6310,13 +6210,13 @@
         <v>#N/A</v>
       </c>
       <c r="K42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N42" t="s">
         <v>156</v>
@@ -6332,7 +6232,7 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="E43" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F43" t="s">
         <v>28</v>
@@ -6343,24 +6243,6 @@
       <c r="H43" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
-      </c>
-      <c r="K43" t="s">
-        <v>190</v>
-      </c>
-      <c r="L43" t="s">
-        <v>181</v>
-      </c>
-      <c r="M43" t="s">
-        <v>182</v>
-      </c>
-      <c r="N43" t="s">
-        <v>156</v>
-      </c>
-      <c r="O43" t="s">
-        <v>93</v>
-      </c>
-      <c r="P43" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
@@ -6418,7 +6300,7 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="E47" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F47" t="s">
         <v>3</v>
@@ -6486,7 +6368,7 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="E51" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F51" t="s">
         <v>18</v>
@@ -6503,7 +6385,7 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="E52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
@@ -6690,7 +6572,7 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="E63" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F63" t="s">
         <v>15</v>
@@ -6911,7 +6793,7 @@
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="E76" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F76" t="s">
         <v>137</v>
@@ -7030,7 +6912,7 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="E83" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F83" t="s">
         <v>1</v>
@@ -7047,7 +6929,7 @@
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="E84" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
         <v>2</v>
@@ -7064,7 +6946,7 @@
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="E85" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F85" t="s">
         <v>4</v>
@@ -7141,10 +7023,10 @@
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E90" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F90" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G90">
         <v>1387</v>
@@ -7156,10 +7038,10 @@
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E91" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F91" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G91">
         <v>1388</v>
@@ -7171,10 +7053,10 @@
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G92">
         <v>1389</v>
@@ -7186,10 +7068,10 @@
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F93" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G93">
         <v>1390</v>

</xml_diff>

<commit_message>
feat: add columns for template
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C218048-D0DB-4C8B-8F7A-8410EE434C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9FB8F7-A87D-4C51-ACC7-F30D321C4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$X$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$AA$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$P$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="218">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -696,6 +696,15 @@
   </si>
   <si>
     <t>DMA MBP BYTPASBUE1116 - .134</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>infr</t>
+  </si>
+  <si>
+    <t>logs</t>
   </si>
 </sst>
 </file>
@@ -784,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -879,12 +888,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -937,6 +968,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1327,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-  <dimension ref="B2:X45"/>
+  <dimension ref="B2:AA45"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1352,36 +1389,37 @@
     <col min="21" max="21" width="7.33203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="1" customWidth="1"/>
     <col min="23" max="23" width="7.44140625" customWidth="1"/>
-    <col min="24" max="24" width="61.5546875" customWidth="1"/>
+    <col min="24" max="26" width="2.44140625" customWidth="1"/>
+    <col min="27" max="27" width="61.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="X2" s="8"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA2" s="8"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="16"/>
-      <c r="X4" s="9"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA4" s="9"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="X5" s="9"/>
-    </row>
-    <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA5" s="9"/>
+    </row>
+    <row r="7" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="12">
         <v>2</v>
       </c>
@@ -1445,11 +1483,14 @@
       <c r="W7" s="12">
         <v>16</v>
       </c>
-      <c r="X7" s="12">
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:24" s="10" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:27" s="10" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>164</v>
       </c>
@@ -1516,11 +1557,20 @@
       <c r="W8" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="X8" s="23" t="s">
+      <c r="X8" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y8" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z8" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA8" s="23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
@@ -1607,9 +1657,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B9,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B9,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X9" s="25"/>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
@@ -1696,9 +1749,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B10,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B10,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X10" s="25"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1785,9 +1841,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B11,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B11,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X11" s="25"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1874,9 +1933,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B12,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B12,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X12" s="25"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>29</v>
       </c>
@@ -1963,9 +2025,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B13,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B13,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X13" s="25"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>30</v>
       </c>
@@ -2052,9 +2117,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B14,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B14,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X14" s="25"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
@@ -2141,9 +2209,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B15,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B15,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X15" s="25"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>7</v>
       </c>
@@ -2230,9 +2301,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B16,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B16,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X16" s="25"/>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="25"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2319,9 +2393,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B17,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B17,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X17" s="25"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="25"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>166</v>
       </c>
@@ -2408,9 +2485,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B18,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B18,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X18" s="25"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="25"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>167</v>
       </c>
@@ -2497,9 +2577,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B19,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B19,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X19" s="25"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="25"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>168</v>
       </c>
@@ -2586,9 +2669,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B20,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B20,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X20" s="25"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="25"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>15</v>
       </c>
@@ -2675,9 +2761,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B21,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B21,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X21" s="25"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="25"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
         <v>16</v>
       </c>
@@ -2764,9 +2853,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B22,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B22,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X22" s="25"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="25"/>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>17</v>
       </c>
@@ -2853,9 +2945,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B23,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B23,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X23" s="25"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X23" s="29"/>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="29"/>
+      <c r="AA23" s="25"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
         <v>28</v>
       </c>
@@ -2942,9 +3037,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B24,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B24,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X24" s="25"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="25"/>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
         <v>3</v>
       </c>
@@ -3031,9 +3129,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B25,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B25,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X25" s="25"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="29"/>
+      <c r="AA25" s="25"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
         <v>4</v>
       </c>
@@ -3120,9 +3221,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B26,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B26,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X26" s="25"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="25"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
         <v>10</v>
       </c>
@@ -3209,9 +3313,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B27,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B27,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X27" s="25"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="25"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
@@ -3298,9 +3405,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B28,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B28,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X28" s="25"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="25"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
@@ -3387,9 +3497,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B29,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B29,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X29" s="25"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="25"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
         <v>20</v>
       </c>
@@ -3476,9 +3589,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B30,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B30,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X30" s="25"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
+      <c r="AA30" s="25"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
         <v>21</v>
       </c>
@@ -3565,9 +3681,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B31,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B31,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X31" s="25"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="29"/>
+      <c r="AA31" s="25"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
         <v>2</v>
       </c>
@@ -3654,9 +3773,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B32,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B32,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X32" s="25"/>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
+      <c r="AA32" s="25"/>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
         <v>5</v>
       </c>
@@ -3743,9 +3865,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B33,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B33,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X33" s="25"/>
-    </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="29"/>
+      <c r="AA33" s="25"/>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
         <v>9</v>
       </c>
@@ -3832,11 +3957,14 @@
         <f>IF(ISNUMBER(VLOOKUP($B34,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B34,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X34" s="25" t="s">
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
+      <c r="AA34" s="25" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" s="12" t="s">
         <v>22</v>
       </c>
@@ -3923,9 +4051,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B35,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B35,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X35" s="25"/>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X35" s="29"/>
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="29"/>
+      <c r="AA35" s="25"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="s">
         <v>23</v>
       </c>
@@ -4012,9 +4143,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B36,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B36,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X36" s="25"/>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X36" s="29"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="25"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" s="12" t="s">
         <v>24</v>
       </c>
@@ -4101,9 +4235,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B37,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B37,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X37" s="25"/>
-    </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="25"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
         <v>187</v>
       </c>
@@ -4190,9 +4327,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B38,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B38,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X38" s="25"/>
-    </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="25"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
         <v>188</v>
       </c>
@@ -4279,9 +4419,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B39,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B39,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X39" s="25"/>
-    </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="25"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B40" s="12" t="s">
         <v>25</v>
       </c>
@@ -4368,9 +4511,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B40,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B40,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X40" s="25"/>
-    </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="25"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B41" s="12" t="s">
         <v>26</v>
       </c>
@@ -4457,9 +4603,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B41,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B41,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X41" s="25"/>
-    </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="25"/>
+    </row>
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B42" s="12" t="s">
         <v>27</v>
       </c>
@@ -4546,9 +4695,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B42,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B42,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X42" s="25"/>
-    </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="25"/>
+    </row>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
         <v>185</v>
       </c>
@@ -4635,9 +4787,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B43,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B43,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X43" s="25"/>
-    </row>
-    <row r="44" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="25"/>
+    </row>
+    <row r="44" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="12" t="s">
         <v>186</v>
       </c>
@@ -4724,9 +4879,12 @@
         <f>IF(ISNUMBER(VLOOKUP($B44,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B44,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
         <v>n/a</v>
       </c>
-      <c r="X44" s="25"/>
-    </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="25"/>
+    </row>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
@@ -4749,10 +4907,13 @@
       <c r="V45" s="27"/>
       <c r="W45" s="26"/>
       <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="26"/>
+      <c r="AA45" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:X44" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:X44">
+  <autoFilter ref="B8:AA44" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA44">
       <sortCondition descending="1" ref="D8:D44"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
feat: add epam nodes to template
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9FB8F7-A87D-4C51-ACC7-F30D321C4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A79EE0-5CBB-4D43-9FFD-55126E90F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$AA$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$AA$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$P$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="222">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -705,6 +705,18 @@
   </si>
   <si>
     <t>logs</t>
+  </si>
+  <si>
+    <t>epam1440/delay.log</t>
+  </si>
+  <si>
+    <t>EPAM</t>
+  </si>
+  <si>
+    <t>epam1441/delay.log</t>
+  </si>
+  <si>
+    <t>epam891/delay.log</t>
   </si>
 </sst>
 </file>
@@ -1364,9 +1376,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-  <dimension ref="B2:AA45"/>
+  <dimension ref="B2:AA48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1490,7 +1502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:27" s="10" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:27" s="10" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>164</v>
       </c>
@@ -4792,7 +4804,7 @@
       <c r="Z43" s="29"/>
       <c r="AA43" s="25"/>
     </row>
-    <row r="44" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
         <v>186</v>
       </c>
@@ -4885,39 +4897,315 @@
       <c r="AA44" s="25"/>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
-      <c r="V45" s="27"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
-      <c r="Z45" s="26"/>
-      <c r="AA45" s="26"/>
+      <c r="B45" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C45" s="24">
+        <v>1440</v>
+      </c>
+      <c r="D45" s="14" t="str">
+        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E45" s="14" t="str">
+        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F45" s="14" t="str">
+        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G45" s="14" t="str">
+        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H45" s="14" t="str">
+        <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP</v>
+      </c>
+      <c r="I45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V45" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B45,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B45,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W45" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B45,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B45,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X45" s="29"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="29"/>
+      <c r="AA45" s="25"/>
+    </row>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="24">
+        <v>1441</v>
+      </c>
+      <c r="D46" s="14" t="str">
+        <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E46" s="14" t="str">
+        <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F46" s="14" t="str">
+        <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G46" s="14" t="str">
+        <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H46" s="14" t="str">
+        <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP</v>
+      </c>
+      <c r="I46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B46,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V46" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B46,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B46,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W46" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B46,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B46,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X46" s="29"/>
+      <c r="Y46" s="29"/>
+      <c r="Z46" s="29"/>
+      <c r="AA46" s="25"/>
+    </row>
+    <row r="47" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="24">
+        <v>891</v>
+      </c>
+      <c r="D47" s="14" t="str">
+        <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E47" s="14" t="str">
+        <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F47" s="14" t="str">
+        <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G47" s="14" t="str">
+        <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H47" s="14" t="str">
+        <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP</v>
+      </c>
+      <c r="I47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B47,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V47" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B47,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B47,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W47" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B47,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B47,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="25"/>
+    </row>
+    <row r="48" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+      <c r="N48" s="27"/>
+      <c r="O48" s="27"/>
+      <c r="P48" s="27"/>
+      <c r="Q48" s="27"/>
+      <c r="R48" s="27"/>
+      <c r="S48" s="27"/>
+      <c r="T48" s="27"/>
+      <c r="U48" s="27"/>
+      <c r="V48" s="27"/>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
+      <c r="Y48" s="26"/>
+      <c r="Z48" s="26"/>
+      <c r="AA48" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:AA44" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA44">
-      <sortCondition descending="1" ref="D8:D44"/>
+  <autoFilter ref="B8:AA47" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA47">
+      <sortCondition descending="1" ref="D8:D47"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C9:H44">
+  <conditionalFormatting sqref="C9:H47">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
     </cfRule>
@@ -4925,7 +5213,7 @@
       <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:H44">
+  <conditionalFormatting sqref="D9:H47">
     <cfRule type="expression" dxfId="5" priority="1">
       <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
@@ -4942,7 +5230,7 @@
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K44">
+  <conditionalFormatting sqref="K9:K47">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -4952,7 +5240,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9:L44">
+  <conditionalFormatting sqref="L9:L47">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -4962,7 +5250,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P9:P44">
+  <conditionalFormatting sqref="P9:P47">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -4972,7 +5260,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q9:Q44">
+  <conditionalFormatting sqref="Q9:Q47">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -4982,7 +5270,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R9:R44">
+  <conditionalFormatting sqref="R9:R47">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -4992,7 +5280,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:U44">
+  <conditionalFormatting sqref="U9:U47">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -5002,12 +5290,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:V44 O9:R44 J9:M44">
+  <conditionalFormatting sqref="U9:V47 O9:R47 J9:M47">
     <cfRule type="expression" dxfId="0" priority="62">
-      <formula>J9=MIN(J$9:J$44)</formula>
+      <formula>J9=MIN(J$9:J$47)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V9:V44">
+  <conditionalFormatting sqref="V9:V47">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -6405,6 +6693,24 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K43" t="s">
+        <v>218</v>
+      </c>
+      <c r="L43" t="s">
+        <v>179</v>
+      </c>
+      <c r="M43" t="s">
+        <v>219</v>
+      </c>
+      <c r="N43" t="s">
+        <v>156</v>
+      </c>
+      <c r="O43" t="s">
+        <v>93</v>
+      </c>
+      <c r="P43" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
@@ -6422,6 +6728,24 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K44" t="s">
+        <v>220</v>
+      </c>
+      <c r="L44" t="s">
+        <v>179</v>
+      </c>
+      <c r="M44" t="s">
+        <v>219</v>
+      </c>
+      <c r="N44" t="s">
+        <v>156</v>
+      </c>
+      <c r="O44" t="s">
+        <v>93</v>
+      </c>
+      <c r="P44" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
@@ -6439,6 +6763,24 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K45" t="s">
+        <v>221</v>
+      </c>
+      <c r="L45" t="s">
+        <v>179</v>
+      </c>
+      <c r="M45" t="s">
+        <v>219</v>
+      </c>
+      <c r="N45" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" t="s">
+        <v>93</v>
+      </c>
+      <c r="P45" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>

</xml_diff>

<commit_message>
feat: add QA nodes to template
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A79EE0-5CBB-4D43-9FFD-55126E90F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B18C0E-7A9F-4CA6-8BB9-95AF5F424DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Users+Static Data" sheetId="33" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$AA$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$B$8:$AA$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Users+Static Data'!$K$6:$P$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="236">
   <si>
     <t>Tamaño muestra</t>
   </si>
@@ -707,16 +707,58 @@
     <t>logs</t>
   </si>
   <si>
-    <t>epam1440/delay.log</t>
-  </si>
-  <si>
     <t>EPAM</t>
   </si>
   <si>
-    <t>epam1441/delay.log</t>
-  </si>
-  <si>
-    <t>epam891/delay.log</t>
+    <t>epam495/delay.log</t>
+  </si>
+  <si>
+    <t>epam076/delay.log</t>
+  </si>
+  <si>
+    <t>epam1127/delay.log</t>
+  </si>
+  <si>
+    <t>261/delay.log</t>
+  </si>
+  <si>
+    <t>1010/delay.log</t>
+  </si>
+  <si>
+    <t>1483/delay.log</t>
+  </si>
+  <si>
+    <t>QA EOMM</t>
+  </si>
+  <si>
+    <t>QA ALGO</t>
+  </si>
+  <si>
+    <t>JAVA 6</t>
+  </si>
+  <si>
+    <t>1353/delay.log</t>
+  </si>
+  <si>
+    <t>MBP FULL</t>
+  </si>
+  <si>
+    <t>MBP R VAR</t>
+  </si>
+  <si>
+    <t>MBP R FIJA</t>
+  </si>
+  <si>
+    <t>MDFULL_1444/delay.log</t>
+  </si>
+  <si>
+    <t>MDFULL_891/delay.log</t>
+  </si>
+  <si>
+    <t>MDRF_1441/delay.log</t>
+  </si>
+  <si>
+    <t>MDRV_1440/delay.log</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1033,29 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1045,6 +1109,16 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1376,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-  <dimension ref="B2:AA48"/>
+  <dimension ref="B2:AA56"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:W55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,7 +1461,7 @@
     <col min="1" max="1" width="2.88671875" customWidth="1"/>
     <col min="2" max="2" width="3.44140625" customWidth="1"/>
     <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="7" width="0.109375" customWidth="1"/>
     <col min="8" max="8" width="11.77734375" customWidth="1"/>
@@ -4898,10 +4972,10 @@
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="C45" s="24">
-        <v>1440</v>
+        <v>1444</v>
       </c>
       <c r="D45" s="14" t="str">
         <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -4921,7 +4995,7 @@
       </c>
       <c r="H45" s="14" t="str">
         <f>+VLOOKUP($B45,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBP</v>
+        <v>MBP FULL</v>
       </c>
       <c r="I45" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B45,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -4990,10 +5064,10 @@
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C46" s="24">
-        <v>1441</v>
+        <v>891</v>
       </c>
       <c r="D46" s="14" t="str">
         <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -5013,7 +5087,7 @@
       </c>
       <c r="H46" s="14" t="str">
         <f>+VLOOKUP($B46,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBP</v>
+        <v>MBP FULL</v>
       </c>
       <c r="I46" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B46,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B46,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -5080,12 +5154,12 @@
       <c r="Z46" s="29"/>
       <c r="AA46" s="25"/>
     </row>
-    <row r="47" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B47" s="12" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C47" s="24">
-        <v>891</v>
+        <v>1441</v>
       </c>
       <c r="D47" s="14" t="str">
         <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,D$7,0)</f>
@@ -5105,7 +5179,7 @@
       </c>
       <c r="H47" s="14" t="str">
         <f>+VLOOKUP($B47,'Users+Static Data'!$K:$P,H$7,0)</f>
-        <v>MBP</v>
+        <v>MBP R FIJA</v>
       </c>
       <c r="I47" s="15" t="str">
         <f>IF(IFERROR(VLOOKUP($B47,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B47,'Users+Static Data'!$F:$H,I$7,0))</f>
@@ -5173,104 +5247,803 @@
       <c r="AA47" s="25"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
-      <c r="S48" s="27"/>
-      <c r="T48" s="27"/>
-      <c r="U48" s="27"/>
-      <c r="V48" s="27"/>
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
-      <c r="Y48" s="26"/>
-      <c r="Z48" s="26"/>
-      <c r="AA48" s="26"/>
+      <c r="B48" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="24">
+        <v>1440</v>
+      </c>
+      <c r="D48" s="14" t="str">
+        <f>+VLOOKUP($B48,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>ALGO</v>
+      </c>
+      <c r="E48" s="14" t="str">
+        <f>+VLOOKUP($B48,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F48" s="14" t="str">
+        <f>+VLOOKUP($B48,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G48" s="14" t="str">
+        <f>+VLOOKUP($B48,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H48" s="14" t="str">
+        <f>+VLOOKUP($B48,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP R VAR</v>
+      </c>
+      <c r="I48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B48,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V48" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B48,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B48,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W48" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B48,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B48,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X48" s="29"/>
+      <c r="Y48" s="29"/>
+      <c r="Z48" s="29"/>
+      <c r="AA48" s="25"/>
+    </row>
+    <row r="49" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B49" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" s="24">
+        <v>261</v>
+      </c>
+      <c r="D49" s="14" t="str">
+        <f>+VLOOKUP($B49,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA EOMM</v>
+      </c>
+      <c r="E49" s="14" t="str">
+        <f>+VLOOKUP($B49,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>JAVA 6</v>
+      </c>
+      <c r="F49" s="14" t="str">
+        <f>+VLOOKUP($B49,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G49" s="14" t="str">
+        <f>+VLOOKUP($B49,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H49" s="14" t="str">
+        <f>+VLOOKUP($B49,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP+MBO</v>
+      </c>
+      <c r="I49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B49,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V49" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B49,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B49,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W49" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B49,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B49,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="25"/>
+    </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B50" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C50" s="24">
+        <v>1010</v>
+      </c>
+      <c r="D50" s="14" t="str">
+        <f>+VLOOKUP($B50,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA EOMM</v>
+      </c>
+      <c r="E50" s="14" t="str">
+        <f>+VLOOKUP($B50,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>MANOLITO</v>
+      </c>
+      <c r="F50" s="14" t="str">
+        <f>+VLOOKUP($B50,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G50" s="14" t="str">
+        <f>+VLOOKUP($B50,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H50" s="14" t="str">
+        <f>+VLOOKUP($B50,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP+MBO</v>
+      </c>
+      <c r="I50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B50,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V50" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B50,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B50,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W50" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B50,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B50,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X50" s="29"/>
+      <c r="Y50" s="29"/>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="25"/>
+    </row>
+    <row r="51" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B51" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C51" s="24">
+        <v>1483</v>
+      </c>
+      <c r="D51" s="14" t="str">
+        <f>+VLOOKUP($B51,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA EOMM</v>
+      </c>
+      <c r="E51" s="14" t="str">
+        <f>+VLOOKUP($B51,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>MANOLITO</v>
+      </c>
+      <c r="F51" s="14" t="str">
+        <f>+VLOOKUP($B51,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G51" s="14" t="str">
+        <f>+VLOOKUP($B51,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H51" s="14" t="str">
+        <f>+VLOOKUP($B51,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP+MBO</v>
+      </c>
+      <c r="I51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B51,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V51" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B51,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B51,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W51" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B51,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B51,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X51" s="29"/>
+      <c r="Y51" s="29"/>
+      <c r="Z51" s="29"/>
+      <c r="AA51" s="25"/>
+    </row>
+    <row r="52" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B52" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C52" s="24">
+        <v>1353</v>
+      </c>
+      <c r="D52" s="14" t="str">
+        <f>+VLOOKUP($B52,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA EOMM</v>
+      </c>
+      <c r="E52" s="14" t="str">
+        <f>+VLOOKUP($B52,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>MANOLITO</v>
+      </c>
+      <c r="F52" s="14" t="str">
+        <f>+VLOOKUP($B52,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G52" s="14" t="str">
+        <f>+VLOOKUP($B52,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H52" s="14" t="str">
+        <f>+VLOOKUP($B52,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP+MBO</v>
+      </c>
+      <c r="I52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B52,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V52" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B52,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B52,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W52" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B52,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B52,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X52" s="29"/>
+      <c r="Y52" s="29"/>
+      <c r="Z52" s="29"/>
+      <c r="AA52" s="25"/>
+    </row>
+    <row r="53" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B53" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" s="24">
+        <v>76</v>
+      </c>
+      <c r="D53" s="14" t="str">
+        <f>+VLOOKUP($B53,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA ALGO</v>
+      </c>
+      <c r="E53" s="14" t="str">
+        <f>+VLOOKUP($B53,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F53" s="14" t="str">
+        <f>+VLOOKUP($B53,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G53" s="14" t="str">
+        <f>+VLOOKUP($B53,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H53" s="14" t="str">
+        <f>+VLOOKUP($B53,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP FULL</v>
+      </c>
+      <c r="I53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B53,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V53" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B53,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B53,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W53" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B53,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B53,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X53" s="29"/>
+      <c r="Y53" s="29"/>
+      <c r="Z53" s="29"/>
+      <c r="AA53" s="25"/>
+    </row>
+    <row r="54" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B54" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" s="24">
+        <v>495</v>
+      </c>
+      <c r="D54" s="14" t="str">
+        <f>+VLOOKUP($B54,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA ALGO</v>
+      </c>
+      <c r="E54" s="14" t="str">
+        <f>+VLOOKUP($B54,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F54" s="14" t="str">
+        <f>+VLOOKUP($B54,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G54" s="14" t="str">
+        <f>+VLOOKUP($B54,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H54" s="14" t="str">
+        <f>+VLOOKUP($B54,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP R VAR</v>
+      </c>
+      <c r="I54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B54,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V54" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B54,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B54,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W54" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B54,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B54,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X54" s="29"/>
+      <c r="Y54" s="29"/>
+      <c r="Z54" s="29"/>
+      <c r="AA54" s="25"/>
+    </row>
+    <row r="55" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C55" s="24">
+        <v>1127</v>
+      </c>
+      <c r="D55" s="14" t="str">
+        <f>+VLOOKUP($B55,'Users+Static Data'!$K:$P,D$7,0)</f>
+        <v>QA ALGO</v>
+      </c>
+      <c r="E55" s="14" t="str">
+        <f>+VLOOKUP($B55,'Users+Static Data'!$K:$P,E$7,0)</f>
+        <v>EPAM</v>
+      </c>
+      <c r="F55" s="14" t="str">
+        <f>+VLOOKUP($B55,'Users+Static Data'!$K:$P,F$7,0)</f>
+        <v>BE</v>
+      </c>
+      <c r="G55" s="14" t="str">
+        <f>+VLOOKUP($B55,'Users+Static Data'!$K:$P,G$7,0)</f>
+        <v>MD</v>
+      </c>
+      <c r="H55" s="14" t="str">
+        <f>+VLOOKUP($B55,'Users+Static Data'!$K:$P,H$7,0)</f>
+        <v>MBP R FIJA</v>
+      </c>
+      <c r="I55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Users+Static Data'!$F:$H,I$7,0),0)=0,"n/a",VLOOKUP($B55,'Users+Static Data'!$F:$H,I$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="J55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,J$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,J$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="K55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,K$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,K$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="L55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,L$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,L$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="M55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,M$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,M$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="N55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,N$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,N$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="O55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,O$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,O$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="P55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,P$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,P$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="Q55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,Q$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,Q$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="R55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,R$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,R$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="S55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,S$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,S$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="T55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,T$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,T$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="U55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,U$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,U$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="V55" s="15" t="str">
+        <f>IF(IFERROR(VLOOKUP($B55,'Report Data'!$A:$AG,V$7,0),0)=0,"n/a",VLOOKUP($B55,'Report Data'!$A:$AG,V$7,0))</f>
+        <v>n/a</v>
+      </c>
+      <c r="W55" s="15" t="str">
+        <f>IF(ISNUMBER(VLOOKUP($B55,'Report Data'!$A:$AG,W$7,0)),VLOOKUP($B55,'Report Data'!$A:$AG,W$7,0),"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="X55" s="29"/>
+      <c r="Y55" s="29"/>
+      <c r="Z55" s="29"/>
+      <c r="AA55" s="25"/>
+    </row>
+    <row r="56" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="27"/>
+      <c r="T56" s="27"/>
+      <c r="U56" s="27"/>
+      <c r="V56" s="27"/>
+      <c r="W56" s="26"/>
+      <c r="X56" s="26"/>
+      <c r="Y56" s="26"/>
+      <c r="Z56" s="26"/>
+      <c r="AA56" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="B8:AA47" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA47">
-      <sortCondition descending="1" ref="D8:D47"/>
+  <autoFilter ref="B8:AA55" xr:uid="{7DFF8785-B9F4-4C0E-9A61-976B2F786FD7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:AA55">
+      <sortCondition descending="1" ref="D8:D55"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C9:H47">
-    <cfRule type="expression" dxfId="7" priority="8">
+  <conditionalFormatting sqref="C1:C8 C56:C1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:H55">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:H47">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="D9:H55">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>IF(ISNUMBER(SEARCH("J21", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K47">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:L47">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P9:P47">
-    <cfRule type="colorScale" priority="58">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q9:Q47">
-    <cfRule type="colorScale" priority="59">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R9:R47">
+  <conditionalFormatting sqref="K9:K55">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -5280,7 +6053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:U47">
+  <conditionalFormatting sqref="L9:L55">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -5290,19 +6063,70 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U9:V47 O9:R47 J9:M47">
-    <cfRule type="expression" dxfId="0" priority="62">
-      <formula>J9=MIN(J$9:J$47)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V9:V47">
-    <cfRule type="colorScale" priority="71">
+  <conditionalFormatting sqref="P9:P55">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q9:Q55">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R9:R55">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U9:U55">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U9:V55 O9:R55 J9:M55">
+    <cfRule type="expression" dxfId="3" priority="66">
+      <formula>J9=MIN(J$9:J$55)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V9:V55">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C55">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C55">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6694,13 +7518,13 @@
         <v>#N/A</v>
       </c>
       <c r="K43" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="L43" t="s">
         <v>179</v>
       </c>
       <c r="M43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N43" t="s">
         <v>156</v>
@@ -6709,7 +7533,7 @@
         <v>93</v>
       </c>
       <c r="P43" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
@@ -6729,13 +7553,13 @@
         <v>#N/A</v>
       </c>
       <c r="K44" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="L44" t="s">
         <v>179</v>
       </c>
       <c r="M44" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N44" t="s">
         <v>156</v>
@@ -6744,7 +7568,7 @@
         <v>93</v>
       </c>
       <c r="P44" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
@@ -6764,13 +7588,13 @@
         <v>#N/A</v>
       </c>
       <c r="K45" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="L45" t="s">
         <v>179</v>
       </c>
       <c r="M45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N45" t="s">
         <v>156</v>
@@ -6779,7 +7603,7 @@
         <v>93</v>
       </c>
       <c r="P45" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
@@ -6798,6 +7622,24 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K46" t="s">
+        <v>235</v>
+      </c>
+      <c r="L46" t="s">
+        <v>179</v>
+      </c>
+      <c r="M46" t="s">
+        <v>218</v>
+      </c>
+      <c r="N46" t="s">
+        <v>156</v>
+      </c>
+      <c r="O46" t="s">
+        <v>93</v>
+      </c>
+      <c r="P46" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
@@ -6815,6 +7657,24 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
+      <c r="K47" t="s">
+        <v>222</v>
+      </c>
+      <c r="L47" t="s">
+        <v>225</v>
+      </c>
+      <c r="M47" t="s">
+        <v>227</v>
+      </c>
+      <c r="N47" t="s">
+        <v>156</v>
+      </c>
+      <c r="O47" t="s">
+        <v>93</v>
+      </c>
+      <c r="P47" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
@@ -6832,8 +7692,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K48" t="s">
+        <v>223</v>
+      </c>
+      <c r="L48" t="s">
+        <v>225</v>
+      </c>
+      <c r="M48" t="s">
+        <v>180</v>
+      </c>
+      <c r="N48" t="s">
+        <v>156</v>
+      </c>
+      <c r="O48" t="s">
+        <v>93</v>
+      </c>
+      <c r="P48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="E49" t="s">
@@ -6849,8 +7727,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K49" t="s">
+        <v>224</v>
+      </c>
+      <c r="L49" t="s">
+        <v>225</v>
+      </c>
+      <c r="M49" t="s">
+        <v>180</v>
+      </c>
+      <c r="N49" t="s">
+        <v>156</v>
+      </c>
+      <c r="O49" t="s">
+        <v>93</v>
+      </c>
+      <c r="P49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="E50" t="s">
@@ -6866,8 +7762,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K50" t="s">
+        <v>228</v>
+      </c>
+      <c r="L50" t="s">
+        <v>225</v>
+      </c>
+      <c r="M50" t="s">
+        <v>180</v>
+      </c>
+      <c r="N50" t="s">
+        <v>156</v>
+      </c>
+      <c r="O50" t="s">
+        <v>93</v>
+      </c>
+      <c r="P50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="E51" t="s">
@@ -6883,8 +7797,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K51" t="s">
+        <v>220</v>
+      </c>
+      <c r="L51" t="s">
+        <v>226</v>
+      </c>
+      <c r="M51" t="s">
+        <v>218</v>
+      </c>
+      <c r="N51" t="s">
+        <v>156</v>
+      </c>
+      <c r="O51" t="s">
+        <v>93</v>
+      </c>
+      <c r="P51" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="E52" t="s">
@@ -6900,8 +7832,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K52" t="s">
+        <v>219</v>
+      </c>
+      <c r="L52" t="s">
+        <v>226</v>
+      </c>
+      <c r="M52" t="s">
+        <v>218</v>
+      </c>
+      <c r="N52" t="s">
+        <v>156</v>
+      </c>
+      <c r="O52" t="s">
+        <v>93</v>
+      </c>
+      <c r="P52" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="E53" t="s">
@@ -6917,8 +7867,26 @@
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K53" t="s">
+        <v>221</v>
+      </c>
+      <c r="L53" t="s">
+        <v>226</v>
+      </c>
+      <c r="M53" t="s">
+        <v>218</v>
+      </c>
+      <c r="N53" t="s">
+        <v>156</v>
+      </c>
+      <c r="O53" t="s">
+        <v>93</v>
+      </c>
+      <c r="P53" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="E54" t="s">
@@ -6935,7 +7903,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" t="s">
@@ -6952,7 +7920,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="E56" t="s">
@@ -6969,7 +7937,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="E57" t="s">
@@ -6986,7 +7954,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="E58" t="s">
@@ -7003,7 +7971,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="E59" t="s">
@@ -7020,7 +7988,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="E60" t="s">
@@ -7037,7 +8005,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="E61" t="s">
@@ -7054,7 +8022,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="E62" t="s">
@@ -7071,7 +8039,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="E63" t="s">
@@ -7088,7 +8056,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="E64" t="s">

</xml_diff>

<commit_message>
feat: change on template
</commit_message>
<xml_diff>
--- a/report-template.xlsx
+++ b/report-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MITCH\PROYECTOS\Latency-Log-Filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B18C0E-7A9F-4CA6-8BB9-95AF5F424DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE89A0AE-E5CF-4D91-9FD8-AF9485292E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,29 +1033,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -1109,6 +1087,16 @@
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1453,7 +1441,7 @@
   <dimension ref="B2:AA56"/>
   <sheetViews>
     <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:W55"/>
+      <selection activeCell="C9" sqref="C9:W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6016,30 +6004,33 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C1:C8 C56:C1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:H55">
-    <cfRule type="expression" dxfId="10" priority="12">
+  <conditionalFormatting sqref="C9:C55">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:H55">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:H55">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>IF(ISNUMBER(SEARCH("Manolito", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>IF(ISNUMBER(SEARCH("J21", $E9))=TRUE,FALSE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>ISNUMBER(SEARCH("ALGO", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>ISNUMBER(SEARCH("EOMM", $D9))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>ISNUMBER(SEARCH("DMA", $D9))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6104,7 +6095,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U9:V55 O9:R55 J9:M55">
-    <cfRule type="expression" dxfId="3" priority="66">
+    <cfRule type="expression" dxfId="0" priority="66">
       <formula>J9=MIN(J$9:J$55)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6116,17 +6107,6 @@
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:C55">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:C55">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISNUMBER(SEARCH("Manolito", $E9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>ISNUMBER(SEARCH("J21", $E9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>